<commit_message>
Removed old conference talks
</commit_message>
<xml_diff>
--- a/static/docs/src/CV.xlsx
+++ b/static/docs/src/CV.xlsx
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="150">
   <si>
     <t xml:space="preserve">SECTION</t>
   </si>
@@ -492,6 +492,9 @@
   </si>
   <si>
     <t xml:space="preserve">2017-Jan Devconf.cz  Unikernels The next big little thing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#LISTITEM</t>
   </si>
   <si>
     <t xml:space="preserve">2016-Oct ContainerCon Europe, Container Orchestration (pres+lab)</t>
@@ -1044,8 +1047,8 @@
   </sheetPr>
   <dimension ref="A1:BF65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D80" activeCellId="0" sqref="D80"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C114" activeCellId="0" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -5773,10 +5776,10 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="13" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
       <c r="D112" s="36" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E112" s="12"/>
       <c r="G112" s="12"/>
@@ -5834,10 +5837,10 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="13" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
       <c r="D113" s="36" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E113" s="12"/>
       <c r="G113" s="12"/>
@@ -5895,10 +5898,10 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="13" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
       <c r="D114" s="36" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E114" s="12"/>
       <c r="G114" s="12"/>
@@ -6021,7 +6024,7 @@
         <v>34</v>
       </c>
       <c r="D116" s="20" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E116" s="12"/>
       <c r="G116" s="12"/>
@@ -6082,7 +6085,7 @@
         <v>63</v>
       </c>
       <c r="D117" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E117" s="12"/>
       <c r="G117" s="12"/>
@@ -6143,7 +6146,7 @@
         <v>63</v>
       </c>
       <c r="D118" s="21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E118" s="12"/>
       <c r="G118" s="12"/>
@@ -6266,7 +6269,7 @@
         <v>34</v>
       </c>
       <c r="D120" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E120" s="12"/>
       <c r="G120" s="12"/>
@@ -6327,7 +6330,7 @@
         <v>63</v>
       </c>
       <c r="D121" s="21" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E121" s="12"/>
       <c r="G121" s="12"/>
@@ -6388,7 +6391,7 @@
         <v>63</v>
       </c>
       <c r="D122" s="21" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E122" s="12"/>
       <c r="G122" s="12"/>

</xml_diff>

<commit_message>
Updated to show "HPE Customer Innovation Center".
</commit_message>
<xml_diff>
--- a/static/docs/src/CV.xlsx
+++ b/static/docs/src/CV.xlsx
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="162">
   <si>
     <t xml:space="preserve">SECTION</t>
   </si>
@@ -250,337 +250,340 @@
     <t xml:space="preserve">Fr:Solution Architecte</t>
   </si>
   <si>
+    <t xml:space="preserve">HPE Customer Innovation Center - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: HPE EG avant-vente - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Native Solution Architect, HPE  EG presales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:NFV  in HPE Customer Innovation Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: 09/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">END</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LISTITEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Native (CaaS, PaaS, DevOps, micro-services)  presentations and labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Container Orchestration Labs (Docker Swarm, Kubernetes, Apache Mesos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: Creation de PoC NFV avec partenaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hands-on OpenStack for NFV partners PoCs, GCE, AWS, Azure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: OpenStack pour NFV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orchestration/Automation (Heat, Ansible, Vagrant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP CMS - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU patent for Prepaid data charging [EP1720335A1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated installations of  AP4SaaS/IaaS cloud products for Telecom service providers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- Successful transfer to India/China development teams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated test frameworks for IaaS cloud product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agile development of Data analytics and service profile platforms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Agile team (SCRUM/Continuous Integration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Software development, unit and functional tests for SOAP and REST frameworks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposed/implemented automated VideoXML dialog creation from PPT for MWC PoC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOOCs in the areas of BigData, Software Defined Networks, Databases, Agile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution Architect/Consultant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP OCBU - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-sales technical consulting on OpenCall products and proof of concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Prepaid voice/data charging, Voice over IP, IN, NextGen service delivery, OSA/Parlay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer/Partner contact and ITSM delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Performance benchtesting, design win prototyping, PoCs, RFP responses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Deployments KT VoIP benchtest, Tuka IN, DCC Prepaid, FT VHE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  ITSE Workshop delivery (Bouygues prepaid, Polkomtel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Technical Lead for HKTel Y2K migration,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tech Lead/Software Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical Lead on Telecom IN products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Service Creation Environment project (IN SCE), 3rd-party editor integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Consulting, debug, training to 8-partner billing project for HDLC/X.25 networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Design and implementation of SCE and SLEE modules (HA, Mib, MemoryHandler).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Port of HP-UX 802.3 LAN driver to HP-RT.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Member of Technical Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Research Labs - Bristol UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research into design and modeling of data/signalling networks (X.25, SS7, ethernet)  leading to PoC demos and HP products </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel Processing research, AI/Qualitative reasoning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Trainee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBC Research Labs - UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/1983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/1984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z-filter design, simulation, bit-slice micro-processor coding and user subjectivity tests of NICAM digital audio subjective noise reduction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKILLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PaaS Google App Engine, OpenShift, Heroku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IaaS Azure, AWS, OpenStack, CloudStack, SDN (OpenDaylight), Docker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Languages and Paradigms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripting languages (Python/Perl/Ruby/PHP), C++/C, Java, Scala, JavaScript, JQuery, FP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embedded Linux Kernel, Android, Raspberry Pi, BeagleBone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eclipse, Git, svn, vim, maven, Jenkins, gdb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtualization (vSphere/PySphere, KVM-Qemu, VirtualBox)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foreign Languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluency in French, basic fluency in Italian, Spanish.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Sc/Dip.Eng in  Electronic Control and Robotics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHOOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Univ. Of Hull,  UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/1980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walter Firth prize for electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 year placement with BBC Research Labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVITIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conference Talks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mjbright.github.io/Talks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-May PyConUS Container Orchestration, Jupyter tutorials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Apr DockerCon US Unikernels Lightning Talk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Mar HPE TES Unikernels, Container Orchestration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Feb Snowcamp.io Unikernels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Feb HPE TSS NFV, Docker Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Jan Devconf.cz  Unikernels The next big little thing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#LISTITEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-Oct ContainerCon Europe, Container Orchestration (pres+lab)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-Jul Europython, Jupyter for Everything Else (pres+lab)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-Oct Pyconfr, Ipython vers Jupyter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sport / Dance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Running, cycling, Roller blading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock, Argentinian Tango, Salsa, Music, Cinema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenoble Python User Group organiser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenoble Docker and FLOSS User Groups co-organiser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution Architect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPE EG presales – Grenoble, France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CloudNative in HPE Customer Innovation Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Native (Container Orchestration, Docker, Unikernels)  presentations and labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hands-on OpenStack for NFV partners PoCs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hands-on GCE, AWS, Azure, DigitalOcean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: Evangelisme Conteneurs (Docker)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenStack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:OpenStack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:OpenStack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution Architect, Container advocate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-sales technical expert in areas of NFV, Cloud, Virtualization, Containers, SDN, Networking</t>
+  </si>
+  <si>
     <t xml:space="preserve">HPE EG presales - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: HPE EG avant-vente - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Native Solution Architect, HPE Customer Innovation Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:NFV  in HPE Customer Innovation Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">START</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: 09/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">END</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Present</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: Present</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LISTITEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Native (PaaS, CaaS, DevOps, micro-services)  presentations and labs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Container Orchestration Labs (Docker Swarm, Kubernetes, Apache Mesos)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: Creation de PoC NFV avec partenaires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hands-on OpenStack for NFV partners PoCs, GCE, AWS, Azure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: OpenStack pour NFV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orchestration/Automation (Heat, Ansible, Vagrant)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP CMS - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU patent for Prepaid data charging [EP1720335A1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automated installations of  AP4SaaS/IaaS cloud products for Telecom service providers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-- Successful transfer to India/China development teams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automated test frameworks for IaaS cloud product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agile development of Data analytics and service profile platforms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Agile team (SCRUM/Continuous Integration)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Software development, unit and functional tests for SOAP and REST frameworks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposed/implemented automated VideoXML dialog creation from PPT for MWC PoC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOOCs in the areas of BigData, Software Defined Networks, Databases, Agile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solution Architect/Consultant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP OCBU - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-sales technical consulting on OpenCall products and proof of concepts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Prepaid voice/data charging, Voice over IP, IN, NextGen service delivery, OSA/Parlay.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer/Partner contact and ITSM delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Performance benchtesting, design win prototyping, PoCs, RFP responses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Deployments KT VoIP benchtest, Tuka IN, DCC Prepaid, FT VHE.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  ITSE Workshop delivery (Bouygues prepaid, Polkomtel)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Technical Lead for HKTel Y2K migration,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tech Lead/Software Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technical Lead on Telecom IN products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Service Creation Environment project (IN SCE), 3rd-party editor integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Consulting, debug, training to 8-partner billing project for HDLC/X.25 networks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Design and implementation of SCE and SLEE modules (HA, Mib, MemoryHandler).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Port of HP-UX 802.3 LAN driver to HP-RT.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Member of Technical Staff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP Research Labs - Bristol UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08/1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research into design and modeling of data/signalling networks (X.25, SS7, ethernet)  leading to PoC demos and HP products </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallel Processing research, AI/Qualitative reasoning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research Trainee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BBC Research Labs - UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/1983</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08/1984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z-filter design, simulation, bit-slice micro-processor coding and user subjectivity tests of NICAM digital audio subjective noise reduction.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKILLS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PaaS Google App Engine, OpenShift, Heroku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IaaS Azure, AWS, OpenStack, CloudStack, SDN (OpenDaylight), Docker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Languages and Paradigms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scripting languages (Python/Perl/Ruby/PHP), C++/C, Java, Scala, JavaScript, JQuery, FP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Embedded Linux Kernel, Android, Raspberry Pi, BeagleBone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eclipse, Git, svn, vim, maven, Jenkins, gdb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virtualization (vSphere/PySphere, KVM-Qemu, VirtualBox)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foreign Languages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluency in French, basic fluency in Italian, Spanish.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDUCATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.Sc/Dip.Eng in  Electronic Control and Robotics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHOOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Univ. Of Hull,  UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/1980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walter Firth prize for electronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 year placement with BBC Research Labs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVITIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conference Talks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://mjbright.github.io/Talks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-May PyConUS Container Orchestration, Jupyter tutorials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Apr DockerCon US Unikernels Lightning Talk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Mar HPE TES Unikernels, Container Orchestration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Feb Snowcamp.io Unikernels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Feb HPE TSS NFV, Docker Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Jan Devconf.cz  Unikernels The next big little thing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#LISTITEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-Oct ContainerCon Europe, Container Orchestration (pres+lab)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-Jul Europython, Jupyter for Everything Else (pres+lab)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-Oct Pyconfr, Ipython vers Jupyter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sport / Dance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Running, cycling, Roller blading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rock, Argentinian Tango, Salsa, Music, Cinema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenoble Python User Group organiser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenoble Docker and FLOSS User Groups co-organiser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solution Architect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPE EG presales – Grenoble, France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CloudNative in HPE Customer Innovation Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Native (Container Orchestration, Docker, Unikernels)  presentations and labs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hands-on OpenStack for NFV partners PoCs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hands-on GCE, AWS, Azure, DigitalOcean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: Evangelisme Conteneurs (Docker)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpenStack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:OpenStack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:OpenStack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solution Architect, Container advocate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-sales technical expert in areas of NFV, Cloud, Virtualization, Containers, SDN, Networking</t>
   </si>
   <si>
     <t xml:space="preserve">NFV  in HPE Customer Innovation Center</t>
@@ -1108,7 +1111,7 @@
   <dimension ref="A1:BF65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -6546,7 +6549,7 @@
         <v>38</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="21" t="s">
@@ -6559,7 +6562,7 @@
         <v>49</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="15" t="s">
@@ -6598,7 +6601,7 @@
         <v>58</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="0" t="s">
@@ -6611,7 +6614,7 @@
         <v>58</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="0" t="s">

</xml_diff>

<commit_message>
Updated with RMLL, Startup Weekend/Archionline
</commit_message>
<xml_diff>
--- a/static/docs/src/CV.xlsx
+++ b/static/docs/src/CV.xlsx
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="174">
   <si>
     <t xml:space="preserve">SECTION</t>
   </si>
@@ -181,400 +181,461 @@
     <t xml:space="preserve">WEBSITE</t>
   </si>
   <si>
+    <t xml:space="preserve">https://mjbright.github.io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:http://mjbright.github.io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:http://mjbright.github.io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINKEDIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/mjbright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking to work from Grenoble as Pre-sales Solution Architect around Cloud Native, Container and Automation technologies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Bright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:Michael Bright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:Michael Bright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Native Solution Architect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:Solution Architecte, adovcate conteneurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:NFV Solution Architect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenoble, France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:Grenoble, France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:Grenoble, France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMPLOYER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPE, Hewlett-Packard Entreprise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:HPE, Hewlett-Packard Entreprise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:HPE, Hewlett-Packard Entreprise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECTIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-sales technical expert in areas of Cloud Native, Containers, Cloud, Virtualization, NFV, SDN, Networking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXPERIENCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBSECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:Solution Architecte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPE Customer Innovation Center - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: HPE EG avant-vente - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Native Solution Architect, HPE EG presales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:NFV  in HPE Customer Innovation Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: 09/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">END</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LISTITEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Native (CaaS, PaaS, DevOps, micro-services)  presentations and labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Container Orchestration Labs (Docker Swarm, Kubernetes, Apache Mesos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: Creation de PoC NFV avec partenaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hands-on OpenStack for NFV partners PoCs, GCE, AWS, Azure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: OpenStack pour NFV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orchestration/Automation (Heat, Ansible, Vagrant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP CMS - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU patent for Prepaid data charging [EP1720335A1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated installations of  AP4SaaS/IaaS cloud products for Telecom service providers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- Successful transfer to India/China development teams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated test frameworks for IaaS cloud product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agile development of Data analytics and service profile platforms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Agile team (SCRUM/Continuous Integration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Software development, unit and functional tests for SOAP and REST frameworks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposed/implemented automated VideoXML dialog creation from PPT for MWC PoC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOOCs in the areas of BigData, Software Defined Networks, Databases, Agile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution Architect/Consultant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP OCBU - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-sales technical consulting on OpenCall products and proof of concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Prepaid voice/data charging, Voice over IP, IN, NextGen service delivery, OSA/Parlay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer/Partner contact and ITSM delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Performance benchtesting, design win prototyping, PoCs, RFP responses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Deployments KT VoIP benchtest, Tuka IN, DCC Prepaid, FT VHE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  ITSE Workshop delivery (Bouygues prepaid, Polkomtel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Technical Lead for HKTel Y2K migration,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tech Lead/Software Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical Lead on Telecom IN products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Service Creation Environment project (IN SCE), 3rd-party editor integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Consulting, debug, training to 8-partner billing project for HDLC/X.25 networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Design and implementation of SCE and SLEE modules (HA, Mib, MemoryHandler).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Port of HP-UX 802.3 LAN driver to HP-RT.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Member of Technical Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Research Labs - Bristol UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research into design and modeling of data/signalling networks (X.25, SS7, ethernet)  leading to PoC demos and HP products </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel Processing research, AI/Qualitative reasoning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Trainee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBC Research Labs - UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/1983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/1984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z-filter design, simulation, bit-slice micro-processor coding and user subjectivity tests of NICAM digital audio subjective noise reduction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKILLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PaaS OpenShift, Google App Engine, Heroku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IaaS Azure, AWS, OpenStack, CloudStack, SDN (OpenDaylight), Docker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Languages and Paradigms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripting languages (Python/Perl/Ruby/PHP), C++/C, Java, Scala, JavaScript, JQuery, FP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embedded Linux Kernel, Android, Raspberry Pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eclipse, Git, svn, vim, maven, Jenkins, gdb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtualization (vSphere/Pyvmomi, KVM-Qemu, VirtualBox)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foreign Languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluency in French, notions of Italian, Spanish.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Sc/Dip.Eng in  Electronic Control and Robotics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHOOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Univ. Of Hull,  UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/1980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walter Firth prize for electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 year placement with BBC Research Labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVITIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conference Talks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mjbright.github.io/Talks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Jul RMLL Docker-py, Unikernels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-May PyConUS Container Orchestration, Jupyter tutorials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Apr DockerCon US Unikernels Lightning Talk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Mar HPE TES Unikernels, Container Orchestration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Feb Snowcamp.io Unikernels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Feb HPE TSS NFV, Docker Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Jan Devconf.cz  Unikernels The next big little thing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-Oct ContainerCon Europe, Container Orchestration (pres+lab)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-Jul Europython, Jupyter for Everything Else (pres+lab)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-Oct Pyconfr, Ipython vers Jupyter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Startup Weekend</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2012-Nov 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> place: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.archionline.com/</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Sport / Dance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Running, cycling, Roller blading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock, Argentinian Tango, Salsa, Music, Cinema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenoble Python User Group organiser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenoble Docker and FLOSS User Groups co-organiser</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://mjbright.github.io</t>
   </si>
   <si>
-    <t xml:space="preserve">Fr:http://mjbright.github.io</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:http://mjbright.github.io</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINKEDIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/mjbright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Looking to work from Grenoble as Solution Architect around Cloud Native, Container technologies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael Bright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:Michael Bright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:Michael Bright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TITLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Native Solution Architect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:Solution Architecte, adovcate conteneurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:NFV Solution Architect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOCATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenoble, France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:Grenoble, France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:Grenoble, France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMPLOYER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPE, Hewlett-Packard Entreprise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:HPE, Hewlett-Packard Entreprise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:HPE, Hewlett-Packard Entreprise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OBJECTIVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-sales technical expert in areas of Cloud Native, Containers, Cloud, Virtualization, NFV, SDN, Networking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXPERIENCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUBSECTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:Solution Architecte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPE Customer Innovation Center - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: HPE EG avant-vente - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Native Solution Architect, HPE EG presales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:NFV  in HPE Customer Innovation Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">START</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: 09/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">END</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Present</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: Present</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LISTITEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Native (CaaS, PaaS, DevOps, micro-services)  presentations and labs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Container Orchestration Labs (Docker Swarm, Kubernetes, Apache Mesos)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: Creation de PoC NFV avec partenaires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hands-on OpenStack for NFV partners PoCs, GCE, AWS, Azure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: OpenStack pour NFV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orchestration/Automation (Heat, Ansible, Vagrant)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP CMS - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU patent for Prepaid data charging [EP1720335A1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automated installations of  AP4SaaS/IaaS cloud products for Telecom service providers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-- Successful transfer to India/China development teams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automated test frameworks for IaaS cloud product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agile development of Data analytics and service profile platforms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Agile team (SCRUM/Continuous Integration)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Software development, unit and functional tests for SOAP and REST frameworks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposed/implemented automated VideoXML dialog creation from PPT for MWC PoC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOOCs in the areas of BigData, Software Defined Networks, Databases, Agile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solution Architect/Consultant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP OCBU - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-sales technical consulting on OpenCall products and proof of concepts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Prepaid voice/data charging, Voice over IP, IN, NextGen service delivery, OSA/Parlay.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer/Partner contact and ITSM delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Performance benchtesting, design win prototyping, PoCs, RFP responses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Deployments KT VoIP benchtest, Tuka IN, DCC Prepaid, FT VHE.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  ITSE Workshop delivery (Bouygues prepaid, Polkomtel)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Technical Lead for HKTel Y2K migration,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tech Lead/Software Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technical Lead on Telecom IN products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Service Creation Environment project (IN SCE), 3rd-party editor integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Consulting, debug, training to 8-partner billing project for HDLC/X.25 networks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Design and implementation of SCE and SLEE modules (HA, Mib, MemoryHandler).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Port of HP-UX 802.3 LAN driver to HP-RT.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Member of Technical Staff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP Research Labs - Bristol UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08/1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research into design and modeling of data/signalling networks (X.25, SS7, ethernet)  leading to PoC demos and HP products </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallel Processing research, AI/Qualitative reasoning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research Trainee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BBC Research Labs - UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/1983</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08/1984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z-filter design, simulation, bit-slice micro-processor coding and user subjectivity tests of NICAM digital audio subjective noise reduction.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKILLS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud</t>
+    <t xml:space="preserve">Solution Architect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPE EG presales – Grenoble, France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CloudNative in HPE Customer Innovation Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Native (Container Orchestration, Docker, Unikernels)  presentations and labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hands-on OpenStack for NFV partners PoCs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hands-on GCE, AWS, Azure, DigitalOcean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: Evangelisme Conteneurs (Docker)</t>
   </si>
   <si>
     <t xml:space="preserve">PaaS Google App Engine, OpenShift, Heroku</t>
   </si>
   <si>
-    <t xml:space="preserve">IaaS Azure, AWS, OpenStack, CloudStack, SDN (OpenDaylight), Docker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Languages and Paradigms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scripting languages (Python/Perl/Ruby/PHP), C++/C, Java, Scala, JavaScript, JQuery, FP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</t>
-  </si>
-  <si>
     <t xml:space="preserve">Embedded Linux Kernel, Android, Raspberry Pi, BeagleBone</t>
   </si>
   <si>
-    <t xml:space="preserve">Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eclipse, Git, svn, vim, maven, Jenkins, gdb</t>
-  </si>
-  <si>
     <t xml:space="preserve">Virtualization (vSphere/PySphere, KVM-Qemu, VirtualBox)</t>
   </si>
   <si>
-    <t xml:space="preserve">Foreign Languages</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fluency in French, basic fluency in Italian, Spanish.</t>
   </si>
   <si>
-    <t xml:space="preserve">EDUCATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.Sc/Dip.Eng in  Electronic Control and Robotics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHOOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Univ. Of Hull,  UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/1980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walter Firth prize for electronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 year placement with BBC Research Labs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVITIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conference Talks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://mjbright.github.io/Talks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-May PyConUS Container Orchestration, Jupyter tutorials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Apr DockerCon US Unikernels Lightning Talk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Mar HPE TES Unikernels, Container Orchestration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Feb Snowcamp.io Unikernels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Feb HPE TSS NFV, Docker Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Jan Devconf.cz  Unikernels The next big little thing</t>
-  </si>
-  <si>
     <t xml:space="preserve">#LISTITEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-Oct ContainerCon Europe, Container Orchestration (pres+lab)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-Jul Europython, Jupyter for Everything Else (pres+lab)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-Oct Pyconfr, Ipython vers Jupyter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sport / Dance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Running, cycling, Roller blading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rock, Argentinian Tango, Salsa, Music, Cinema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenoble Python User Group organiser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenoble Docker and FLOSS User Groups co-organiser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solution Architect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPE EG presales – Grenoble, France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CloudNative in HPE Customer Innovation Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Native (Container Orchestration, Docker, Unikernels)  presentations and labs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hands-on OpenStack for NFV partners PoCs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hands-on GCE, AWS, Azure, DigitalOcean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: Evangelisme Conteneurs (Docker)</t>
   </si>
   <si>
     <t xml:space="preserve">ATC</t>
@@ -616,7 +677,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="MMM\-YY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -676,6 +737,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -808,7 +883,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -945,6 +1020,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1025,6 +1104,21 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="WeeklyCalendar"/>
+      <sheetName val="Formulas"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="Sport-06"/>
       <sheetName val="Sport"/>
       <sheetName val="KDO"/>
@@ -1100,21 +1194,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="WeeklyCalendar"/>
-      <sheetName val="Formulas"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1123,21 +1202,21 @@
   <dimension ref="A1:BF65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.7295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.1938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2812,7 +2891,7 @@
       <c r="E106" s="12"/>
       <c r="G106" s="12"/>
     </row>
-    <row r="107" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="15" t="s">
         <v>62</v>
       </c>
@@ -2826,7 +2905,7 @@
       <c r="C108" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D108" s="13" t="s">
+      <c r="D108" s="34" t="s">
         <v>133</v>
       </c>
       <c r="E108" s="12"/>
@@ -2883,72 +2962,72 @@
       <c r="G113" s="12"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C114" s="13" t="s">
+      <c r="C114" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D114" s="13" t="s">
         <v>139</v>
-      </c>
-      <c r="D114" s="34" t="s">
-        <v>140</v>
       </c>
       <c r="E114" s="12"/>
       <c r="G114" s="12"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D115" s="34" t="s">
-        <v>141</v>
+        <v>62</v>
+      </c>
+      <c r="D115" s="35" t="s">
+        <v>140</v>
       </c>
       <c r="E115" s="12"/>
       <c r="G115" s="12"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D116" s="34" t="s">
-        <v>142</v>
+        <v>62</v>
+      </c>
+      <c r="D116" s="35" t="s">
+        <v>141</v>
       </c>
       <c r="E116" s="12"/>
       <c r="G116" s="12"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="23" t="s">
+      <c r="C117" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D117" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="E117" s="12"/>
+      <c r="G117" s="12"/>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B117" s="24"/>
-      <c r="C117" s="25"/>
-      <c r="D117" s="24"/>
-      <c r="E117" s="12"/>
-      <c r="F117" s="24"/>
-      <c r="G117" s="12"/>
-    </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="13" t="s">
+      <c r="B118" s="24"/>
+      <c r="C118" s="25"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="12"/>
+      <c r="F118" s="24"/>
+      <c r="G118" s="12"/>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C119" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D118" s="20" t="s">
+      <c r="D119" s="20" t="s">
         <v>143</v>
-      </c>
-      <c r="E118" s="12"/>
-      <c r="G118" s="12"/>
-    </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D119" s="21" t="s">
-        <v>144</v>
       </c>
       <c r="E119" s="12"/>
       <c r="G119" s="12"/>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C120" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D120" s="21" t="s">
-        <v>145</v>
+    <row r="120" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C120" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D120" s="35" t="s">
+        <v>144</v>
       </c>
       <c r="E120" s="12"/>
       <c r="G120" s="12"/>
@@ -2969,7 +3048,7 @@
         <v>34</v>
       </c>
       <c r="D122" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E122" s="12"/>
       <c r="G122" s="12"/>
@@ -2979,7 +3058,7 @@
         <v>62</v>
       </c>
       <c r="D123" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E123" s="12"/>
       <c r="G123" s="12"/>
@@ -2989,7 +3068,7 @@
         <v>62</v>
       </c>
       <c r="D124" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E124" s="12"/>
       <c r="G124" s="12"/>
@@ -3002,12 +3081,49 @@
       <c r="C125" s="25"/>
       <c r="D125" s="24"/>
       <c r="E125" s="12"/>
+      <c r="F125" s="24"/>
       <c r="G125" s="12"/>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C126" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D126" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="E126" s="12"/>
+      <c r="G126" s="12"/>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C127" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D127" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E127" s="12"/>
+      <c r="G127" s="12"/>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C128" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D128" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E128" s="12"/>
+      <c r="G128" s="12"/>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B129" s="24"/>
+      <c r="C129" s="25"/>
+      <c r="D129" s="24"/>
+      <c r="E129" s="12"/>
+      <c r="G129" s="12"/>
+    </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3049,10 +3165,10 @@
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3067,6 +3183,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D107" r:id="rId1" display="https://mjbright.github.io/Talks"/>
+    <hyperlink ref="D120" r:id="rId2" display="https://www.archionline.com/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3091,16 +3208,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.7295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.1938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3224,7 +3341,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>24</v>
+        <v>151</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="13" t="s">
@@ -3332,7 +3449,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="11" t="s">
@@ -3345,7 +3462,7 @@
         <v>42</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="21" t="s">
@@ -3358,7 +3475,7 @@
         <v>53</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="15" t="s">
@@ -3397,7 +3514,7 @@
         <v>62</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="0" t="s">
@@ -3410,7 +3527,7 @@
         <v>62</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="0" t="s">
@@ -3423,11 +3540,11 @@
         <v>62</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="13"/>
@@ -4155,7 +4272,7 @@
         <v>62</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="E77" s="12"/>
       <c r="G77" s="12"/>
@@ -4317,7 +4434,7 @@
         <v>62</v>
       </c>
       <c r="D83" s="21" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="E83" s="12"/>
       <c r="G83" s="12"/>
@@ -4359,7 +4476,7 @@
         <v>62</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="E87" s="12"/>
       <c r="F87" s="0"/>
@@ -4546,7 +4663,7 @@
         <v>62</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
       <c r="E90" s="12"/>
       <c r="G90" s="12"/>
@@ -4760,7 +4877,7 @@
         <v>62</v>
       </c>
       <c r="D105" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E105" s="12"/>
       <c r="G105" s="12"/>
@@ -4770,7 +4887,7 @@
         <v>62</v>
       </c>
       <c r="D106" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E106" s="12"/>
       <c r="G106" s="12"/>
@@ -4780,7 +4897,7 @@
         <v>62</v>
       </c>
       <c r="D107" s="13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E107" s="12"/>
       <c r="G107" s="12"/>
@@ -4790,7 +4907,7 @@
         <v>62</v>
       </c>
       <c r="D108" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E108" s="12"/>
       <c r="G108" s="12"/>
@@ -4800,7 +4917,7 @@
         <v>62</v>
       </c>
       <c r="D109" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E109" s="12"/>
       <c r="G109" s="12"/>
@@ -4810,16 +4927,16 @@
         <v>62</v>
       </c>
       <c r="D110" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E110" s="12"/>
       <c r="G110" s="12"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D111" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D111" s="35" t="s">
         <v>140</v>
       </c>
       <c r="E111" s="12"/>
@@ -4827,9 +4944,9 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D112" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D112" s="35" t="s">
         <v>141</v>
       </c>
       <c r="E112" s="12"/>
@@ -4837,9 +4954,9 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D113" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D113" s="35" t="s">
         <v>142</v>
       </c>
       <c r="E113" s="12"/>
@@ -4861,7 +4978,7 @@
         <v>34</v>
       </c>
       <c r="D115" s="20" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E115" s="12"/>
       <c r="G115" s="12"/>
@@ -4871,7 +4988,7 @@
         <v>62</v>
       </c>
       <c r="D116" s="21" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E116" s="12"/>
       <c r="G116" s="12"/>
@@ -4881,7 +4998,7 @@
         <v>62</v>
       </c>
       <c r="D117" s="21" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E117" s="12"/>
       <c r="G117" s="12"/>
@@ -4902,7 +5019,7 @@
         <v>34</v>
       </c>
       <c r="D119" s="20" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E119" s="12"/>
       <c r="G119" s="12"/>
@@ -4912,7 +5029,7 @@
         <v>62</v>
       </c>
       <c r="D120" s="21" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E120" s="12"/>
       <c r="G120" s="12"/>
@@ -4922,7 +5039,7 @@
         <v>62</v>
       </c>
       <c r="D121" s="21" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E121" s="12"/>
       <c r="G121" s="12"/>
@@ -5028,16 +5145,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.7295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.1938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5142,18 +5259,18 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="13" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="13" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="13" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5177,7 +5294,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>24</v>
+        <v>151</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="13" t="s">
@@ -5209,7 +5326,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="13" t="s">
@@ -5257,7 +5374,7 @@
         <v>46</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
@@ -5285,7 +5402,7 @@
         <v>34</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="11" t="s">
@@ -5298,7 +5415,7 @@
         <v>42</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="21" t="s">
@@ -5311,7 +5428,7 @@
         <v>53</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="15" t="s">
@@ -5350,7 +5467,7 @@
         <v>62</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="0" t="s">
@@ -5363,7 +5480,7 @@
         <v>62</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="0" t="s">
@@ -5376,11 +5493,11 @@
         <v>62</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G23" s="12"/>
     </row>
@@ -6107,7 +6224,7 @@
         <v>62</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="E78" s="12"/>
       <c r="G78" s="12"/>
@@ -6269,7 +6386,7 @@
         <v>62</v>
       </c>
       <c r="D84" s="21" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="E84" s="12"/>
       <c r="G84" s="12"/>
@@ -6311,7 +6428,7 @@
         <v>62</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="E88" s="12"/>
       <c r="F88" s="0"/>
@@ -6498,7 +6615,7 @@
         <v>62</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
       <c r="E91" s="12"/>
       <c r="G91" s="12"/>
@@ -6712,7 +6829,7 @@
         <v>62</v>
       </c>
       <c r="D106" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E106" s="12"/>
       <c r="G106" s="12"/>
@@ -6722,7 +6839,7 @@
         <v>62</v>
       </c>
       <c r="D107" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E107" s="12"/>
       <c r="G107" s="12"/>
@@ -6732,7 +6849,7 @@
         <v>62</v>
       </c>
       <c r="D108" s="13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E108" s="12"/>
       <c r="G108" s="12"/>
@@ -6742,7 +6859,7 @@
         <v>62</v>
       </c>
       <c r="D109" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E109" s="12"/>
       <c r="G109" s="12"/>
@@ -6752,7 +6869,7 @@
         <v>62</v>
       </c>
       <c r="D110" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E110" s="12"/>
       <c r="G110" s="12"/>
@@ -6762,16 +6879,16 @@
         <v>62</v>
       </c>
       <c r="D111" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E111" s="12"/>
       <c r="G111" s="12"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D112" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D112" s="35" t="s">
         <v>140</v>
       </c>
       <c r="E112" s="12"/>
@@ -6779,9 +6896,9 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D113" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D113" s="35" t="s">
         <v>141</v>
       </c>
       <c r="E113" s="12"/>
@@ -6789,9 +6906,9 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D114" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D114" s="35" t="s">
         <v>142</v>
       </c>
       <c r="E114" s="12"/>
@@ -6813,7 +6930,7 @@
         <v>34</v>
       </c>
       <c r="D116" s="20" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E116" s="12"/>
       <c r="G116" s="12"/>
@@ -6823,7 +6940,7 @@
         <v>62</v>
       </c>
       <c r="D117" s="21" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E117" s="12"/>
       <c r="G117" s="12"/>
@@ -6833,7 +6950,7 @@
         <v>62</v>
       </c>
       <c r="D118" s="21" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E118" s="12"/>
       <c r="G118" s="12"/>
@@ -6854,7 +6971,7 @@
         <v>34</v>
       </c>
       <c r="D120" s="20" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E120" s="12"/>
       <c r="G120" s="12"/>
@@ -6864,7 +6981,7 @@
         <v>62</v>
       </c>
       <c r="D121" s="21" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E121" s="12"/>
       <c r="G121" s="12"/>
@@ -6874,7 +6991,7 @@
         <v>62</v>
       </c>
       <c r="D122" s="21" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E122" s="12"/>
       <c r="G122" s="12"/>

</xml_diff>

<commit_message>
Reduced Goal field to keep down to 2 pages.
</commit_message>
<xml_diff>
--- a/static/docs/src/CV.xlsx
+++ b/static/docs/src/CV.xlsx
@@ -199,7 +199,7 @@
     <t xml:space="preserve">GOAL</t>
   </si>
   <si>
-    <t xml:space="preserve">Looking to work from Grenoble as Pre-sales Solution Architect around Cloud Native, Container and Automation technologies</t>
+    <t xml:space="preserve">Objective - Pre-sales Solution Architect around Cloud Native, Container and Automation technologies</t>
   </si>
   <si>
     <t xml:space="preserve">Michael Bright</t>
@@ -1202,7 +1202,7 @@
   <dimension ref="A1:BF65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>

</xml_diff>

<commit_message>
Added CNCF Kubernetes (CKA) certification.
</commit_message>
<xml_diff>
--- a/static/docs/src/CV.xlsx
+++ b/static/docs/src/CV.xlsx
@@ -9,12 +9,13 @@
   </bookViews>
   <sheets>
     <sheet name="CV" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CV.fails" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="CV_2017-Mars_ATC" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="CV_2017_Jul_RedHat_AnsibleSpecialiste" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="CV.fails" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="CV_2017-Mars_ATC" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName function="false" hidden="false" name="ampm" vbProcedure="false">[2]Formulas!$C$31:$C$72</definedName>
@@ -60,9 +61,9 @@
     <definedName function="false" hidden="false" name="WeekNo" vbProcedure="false">[2]Formulas!$A$21:$A$27</definedName>
     <definedName function="false" hidden="false" name="year" vbProcedure="false">[2]Formulas!$H$6</definedName>
     <definedName function="false" hidden="false" name="_DAY1" vbProcedure="false">[1]W1!$C$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="GAIN" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="GAIN2" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="MONINT" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="GAIN" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="GAIN2" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="MONINT" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -73,7 +74,7 @@
 </workbook>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="175">
   <si>
     <t xml:space="preserve">SECTION</t>
   </si>
@@ -145,458 +146,424 @@
     <t xml:space="preserve">CERTIFICATION</t>
   </si>
   <si>
+    <t xml:space="preserve">CNCF Kubernetes CKA, RHCE, RHCSA, HPE Expert One SDN Apps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:RHCE, RHCSA, HP Expert One SDN Apps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:RHCE, RHCSA, HP Expert One SDN Apps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+33 (0)672991647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:+33 (0)67299 1647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:+33 (0)67299 1647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cv@mjbright.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:cv@mjbright.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:cv@mjbright.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEBSITE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mjbright.github.io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:http://mjbright.github.io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:http://mjbright.github.io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINKEDIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/mjbright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective - Pre-sales Solution Architect around Cloud Native, Container and Automation technologies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Bright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:Michael Bright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:Michael Bright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Native Solution Architect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:Solution Architecte, adovcate conteneurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:NFV Solution Architect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenoble, France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:Grenoble, France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:Grenoble, France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMPLOYER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPE, Hewlett-Packard Entreprise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:HPE, Hewlett-Packard Entreprise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es:HPE, Hewlett-Packard Entreprise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECTIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-sales technical expert in areas of Cloud Native, Containers, Cloud, Virtualization, NFV, SDN, Networking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXPERIENCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBSECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:Solution Architecte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPE Customer Innovation Center - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: HPE EG avant-vente - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Native Solution Architect, HPE EG presales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr:NFV  in HPE Customer Innovation Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: 09/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">END</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LISTITEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Native (CaaS, PaaS, DevOps, micro-services)  presentations and labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Container Orchestration Labs (Docker Swarm, Kubernetes, Apache Mesos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: Creation de PoC NFV avec partenaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hands-on OpenStack for NFV partners PoCs, GCE, AWS, Azure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr: OpenStack pour NFV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orchestration/Automation (Heat, Ansible, Vagrant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP CMS - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU patent for Prepaid data charging [EP1720335A1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated installations of  AP4SaaS/IaaS cloud products for Telecom service providers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- Successful transfer to India/China development teams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated test frameworks for IaaS cloud product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agile development of Data analytics and service profile platforms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Agile team (SCRUM/Continuous Integration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Software development, unit and functional tests for SOAP and REST frameworks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposed/implemented automated VideoXML dialog creation from PPT for MWC PoC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOOCs in the areas of BigData, Software Defined Networks, Databases, Agile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution Architect/Consultant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP OCBU - Grenoble France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-sales technical consulting on OpenCall products and proof of concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Prepaid voice/data charging, Voice over IP, IN, NextGen service delivery, OSA/Parlay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer/Partner contact and ITSM delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Performance benchtesting, design win prototyping, PoCs, RFP responses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Deployments KT VoIP benchtest, Tuka IN, DCC Prepaid, FT VHE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  ITSE Workshop delivery (Bouygues prepaid, Polkomtel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Technical Lead for HKTel Y2K migration,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tech Lead/Software Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical Lead on Telecom IN products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Service Creation Environment project (IN SCE), 3rd-party editor integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Consulting, debug, training to 8-partner billing project for HDLC/X.25 networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Design and implementation of SCE and SLEE modules (HA, Mib, MemoryHandler).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Port of HP-UX 802.3 LAN driver to HP-RT.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Member of Technical Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Research Labs - Bristol UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research into design and modeling of data/signalling networks (X.25, SS7, ethernet)  leading to PoC demos and HP products </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel Processing research, AI/Qualitative reasoning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Trainee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBC Research Labs - UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/1983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/1984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z-filter design, simulation, bit-slice micro-processor coding and user subjectivity tests of NICAM digital audio subjective noise reduction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKILLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PaaS OpenShift, Google App Engine, Heroku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IaaS Azure, AWS, OpenStack, CloudStack, SDN (OpenDaylight), Docker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Languages and Paradigms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripting languages (Python/Perl/Ruby/PHP), C++/C, Java, Scala, JavaScript, JQuery, FP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embedded Linux Kernel, Android, Raspberry Pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eclipse, Git, svn, vim, maven, Jenkins, gdb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtualization (vSphere/Pyvmomi, KVM-Qemu, VirtualBox)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foreign Languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluency in French, notions of Italian, Spanish.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Sc/Dip.Eng in  Electronic Control and Robotics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHOOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Univ. Of Hull,  UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/1980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walter Firth prize for electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 year placement with BBC Research Labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVITIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conference Talks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mjbright.github.io/Talks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Jul RMLL Docker-py, Unikernels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-May PyConUS Container Orchestration, Jupyter tutorials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Apr DockerCon US Unikernels Lightning Talk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Mar HPE TES Unikernels, Container Orchestration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Feb Snowcamp.io Unikernels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Feb HPE TSS NFV, Docker Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Jan Devconf.cz  Unikernels The next big little thing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-Oct ContainerCon Europe, Container Orchestration (pres+lab)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-Jul Europython, Jupyter for Everything Else (pres+lab)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-Oct Pyconfr, Ipython vers Jupyter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Startup Weekend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-Nov 2nd place: https://www.archionline.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sport / Dance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Running, cycling, Roller blading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock, Argentinian Tango, Salsa, Music, Cinema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenoble Python User Group organiser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenoble Docker and FLOSS User Groups co-organiser</t>
+  </si>
+  <si>
     <t xml:space="preserve">RHCE, RHCSA, HPE Expert One SDN Apps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:RHCE, RHCSA, HP Expert One SDN Apps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:RHCE, RHCSA, HP Expert One SDN Apps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+33 (0)672991647</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:+33 (0)67299 1647</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:+33 (0)67299 1647</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cv@mjbright.net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:cv@mjbright.net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:cv@mjbright.net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WEBSITE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://mjbright.github.io</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:http://mjbright.github.io</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:http://mjbright.github.io</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINKEDIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/mjbright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Objective - Pre-sales Solution Architect around Cloud Native, Container and Automation technologies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael Bright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:Michael Bright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:Michael Bright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TITLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Native Solution Architect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:Solution Architecte, adovcate conteneurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:NFV Solution Architect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOCATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenoble, France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:Grenoble, France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:Grenoble, France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMPLOYER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPE, Hewlett-Packard Entreprise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:HPE, Hewlett-Packard Entreprise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es:HPE, Hewlett-Packard Entreprise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OBJECTIVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-sales technical expert in areas of Cloud Native, Containers, Cloud, Virtualization, NFV, SDN, Networking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXPERIENCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUBSECTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:Solution Architecte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPE Customer Innovation Center - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: HPE EG avant-vente - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Native Solution Architect, HPE EG presales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr:NFV  in HPE Customer Innovation Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">START</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: 09/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">END</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Present</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: Present</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LISTITEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Native (CaaS, PaaS, DevOps, micro-services)  presentations and labs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Container Orchestration Labs (Docker Swarm, Kubernetes, Apache Mesos)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: Creation de PoC NFV avec partenaires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hands-on OpenStack for NFV partners PoCs, GCE, AWS, Azure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr: OpenStack pour NFV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orchestration/Automation (Heat, Ansible, Vagrant)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP CMS - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU patent for Prepaid data charging [EP1720335A1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automated installations of  AP4SaaS/IaaS cloud products for Telecom service providers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-- Successful transfer to India/China development teams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automated test frameworks for IaaS cloud product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agile development of Data analytics and service profile platforms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Agile team (SCRUM/Continuous Integration)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Software development, unit and functional tests for SOAP and REST frameworks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposed/implemented automated VideoXML dialog creation from PPT for MWC PoC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOOCs in the areas of BigData, Software Defined Networks, Databases, Agile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solution Architect/Consultant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP OCBU - Grenoble France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-sales technical consulting on OpenCall products and proof of concepts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Prepaid voice/data charging, Voice over IP, IN, NextGen service delivery, OSA/Parlay.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer/Partner contact and ITSM delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Performance benchtesting, design win prototyping, PoCs, RFP responses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Deployments KT VoIP benchtest, Tuka IN, DCC Prepaid, FT VHE.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  ITSE Workshop delivery (Bouygues prepaid, Polkomtel)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Technical Lead for HKTel Y2K migration,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tech Lead/Software Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technical Lead on Telecom IN products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Service Creation Environment project (IN SCE), 3rd-party editor integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Consulting, debug, training to 8-partner billing project for HDLC/X.25 networks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Design and implementation of SCE and SLEE modules (HA, Mib, MemoryHandler).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Port of HP-UX 802.3 LAN driver to HP-RT.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Member of Technical Staff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP Research Labs - Bristol UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08/1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research into design and modeling of data/signalling networks (X.25, SS7, ethernet)  leading to PoC demos and HP products </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallel Processing research, AI/Qualitative reasoning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research Trainee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BBC Research Labs - UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/1983</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08/1984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z-filter design, simulation, bit-slice micro-processor coding and user subjectivity tests of NICAM digital audio subjective noise reduction.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKILLS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PaaS OpenShift, Google App Engine, Heroku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IaaS Azure, AWS, OpenStack, CloudStack, SDN (OpenDaylight), Docker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Languages and Paradigms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scripting languages (Python/Perl/Ruby/PHP), C++/C, Java, Scala, JavaScript, JQuery, FP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Embedded Linux Kernel, Android, Raspberry Pi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eclipse, Git, svn, vim, maven, Jenkins, gdb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virtualization (vSphere/Pyvmomi, KVM-Qemu, VirtualBox)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foreign Languages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluency in French, notions of Italian, Spanish.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDUCATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.Sc/Dip.Eng in  Electronic Control and Robotics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHOOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Univ. Of Hull,  UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/1980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walter Firth prize for electronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 year placement with BBC Research Labs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVITIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conference Talks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://mjbright.github.io/Talks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Jul RMLL Docker-py, Unikernels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-May PyConUS Container Orchestration, Jupyter tutorials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Apr DockerCon US Unikernels Lightning Talk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Mar HPE TES Unikernels, Container Orchestration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Feb Snowcamp.io Unikernels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Feb HPE TSS NFV, Docker Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-Jan Devconf.cz  Unikernels The next big little thing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-Oct ContainerCon Europe, Container Orchestration (pres+lab)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-Jul Europython, Jupyter for Everything Else (pres+lab)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-Oct Pyconfr, Ipython vers Jupyter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Startup Weekend</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2012-Nov 2</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">nd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> place: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.archionline.com/</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Sport / Dance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Running, cycling, Roller blading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rock, Argentinian Tango, Salsa, Music, Cinema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenoble Python User Group organiser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenoble Docker and FLOSS User Groups co-organiser</t>
   </si>
   <si>
     <t xml:space="preserve">http://mjbright.github.io</t>
@@ -677,7 +644,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="MMM\-YY"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -744,13 +711,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -883,7 +843,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1028,6 +988,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1101,21 +1065,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="WeeklyCalendar"/>
-      <sheetName val="Formulas"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1194,6 +1143,21 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="WeeklyCalendar"/>
+      <sheetName val="Formulas"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1202,21 +1166,21 @@
   <dimension ref="A1:BF65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.1938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3026,7 +2990,7 @@
       <c r="C120" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D120" s="35" t="s">
+      <c r="D120" s="36" t="s">
         <v>144</v>
       </c>
       <c r="E120" s="12"/>
@@ -3183,7 +3147,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D107" r:id="rId1" display="https://mjbright.github.io/Talks"/>
-    <hyperlink ref="D120" r:id="rId2" display="https://www.archionline.com/"/>
+    <hyperlink ref="D120" r:id="rId2" display="2012-Nov 2nd place: https://www.archionline.com/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3203,21 +3167,21 @@
   <dimension ref="A1:BF65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.1938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3293,7 +3257,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>12</v>
+        <v>151</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="13" t="s">
@@ -3341,7 +3305,2008 @@
         <v>23</v>
       </c>
       <c r="D7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" s="16" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="E16" s="12"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="14"/>
+      <c r="G27" s="26"/>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="G28" s="26"/>
+      <c r="I28" s="27"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="G29" s="26"/>
+      <c r="I29" s="27"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="G30" s="26"/>
+      <c r="I30" s="27"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="G31" s="26"/>
+      <c r="I31" s="27"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="G32" s="12"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="14"/>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="G35" s="12"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="14"/>
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" s="14"/>
+      <c r="G38" s="12"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="G39" s="26"/>
+      <c r="I39" s="27"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="24"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" s="14"/>
+      <c r="G41" s="12"/>
+    </row>
+    <row r="42" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="B42" s="0"/>
+      <c r="C42" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="14"/>
+      <c r="F42" s="0"/>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" s="14"/>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="14"/>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" s="14"/>
+      <c r="G45" s="12"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="14"/>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47" s="14"/>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" s="14"/>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0"/>
+      <c r="B49" s="0"/>
+      <c r="C49" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E49" s="14"/>
+      <c r="F49" s="0"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="0"/>
+      <c r="I49" s="0"/>
+      <c r="J49" s="0"/>
+      <c r="K49" s="0"/>
+      <c r="L49" s="0"/>
+      <c r="M49" s="0"/>
+      <c r="N49" s="0"/>
+      <c r="O49" s="0"/>
+      <c r="P49" s="0"/>
+      <c r="Q49" s="0"/>
+      <c r="R49" s="0"/>
+      <c r="S49" s="0"/>
+      <c r="T49" s="0"/>
+      <c r="U49" s="0"/>
+      <c r="V49" s="0"/>
+      <c r="W49" s="0"/>
+      <c r="X49" s="0"/>
+      <c r="Y49" s="0"/>
+      <c r="Z49" s="0"/>
+      <c r="AA49" s="0"/>
+      <c r="AB49" s="0"/>
+      <c r="AC49" s="0"/>
+      <c r="AD49" s="0"/>
+      <c r="AE49" s="0"/>
+      <c r="AF49" s="0"/>
+      <c r="AG49" s="0"/>
+      <c r="AH49" s="0"/>
+      <c r="AI49" s="0"/>
+      <c r="AJ49" s="0"/>
+      <c r="AK49" s="0"/>
+      <c r="AL49" s="0"/>
+      <c r="AM49" s="0"/>
+      <c r="AN49" s="0"/>
+      <c r="AO49" s="0"/>
+      <c r="AP49" s="0"/>
+      <c r="AQ49" s="0"/>
+      <c r="AR49" s="0"/>
+      <c r="AS49" s="0"/>
+      <c r="AT49" s="0"/>
+      <c r="AU49" s="0"/>
+      <c r="AV49" s="0"/>
+      <c r="AW49" s="0"/>
+      <c r="AX49" s="0"/>
+      <c r="AY49" s="0"/>
+      <c r="AZ49" s="0"/>
+      <c r="BA49" s="0"/>
+      <c r="BB49" s="0"/>
+      <c r="BC49" s="0"/>
+      <c r="BD49" s="0"/>
+      <c r="BE49" s="0"/>
+      <c r="BF49" s="0"/>
+    </row>
+    <row r="50" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0"/>
+      <c r="B50" s="0"/>
+      <c r="C50" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E50" s="14"/>
+      <c r="F50" s="0"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="7"/>
+      <c r="U50" s="7"/>
+      <c r="V50" s="7"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="7"/>
+      <c r="Y50" s="7"/>
+      <c r="Z50" s="7"/>
+      <c r="AA50" s="7"/>
+      <c r="AB50" s="7"/>
+      <c r="AC50" s="7"/>
+      <c r="AD50" s="7"/>
+      <c r="AE50" s="7"/>
+      <c r="AF50" s="7"/>
+      <c r="AG50" s="7"/>
+      <c r="AH50" s="7"/>
+      <c r="AI50" s="7"/>
+      <c r="AJ50" s="7"/>
+      <c r="AK50" s="7"/>
+      <c r="AL50" s="7"/>
+      <c r="AM50" s="7"/>
+      <c r="AN50" s="7"/>
+      <c r="AO50" s="7"/>
+      <c r="AP50" s="7"/>
+      <c r="AQ50" s="7"/>
+      <c r="AR50" s="7"/>
+      <c r="AS50" s="7"/>
+      <c r="AT50" s="7"/>
+      <c r="AU50" s="7"/>
+      <c r="AV50" s="7"/>
+      <c r="AW50" s="7"/>
+      <c r="AX50" s="7"/>
+      <c r="AY50" s="7"/>
+      <c r="AZ50" s="7"/>
+      <c r="BA50" s="7"/>
+      <c r="BB50" s="7"/>
+      <c r="BC50" s="7"/>
+      <c r="BD50" s="7"/>
+      <c r="BE50" s="7"/>
+      <c r="BF50" s="7"/>
+    </row>
+    <row r="51" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0"/>
+      <c r="B51" s="0"/>
+      <c r="C51" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="14"/>
+      <c r="F51" s="0"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="0"/>
+      <c r="I51" s="0"/>
+      <c r="J51" s="0"/>
+      <c r="K51" s="0"/>
+      <c r="L51" s="0"/>
+      <c r="M51" s="0"/>
+      <c r="N51" s="0"/>
+      <c r="O51" s="0"/>
+      <c r="P51" s="0"/>
+      <c r="Q51" s="0"/>
+      <c r="R51" s="0"/>
+      <c r="S51" s="0"/>
+      <c r="T51" s="0"/>
+      <c r="U51" s="0"/>
+      <c r="V51" s="0"/>
+      <c r="W51" s="0"/>
+      <c r="X51" s="0"/>
+      <c r="Y51" s="0"/>
+      <c r="Z51" s="0"/>
+      <c r="AA51" s="0"/>
+      <c r="AB51" s="0"/>
+      <c r="AC51" s="0"/>
+      <c r="AD51" s="0"/>
+      <c r="AE51" s="0"/>
+      <c r="AF51" s="0"/>
+      <c r="AG51" s="0"/>
+      <c r="AH51" s="0"/>
+      <c r="AI51" s="0"/>
+      <c r="AJ51" s="0"/>
+      <c r="AK51" s="0"/>
+      <c r="AL51" s="0"/>
+      <c r="AM51" s="0"/>
+      <c r="AN51" s="0"/>
+      <c r="AO51" s="0"/>
+      <c r="AP51" s="0"/>
+      <c r="AQ51" s="0"/>
+      <c r="AR51" s="0"/>
+      <c r="AS51" s="0"/>
+      <c r="AT51" s="0"/>
+      <c r="AU51" s="0"/>
+      <c r="AV51" s="0"/>
+      <c r="AW51" s="0"/>
+      <c r="AX51" s="0"/>
+      <c r="AY51" s="0"/>
+      <c r="AZ51" s="0"/>
+      <c r="BA51" s="0"/>
+      <c r="BB51" s="0"/>
+      <c r="BC51" s="0"/>
+      <c r="BD51" s="0"/>
+      <c r="BE51" s="0"/>
+      <c r="BF51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="24"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="14"/>
+      <c r="G52" s="12"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="G53" s="12"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="14"/>
+      <c r="G54" s="12"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E55" s="14"/>
+      <c r="G55" s="12"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" s="14"/>
+      <c r="G56" s="12"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E57" s="14"/>
+      <c r="G57" s="12"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E58" s="14"/>
+      <c r="G58" s="12"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E59" s="14"/>
+      <c r="G59" s="12"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C60" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E60" s="14"/>
+      <c r="G60" s="12"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C61" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E61" s="14"/>
+      <c r="G61" s="12"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E62" s="14"/>
+      <c r="G62" s="12"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63" s="24"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="14"/>
+      <c r="G63" s="12"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E64" s="14"/>
+      <c r="G64" s="12"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C65" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E65" s="14"/>
+      <c r="G65" s="12"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E66" s="14"/>
+      <c r="G66" s="12"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E67" s="14"/>
+      <c r="G67" s="12"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E68" s="14"/>
+      <c r="G68" s="12"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E69" s="14"/>
+      <c r="G69" s="12"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B70" s="24"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="14"/>
+      <c r="G70" s="12"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E71" s="14"/>
+      <c r="G71" s="12"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E72" s="14"/>
+      <c r="G72" s="12"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C73" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D73" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E73" s="14"/>
+      <c r="G73" s="12"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D74" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E74" s="14"/>
+      <c r="G74" s="12"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C75" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E75" s="14"/>
+      <c r="G75" s="12"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B76" s="24"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="14"/>
+      <c r="G76" s="12"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C77" s="30"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="12"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B78" s="24"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="12"/>
+      <c r="G78" s="12"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C79" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E79" s="12"/>
+      <c r="G79" s="12"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C80" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D80" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E80" s="12"/>
+      <c r="G80" s="12"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C81" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E81" s="12"/>
+      <c r="G81" s="12"/>
+    </row>
+    <row r="82" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B82" s="24"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="24"/>
+      <c r="H82" s="7"/>
+      <c r="I82" s="7"/>
+      <c r="J82" s="7"/>
+      <c r="K82" s="7"/>
+      <c r="L82" s="7"/>
+      <c r="M82" s="7"/>
+      <c r="N82" s="7"/>
+      <c r="O82" s="7"/>
+      <c r="P82" s="7"/>
+      <c r="Q82" s="7"/>
+      <c r="R82" s="7"/>
+      <c r="S82" s="7"/>
+      <c r="T82" s="7"/>
+      <c r="U82" s="7"/>
+      <c r="V82" s="7"/>
+      <c r="W82" s="7"/>
+      <c r="X82" s="7"/>
+      <c r="Y82" s="7"/>
+      <c r="Z82" s="7"/>
+      <c r="AA82" s="7"/>
+      <c r="AB82" s="7"/>
+      <c r="AC82" s="7"/>
+      <c r="AD82" s="7"/>
+      <c r="AE82" s="7"/>
+      <c r="AF82" s="7"/>
+      <c r="AG82" s="7"/>
+      <c r="AH82" s="7"/>
+      <c r="AI82" s="7"/>
+      <c r="AJ82" s="7"/>
+      <c r="AK82" s="7"/>
+      <c r="AL82" s="7"/>
+      <c r="AM82" s="7"/>
+      <c r="AN82" s="7"/>
+      <c r="AO82" s="7"/>
+      <c r="AP82" s="7"/>
+      <c r="AQ82" s="7"/>
+      <c r="AR82" s="7"/>
+      <c r="AS82" s="7"/>
+      <c r="AT82" s="7"/>
+      <c r="AU82" s="7"/>
+      <c r="AV82" s="7"/>
+      <c r="AW82" s="7"/>
+      <c r="AX82" s="7"/>
+      <c r="AY82" s="7"/>
+      <c r="AZ82" s="7"/>
+      <c r="BA82" s="7"/>
+      <c r="BB82" s="7"/>
+      <c r="BC82" s="7"/>
+      <c r="BD82" s="7"/>
+      <c r="BE82" s="7"/>
+      <c r="BF82" s="7"/>
+    </row>
+    <row r="83" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0"/>
+      <c r="B83" s="0"/>
+      <c r="C83" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D83" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="0"/>
+      <c r="I83" s="0"/>
+      <c r="J83" s="0"/>
+      <c r="K83" s="0"/>
+      <c r="L83" s="0"/>
+      <c r="M83" s="0"/>
+      <c r="N83" s="0"/>
+      <c r="O83" s="0"/>
+      <c r="P83" s="0"/>
+      <c r="Q83" s="0"/>
+      <c r="R83" s="0"/>
+      <c r="S83" s="0"/>
+      <c r="T83" s="0"/>
+      <c r="U83" s="0"/>
+      <c r="V83" s="0"/>
+      <c r="W83" s="0"/>
+      <c r="X83" s="0"/>
+      <c r="Y83" s="0"/>
+      <c r="Z83" s="0"/>
+      <c r="AA83" s="0"/>
+      <c r="AB83" s="0"/>
+      <c r="AC83" s="0"/>
+      <c r="AD83" s="0"/>
+      <c r="AE83" s="0"/>
+      <c r="AF83" s="0"/>
+      <c r="AG83" s="0"/>
+      <c r="AH83" s="0"/>
+      <c r="AI83" s="0"/>
+      <c r="AJ83" s="0"/>
+      <c r="AK83" s="0"/>
+      <c r="AL83" s="0"/>
+      <c r="AM83" s="0"/>
+      <c r="AN83" s="0"/>
+      <c r="AO83" s="0"/>
+      <c r="AP83" s="0"/>
+      <c r="AQ83" s="0"/>
+      <c r="AR83" s="0"/>
+      <c r="AS83" s="0"/>
+      <c r="AT83" s="0"/>
+      <c r="AU83" s="0"/>
+      <c r="AV83" s="0"/>
+      <c r="AW83" s="0"/>
+      <c r="AX83" s="0"/>
+      <c r="AY83" s="0"/>
+      <c r="AZ83" s="0"/>
+      <c r="BA83" s="0"/>
+      <c r="BB83" s="0"/>
+      <c r="BC83" s="0"/>
+      <c r="BD83" s="0"/>
+      <c r="BE83" s="0"/>
+      <c r="BF83" s="0"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D84" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E84" s="12"/>
+      <c r="G84" s="12"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C85" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D85" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E85" s="12"/>
+      <c r="G85" s="12"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C86" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D86" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E86" s="12"/>
+      <c r="G86" s="12"/>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B87" s="24"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="12"/>
+      <c r="G87" s="12"/>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D88" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E88" s="12"/>
+      <c r="G88" s="12"/>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E89" s="12"/>
+      <c r="G89" s="12"/>
+    </row>
+    <row r="90" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0"/>
+      <c r="B90" s="0"/>
+      <c r="C90" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D90" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E90" s="12"/>
+      <c r="F90" s="0"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="0"/>
+      <c r="I90" s="0"/>
+      <c r="J90" s="0"/>
+      <c r="K90" s="0"/>
+      <c r="L90" s="0"/>
+      <c r="M90" s="0"/>
+      <c r="N90" s="0"/>
+      <c r="O90" s="0"/>
+      <c r="P90" s="0"/>
+      <c r="Q90" s="0"/>
+      <c r="R90" s="0"/>
+      <c r="S90" s="0"/>
+      <c r="T90" s="0"/>
+      <c r="U90" s="0"/>
+      <c r="V90" s="0"/>
+      <c r="W90" s="0"/>
+      <c r="X90" s="0"/>
+      <c r="Y90" s="0"/>
+      <c r="Z90" s="0"/>
+      <c r="AA90" s="0"/>
+      <c r="AB90" s="0"/>
+      <c r="AC90" s="0"/>
+      <c r="AD90" s="0"/>
+      <c r="AE90" s="0"/>
+      <c r="AF90" s="0"/>
+      <c r="AG90" s="0"/>
+      <c r="AH90" s="0"/>
+      <c r="AI90" s="0"/>
+      <c r="AJ90" s="0"/>
+      <c r="AK90" s="0"/>
+      <c r="AL90" s="0"/>
+      <c r="AM90" s="0"/>
+      <c r="AN90" s="0"/>
+      <c r="AO90" s="0"/>
+      <c r="AP90" s="0"/>
+      <c r="AQ90" s="0"/>
+      <c r="AR90" s="0"/>
+      <c r="AS90" s="0"/>
+      <c r="AT90" s="0"/>
+      <c r="AU90" s="0"/>
+      <c r="AV90" s="0"/>
+      <c r="AW90" s="0"/>
+      <c r="AX90" s="0"/>
+      <c r="AY90" s="0"/>
+      <c r="AZ90" s="0"/>
+      <c r="BA90" s="0"/>
+      <c r="BB90" s="0"/>
+      <c r="BC90" s="0"/>
+      <c r="BD90" s="0"/>
+      <c r="BE90" s="0"/>
+      <c r="BF90" s="0"/>
+    </row>
+    <row r="91" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B91" s="24"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="H91" s="7"/>
+      <c r="I91" s="7"/>
+      <c r="J91" s="7"/>
+      <c r="K91" s="7"/>
+      <c r="L91" s="7"/>
+      <c r="M91" s="7"/>
+      <c r="N91" s="7"/>
+      <c r="O91" s="7"/>
+      <c r="P91" s="7"/>
+      <c r="Q91" s="7"/>
+      <c r="R91" s="7"/>
+      <c r="S91" s="7"/>
+      <c r="T91" s="7"/>
+      <c r="U91" s="7"/>
+      <c r="V91" s="7"/>
+      <c r="W91" s="7"/>
+      <c r="X91" s="7"/>
+      <c r="Y91" s="7"/>
+      <c r="Z91" s="7"/>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7"/>
+      <c r="AC91" s="7"/>
+      <c r="AD91" s="7"/>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="7"/>
+      <c r="AG91" s="7"/>
+      <c r="AH91" s="7"/>
+      <c r="AI91" s="7"/>
+      <c r="AJ91" s="7"/>
+      <c r="AK91" s="7"/>
+      <c r="AL91" s="7"/>
+      <c r="AM91" s="7"/>
+      <c r="AN91" s="7"/>
+      <c r="AO91" s="7"/>
+      <c r="AP91" s="7"/>
+      <c r="AQ91" s="7"/>
+      <c r="AR91" s="7"/>
+      <c r="AS91" s="7"/>
+      <c r="AT91" s="7"/>
+      <c r="AU91" s="7"/>
+      <c r="AV91" s="7"/>
+      <c r="AW91" s="7"/>
+      <c r="AX91" s="7"/>
+      <c r="AY91" s="7"/>
+      <c r="AZ91" s="7"/>
+      <c r="BA91" s="7"/>
+      <c r="BB91" s="7"/>
+      <c r="BC91" s="7"/>
+      <c r="BD91" s="7"/>
+      <c r="BE91" s="7"/>
+      <c r="BF91" s="7"/>
+    </row>
+    <row r="92" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0"/>
+      <c r="B92" s="0"/>
+      <c r="C92" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D92" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E92" s="12"/>
+      <c r="F92" s="0"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="0"/>
+      <c r="I92" s="0"/>
+      <c r="J92" s="0"/>
+      <c r="K92" s="0"/>
+      <c r="L92" s="0"/>
+      <c r="M92" s="0"/>
+      <c r="N92" s="0"/>
+      <c r="O92" s="0"/>
+      <c r="P92" s="0"/>
+      <c r="Q92" s="0"/>
+      <c r="R92" s="0"/>
+      <c r="S92" s="0"/>
+      <c r="T92" s="0"/>
+      <c r="U92" s="0"/>
+      <c r="V92" s="0"/>
+      <c r="W92" s="0"/>
+      <c r="X92" s="0"/>
+      <c r="Y92" s="0"/>
+      <c r="Z92" s="0"/>
+      <c r="AA92" s="0"/>
+      <c r="AB92" s="0"/>
+      <c r="AC92" s="0"/>
+      <c r="AD92" s="0"/>
+      <c r="AE92" s="0"/>
+      <c r="AF92" s="0"/>
+      <c r="AG92" s="0"/>
+      <c r="AH92" s="0"/>
+      <c r="AI92" s="0"/>
+      <c r="AJ92" s="0"/>
+      <c r="AK92" s="0"/>
+      <c r="AL92" s="0"/>
+      <c r="AM92" s="0"/>
+      <c r="AN92" s="0"/>
+      <c r="AO92" s="0"/>
+      <c r="AP92" s="0"/>
+      <c r="AQ92" s="0"/>
+      <c r="AR92" s="0"/>
+      <c r="AS92" s="0"/>
+      <c r="AT92" s="0"/>
+      <c r="AU92" s="0"/>
+      <c r="AV92" s="0"/>
+      <c r="AW92" s="0"/>
+      <c r="AX92" s="0"/>
+      <c r="AY92" s="0"/>
+      <c r="AZ92" s="0"/>
+      <c r="BA92" s="0"/>
+      <c r="BB92" s="0"/>
+      <c r="BC92" s="0"/>
+      <c r="BD92" s="0"/>
+      <c r="BE92" s="0"/>
+      <c r="BF92" s="0"/>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C93" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D93" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E93" s="12"/>
+      <c r="G93" s="12"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B94" s="24"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="12"/>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C95" s="30"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="29"/>
+      <c r="G95" s="12"/>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B96" s="24"/>
+      <c r="C96" s="25"/>
+      <c r="D96" s="24"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="24"/>
+      <c r="G96" s="12"/>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C97" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D97" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E97" s="12"/>
+      <c r="G97" s="12"/>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C98" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D98" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E98" s="12"/>
+      <c r="G98" s="12"/>
+    </row>
+    <row r="99" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0"/>
+      <c r="B99" s="0"/>
+      <c r="C99" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D99" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E99" s="12"/>
+      <c r="F99" s="0"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="0"/>
+      <c r="I99" s="0"/>
+      <c r="J99" s="0"/>
+      <c r="K99" s="0"/>
+      <c r="L99" s="0"/>
+      <c r="M99" s="0"/>
+      <c r="N99" s="0"/>
+      <c r="O99" s="0"/>
+      <c r="P99" s="0"/>
+      <c r="Q99" s="0"/>
+      <c r="R99" s="0"/>
+      <c r="S99" s="0"/>
+      <c r="T99" s="0"/>
+      <c r="U99" s="0"/>
+      <c r="V99" s="0"/>
+      <c r="W99" s="0"/>
+      <c r="X99" s="0"/>
+      <c r="Y99" s="0"/>
+      <c r="Z99" s="0"/>
+      <c r="AA99" s="0"/>
+      <c r="AB99" s="0"/>
+      <c r="AC99" s="0"/>
+      <c r="AD99" s="0"/>
+      <c r="AE99" s="0"/>
+      <c r="AF99" s="0"/>
+      <c r="AG99" s="0"/>
+      <c r="AH99" s="0"/>
+      <c r="AI99" s="0"/>
+      <c r="AJ99" s="0"/>
+      <c r="AK99" s="0"/>
+      <c r="AL99" s="0"/>
+      <c r="AM99" s="0"/>
+      <c r="AN99" s="0"/>
+      <c r="AO99" s="0"/>
+      <c r="AP99" s="0"/>
+      <c r="AQ99" s="0"/>
+      <c r="AR99" s="0"/>
+      <c r="AS99" s="0"/>
+      <c r="AT99" s="0"/>
+      <c r="AU99" s="0"/>
+      <c r="AV99" s="0"/>
+      <c r="AW99" s="0"/>
+      <c r="AX99" s="0"/>
+      <c r="AY99" s="0"/>
+      <c r="AZ99" s="0"/>
+      <c r="BA99" s="0"/>
+      <c r="BB99" s="0"/>
+      <c r="BC99" s="0"/>
+      <c r="BD99" s="0"/>
+      <c r="BE99" s="0"/>
+      <c r="BF99" s="0"/>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C100" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D100" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E100" s="12"/>
+      <c r="G100" s="12"/>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C101" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D101" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E101" s="12"/>
+      <c r="G101" s="12"/>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C102" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D102" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E102" s="12"/>
+      <c r="G102" s="12"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B103" s="24"/>
+      <c r="C103" s="25"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="12"/>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C104" s="31"/>
+      <c r="D104" s="29"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="29"/>
+      <c r="G104" s="12"/>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B105" s="24"/>
+      <c r="C105" s="25"/>
+      <c r="D105" s="24"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="12"/>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C106" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D106" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E106" s="12"/>
+      <c r="G106" s="12"/>
+    </row>
+    <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C107" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D107" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="E107" s="12"/>
+      <c r="G107" s="12"/>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C108" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D108" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="E108" s="12"/>
+      <c r="G108" s="12"/>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C109" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E109" s="12"/>
+      <c r="G109" s="12"/>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C110" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D110" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E110" s="12"/>
+      <c r="G110" s="12"/>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C111" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D111" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E111" s="12"/>
+      <c r="G111" s="12"/>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C112" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D112" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E112" s="12"/>
+      <c r="G112" s="12"/>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C113" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D113" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E113" s="12"/>
+      <c r="G113" s="12"/>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C114" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D114" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E114" s="12"/>
+      <c r="G114" s="12"/>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C115" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D115" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E115" s="12"/>
+      <c r="G115" s="12"/>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C116" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D116" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="E116" s="12"/>
+      <c r="G116" s="12"/>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C117" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D117" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="E117" s="12"/>
+      <c r="G117" s="12"/>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B118" s="24"/>
+      <c r="C118" s="25"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="12"/>
+      <c r="F118" s="24"/>
+      <c r="G118" s="12"/>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C119" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D119" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E119" s="12"/>
+      <c r="G119" s="12"/>
+    </row>
+    <row r="120" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C120" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D120" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="E120" s="12"/>
+      <c r="G120" s="12"/>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B121" s="24"/>
+      <c r="C121" s="25"/>
+      <c r="D121" s="24"/>
+      <c r="E121" s="12"/>
+      <c r="F121" s="24"/>
+      <c r="G121" s="12"/>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C122" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D122" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="E122" s="12"/>
+      <c r="G122" s="12"/>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C123" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D123" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E123" s="12"/>
+      <c r="G123" s="12"/>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C124" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D124" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E124" s="12"/>
+      <c r="G124" s="12"/>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B125" s="24"/>
+      <c r="C125" s="25"/>
+      <c r="D125" s="24"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="24"/>
+      <c r="G125" s="12"/>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C126" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D126" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="E126" s="12"/>
+      <c r="G126" s="12"/>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C127" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D127" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E127" s="12"/>
+      <c r="G127" s="12"/>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C128" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D128" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E128" s="12"/>
+      <c r="G128" s="12"/>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B129" s="24"/>
+      <c r="C129" s="25"/>
+      <c r="D129" s="24"/>
+      <c r="E129" s="12"/>
+      <c r="G129" s="12"/>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D107" r:id="rId1" display="https://mjbright.github.io/Talks"/>
+    <hyperlink ref="D120" r:id="rId2" display="2012-Nov 2nd place: https://www.archionline.com/"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
+  <dimension ref="A1:BF65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>151</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>152</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="13" t="s">
@@ -3449,7 +5414,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="11" t="s">
@@ -3462,7 +5427,7 @@
         <v>42</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="21" t="s">
@@ -3475,7 +5440,7 @@
         <v>53</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="15" t="s">
@@ -3514,7 +5479,7 @@
         <v>62</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="0" t="s">
@@ -3527,7 +5492,7 @@
         <v>62</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="0" t="s">
@@ -3540,11 +5505,11 @@
         <v>62</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="13"/>
@@ -4272,7 +6237,7 @@
         <v>62</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E77" s="12"/>
       <c r="G77" s="12"/>
@@ -4434,7 +6399,7 @@
         <v>62</v>
       </c>
       <c r="D83" s="21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E83" s="12"/>
       <c r="G83" s="12"/>
@@ -4476,7 +6441,7 @@
         <v>62</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E87" s="12"/>
       <c r="F87" s="0"/>
@@ -4663,7 +6628,7 @@
         <v>62</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E90" s="12"/>
       <c r="G90" s="12"/>
@@ -4934,7 +6899,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D111" s="35" t="s">
         <v>140</v>
@@ -4944,7 +6909,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D112" s="35" t="s">
         <v>141</v>
@@ -4954,7 +6919,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D113" s="35" t="s">
         <v>142</v>
@@ -5132,7 +7097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
@@ -5145,16 +7110,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.1938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5230,7 +7195,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>12</v>
+        <v>151</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="13" t="s">
@@ -5259,18 +7224,18 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="13" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5294,7 +7259,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="13" t="s">
@@ -5326,7 +7291,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="13" t="s">
@@ -5374,7 +7339,7 @@
         <v>46</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
@@ -5402,7 +7367,7 @@
         <v>34</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="11" t="s">
@@ -5415,7 +7380,7 @@
         <v>42</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="21" t="s">
@@ -5428,7 +7393,7 @@
         <v>53</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="15" t="s">
@@ -5467,7 +7432,7 @@
         <v>62</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="0" t="s">
@@ -5480,7 +7445,7 @@
         <v>62</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="0" t="s">
@@ -5493,11 +7458,11 @@
         <v>62</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G23" s="12"/>
     </row>
@@ -6224,7 +8189,7 @@
         <v>62</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E78" s="12"/>
       <c r="G78" s="12"/>
@@ -6386,7 +8351,7 @@
         <v>62</v>
       </c>
       <c r="D84" s="21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E84" s="12"/>
       <c r="G84" s="12"/>
@@ -6428,7 +8393,7 @@
         <v>62</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E88" s="12"/>
       <c r="F88" s="0"/>
@@ -6615,7 +8580,7 @@
         <v>62</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E91" s="12"/>
       <c r="G91" s="12"/>
@@ -6886,7 +8851,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D112" s="35" t="s">
         <v>140</v>
@@ -6896,7 +8861,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D113" s="35" t="s">
         <v>141</v>
@@ -6906,7 +8871,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D114" s="35" t="s">
         <v>142</v>

</xml_diff>

<commit_message>
Changed subsection title to 'Meetup Organizer' and added Meetup links.
</commit_message>
<xml_diff>
--- a/static/docs/src/CV.xlsx
+++ b/static/docs/src/CV.xlsx
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="216">
   <si>
     <t xml:space="preserve">SECTION</t>
   </si>
@@ -585,70 +585,79 @@
     <t xml:space="preserve">Rock, Argentinian Tango, Salsa, Music, Cinema</t>
   </si>
   <si>
+    <t xml:space="preserve">Meetup Organizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenoble Python User Group organiser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- https://www.meetup.com/Groupe-dutilisateurs-Python-Grenoble/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenoble Docker and FLOSS User Groups co-organiser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- https://www.meetup.com/Docker-Grenoble/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNCF Kubernetes CKA, RHCE, RHCSA, HPE Expert One SDN Apps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective - Pre-sales Solution Architect or Technical Lead on Cloud Native, Container and Automation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Container Orchestration Labs (Docker Swarm, Kubernetes, Apache Mesos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated test frameworks for IaaS cloud product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agile development of Data analytics and service profile platforms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Agile team (SCRUM, TDD, Continuous Integration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Software development, unit and functional tests for SOAP and REST frameworks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposed/implemented automated VideoXML dialog creation from PPT for MWC PoC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOOCs in the areas of BigData, Software Defined Networks, Databases, Agile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-sales technical consulting on OpenCall products and proof of concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer/Partner contact and ITSM delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Deployments KT VoIP benchtest, Tuka IN, DCC Prepaid, FT VHE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  ITSE Workshop delivery (Bouygues prepaid, Polkomtel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Technical Lead for HKTel Y2K migration,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--  Design and implementation of SCE and SLEE modules (HA, Mib, MemoryHandler).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research into design and modeling of data/signalling networks (X.25, SS7, ethernet)  leading to PoC demos and HP products </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z-filter design, simulation, bit-slice micro-processor coding and user subjectivity tests of NICAM digital audio subjective noise reduction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripting languages (Python/Perl/Ruby/PHP), C++/C, Java, Scala, JavaScript, JQuery, FP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</t>
+  </si>
+  <si>
     <t xml:space="preserve">Technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenoble Python User Group organiser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenoble Docker and FLOSS User Groups co-organiser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNCF Kubernetes CKA, RHCE, RHCSA, HPE Expert One SDN Apps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Objective - Pre-sales Solution Architect or Technical Lead on Cloud Native, Container and Automation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Container Orchestration Labs (Docker Swarm, Kubernetes, Apache Mesos)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automated test frameworks for IaaS cloud product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agile development of Data analytics and service profile platforms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Agile team (SCRUM, TDD, Continuous Integration)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Software development, unit and functional tests for SOAP and REST frameworks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposed/implemented automated VideoXML dialog creation from PPT for MWC PoC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOOCs in the areas of BigData, Software Defined Networks, Databases, Agile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-sales technical consulting on OpenCall products and proof of concepts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer/Partner contact and ITSM delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Deployments KT VoIP benchtest, Tuka IN, DCC Prepaid, FT VHE.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  ITSE Workshop delivery (Bouygues prepaid, Polkomtel)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Technical Lead for HKTel Y2K migration,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--  Design and implementation of SCE and SLEE modules (HA, Mib, MemoryHandler).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research into design and modeling of data/signalling networks (X.25, SS7, ethernet)  leading to PoC demos and HP products </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z-filter design, simulation, bit-slice micro-processor coding and user subjectivity tests of NICAM digital audio subjective noise reduction.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scripting languages (Python/Perl/Ruby/PHP), C++/C, Java, Scala, JavaScript, JQuery, FP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</t>
   </si>
   <si>
     <t xml:space="preserve">RHCE, RHCSA, HPE Expert One SDN Apps</t>
@@ -1289,10 +1298,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:BF139"/>
+  <dimension ref="A1:BF141"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A104" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D129" activeCellId="0" sqref="D129"/>
+      <selection pane="topLeft" activeCell="D136" activeCellId="0" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -3297,17 +3306,35 @@
       <c r="G137" s="12"/>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B138" s="24"/>
-      <c r="C138" s="25"/>
-      <c r="D138" s="24"/>
+      <c r="C138" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D138" s="20" t="s">
+        <v>161</v>
+      </c>
       <c r="E138" s="12"/>
       <c r="G138" s="12"/>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C139" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D139" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="E139" s="12"/>
+      <c r="G139" s="12"/>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B140" s="24"/>
+      <c r="C140" s="25"/>
+      <c r="D140" s="24"/>
+      <c r="E140" s="12"/>
+      <c r="G140" s="12"/>
+    </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3351,6 +3378,8 @@
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
@@ -3470,7 +3499,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="13" t="s">
@@ -3546,7 +3575,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="13"/>
@@ -3713,7 +3742,7 @@
         <v>61</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="0" t="s">
@@ -3837,7 +3866,7 @@
         <v>61</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="0"/>
@@ -3848,7 +3877,7 @@
         <v>61</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E34" s="14"/>
       <c r="G34" s="12"/>
@@ -3858,7 +3887,7 @@
         <v>61</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E35" s="14"/>
       <c r="G35" s="12"/>
@@ -3868,7 +3897,7 @@
         <v>61</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="12"/>
@@ -3878,7 +3907,7 @@
         <v>61</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E37" s="14"/>
       <c r="G37" s="12"/>
@@ -3888,7 +3917,7 @@
         <v>61</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E38" s="14"/>
       <c r="G38" s="26"/>
@@ -3953,7 +3982,7 @@
         <v>61</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E44" s="14"/>
       <c r="G44" s="12"/>
@@ -3973,7 +4002,7 @@
         <v>61</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E46" s="14"/>
       <c r="G46" s="12"/>
@@ -3995,7 +4024,7 @@
         <v>61</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="0"/>
@@ -4059,7 +4088,7 @@
         <v>61</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="0"/>
@@ -4122,7 +4151,7 @@
         <v>61</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="0"/>
@@ -4274,7 +4303,7 @@
         <v>61</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E60" s="14"/>
       <c r="G60" s="12"/>
@@ -4344,7 +4373,7 @@
         <v>61</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E67" s="14"/>
       <c r="G67" s="12"/>
@@ -4414,7 +4443,7 @@
         <v>61</v>
       </c>
       <c r="D74" s="20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E74" s="14"/>
       <c r="G74" s="12"/>
@@ -4659,7 +4688,7 @@
         <v>61</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E88" s="12"/>
       <c r="G88" s="12"/>
@@ -4669,7 +4698,7 @@
         <v>61</v>
       </c>
       <c r="D89" s="20" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E89" s="12"/>
       <c r="G89" s="12"/>
@@ -5305,7 +5334,7 @@
         <v>34</v>
       </c>
       <c r="D130" s="19" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="E130" s="12"/>
       <c r="G130" s="12"/>
@@ -5325,7 +5354,7 @@
         <v>61</v>
       </c>
       <c r="D132" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E132" s="12"/>
       <c r="G132" s="12"/>
@@ -5505,7 +5534,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="13" t="s">
@@ -5581,7 +5610,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="13"/>
@@ -5654,10 +5683,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="13" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="22"/>
@@ -5750,7 +5779,7 @@
         <v>61</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E22" s="12"/>
       <c r="G22" s="12"/>
@@ -5760,7 +5789,7 @@
         <v>61</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="0" t="s">
@@ -5773,7 +5802,7 @@
         <v>61</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="0" t="s">
@@ -5786,7 +5815,7 @@
         <v>61</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E25" s="12"/>
       <c r="G25" s="12"/>
@@ -5884,7 +5913,7 @@
         <v>61</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="0"/>
@@ -5895,7 +5924,7 @@
         <v>61</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E35" s="14"/>
       <c r="G35" s="12"/>
@@ -5905,7 +5934,7 @@
         <v>61</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="12"/>
@@ -5915,7 +5944,7 @@
         <v>61</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E37" s="14"/>
       <c r="G37" s="12"/>
@@ -5925,7 +5954,7 @@
         <v>61</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E38" s="14"/>
       <c r="G38" s="12"/>
@@ -5935,7 +5964,7 @@
         <v>61</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E39" s="14"/>
       <c r="G39" s="26"/>
@@ -6000,7 +6029,7 @@
         <v>61</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E45" s="14"/>
       <c r="G45" s="12"/>
@@ -6010,7 +6039,7 @@
         <v>61</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E46" s="14"/>
       <c r="G46" s="12"/>
@@ -6020,7 +6049,7 @@
         <v>61</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E47" s="14"/>
       <c r="G47" s="12"/>
@@ -6042,7 +6071,7 @@
         <v>61</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="0"/>
@@ -6106,7 +6135,7 @@
         <v>61</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="0"/>
@@ -6169,7 +6198,7 @@
         <v>61</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E51" s="14"/>
       <c r="F51" s="0"/>
@@ -6241,7 +6270,7 @@
         <v>34</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E53" s="14"/>
       <c r="G53" s="12"/>
@@ -6321,7 +6350,7 @@
         <v>61</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E61" s="14"/>
       <c r="G61" s="12"/>
@@ -6391,7 +6420,7 @@
         <v>61</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E68" s="14"/>
       <c r="G68" s="12"/>
@@ -6461,7 +6490,7 @@
         <v>61</v>
       </c>
       <c r="D75" s="20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E75" s="14"/>
       <c r="G75" s="12"/>
@@ -6656,7 +6685,7 @@
         <v>61</v>
       </c>
       <c r="D84" s="20" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E84" s="12"/>
       <c r="G84" s="12"/>
@@ -6666,7 +6695,7 @@
         <v>61</v>
       </c>
       <c r="D85" s="20" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E85" s="12"/>
       <c r="G85" s="12"/>
@@ -7302,7 +7331,7 @@
         <v>34</v>
       </c>
       <c r="D126" s="19" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="E126" s="12"/>
       <c r="G126" s="12"/>
@@ -7322,7 +7351,7 @@
         <v>61</v>
       </c>
       <c r="D128" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E128" s="12"/>
       <c r="G128" s="12"/>
@@ -7506,7 +7535,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="13" t="s">
@@ -7554,7 +7583,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="13" t="s">
@@ -7631,10 +7660,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="13" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="22"/>
@@ -7662,7 +7691,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="11" t="s">
@@ -7675,7 +7704,7 @@
         <v>42</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="20" t="s">
@@ -7688,7 +7717,7 @@
         <v>52</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="22" t="s">
@@ -7727,7 +7756,7 @@
         <v>61</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="0" t="s">
@@ -7740,7 +7769,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="0" t="s">
@@ -7753,11 +7782,11 @@
         <v>61</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="13"/>
@@ -7855,7 +7884,7 @@
         <v>61</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="0"/>
@@ -7866,7 +7895,7 @@
         <v>61</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E32" s="14"/>
       <c r="G32" s="12"/>
@@ -7876,7 +7905,7 @@
         <v>61</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E33" s="14"/>
       <c r="G33" s="12"/>
@@ -7886,7 +7915,7 @@
         <v>61</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E34" s="14"/>
       <c r="G34" s="12"/>
@@ -7896,7 +7925,7 @@
         <v>61</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E35" s="14"/>
       <c r="G35" s="12"/>
@@ -7906,7 +7935,7 @@
         <v>61</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="26"/>
@@ -7971,7 +8000,7 @@
         <v>61</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E42" s="14"/>
       <c r="G42" s="12"/>
@@ -7981,7 +8010,7 @@
         <v>61</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E43" s="14"/>
       <c r="G43" s="12"/>
@@ -7991,7 +8020,7 @@
         <v>61</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E44" s="14"/>
       <c r="G44" s="12"/>
@@ -8013,7 +8042,7 @@
         <v>61</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="0"/>
@@ -8077,7 +8106,7 @@
         <v>61</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="0"/>
@@ -8140,7 +8169,7 @@
         <v>61</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="0"/>
@@ -8212,7 +8241,7 @@
         <v>34</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E50" s="14"/>
       <c r="G50" s="12"/>
@@ -8292,7 +8321,7 @@
         <v>61</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E58" s="14"/>
       <c r="G58" s="12"/>
@@ -8362,7 +8391,7 @@
         <v>61</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E65" s="14"/>
       <c r="G65" s="12"/>
@@ -8432,7 +8461,7 @@
         <v>61</v>
       </c>
       <c r="D72" s="20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E72" s="14"/>
       <c r="G72" s="12"/>
@@ -8485,7 +8514,7 @@
         <v>61</v>
       </c>
       <c r="D77" s="20" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E77" s="12"/>
       <c r="G77" s="12"/>
@@ -8627,7 +8656,7 @@
         <v>61</v>
       </c>
       <c r="D81" s="20" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E81" s="12"/>
       <c r="G81" s="12"/>
@@ -8637,7 +8666,7 @@
         <v>61</v>
       </c>
       <c r="D82" s="20" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E82" s="12"/>
       <c r="G82" s="12"/>
@@ -8647,7 +8676,7 @@
         <v>61</v>
       </c>
       <c r="D83" s="20" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E83" s="12"/>
       <c r="G83" s="12"/>
@@ -8689,7 +8718,7 @@
         <v>61</v>
       </c>
       <c r="D87" s="20" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E87" s="12"/>
       <c r="F87" s="0"/>
@@ -8876,7 +8905,7 @@
         <v>61</v>
       </c>
       <c r="D90" s="20" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E90" s="12"/>
       <c r="G90" s="12"/>
@@ -9147,7 +9176,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="13" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D111" s="36" t="s">
         <v>150</v>
@@ -9157,7 +9186,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="13" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D112" s="36" t="s">
         <v>151</v>
@@ -9167,7 +9196,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="13" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D113" s="36" t="s">
         <v>152</v>
@@ -9232,7 +9261,7 @@
         <v>34</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="E119" s="12"/>
       <c r="G119" s="12"/>
@@ -9252,7 +9281,7 @@
         <v>61</v>
       </c>
       <c r="D121" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E121" s="12"/>
       <c r="G121" s="12"/>
@@ -9443,7 +9472,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="13" t="s">
@@ -9472,18 +9501,18 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="13" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="13" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="13" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9507,7 +9536,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="13" t="s">
@@ -9539,7 +9568,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="13" t="s">
@@ -9584,10 +9613,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="13" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="22"/>
@@ -9615,7 +9644,7 @@
         <v>34</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="11" t="s">
@@ -9628,7 +9657,7 @@
         <v>42</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="20" t="s">
@@ -9641,7 +9670,7 @@
         <v>52</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="22" t="s">
@@ -9680,7 +9709,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="0" t="s">
@@ -9693,7 +9722,7 @@
         <v>61</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="0" t="s">
@@ -9706,11 +9735,11 @@
         <v>61</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G23" s="12"/>
     </row>
@@ -9807,7 +9836,7 @@
         <v>61</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="0"/>
@@ -9818,7 +9847,7 @@
         <v>61</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E33" s="14"/>
       <c r="G33" s="12"/>
@@ -9828,7 +9857,7 @@
         <v>61</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E34" s="14"/>
       <c r="G34" s="12"/>
@@ -9838,7 +9867,7 @@
         <v>61</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E35" s="14"/>
       <c r="G35" s="12"/>
@@ -9848,7 +9877,7 @@
         <v>61</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="12"/>
@@ -9858,7 +9887,7 @@
         <v>61</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E37" s="14"/>
       <c r="G37" s="26"/>
@@ -9923,7 +9952,7 @@
         <v>61</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E43" s="14"/>
       <c r="G43" s="12"/>
@@ -9933,7 +9962,7 @@
         <v>61</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E44" s="14"/>
       <c r="G44" s="12"/>
@@ -9943,7 +9972,7 @@
         <v>61</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E45" s="14"/>
       <c r="G45" s="12"/>
@@ -9965,7 +9994,7 @@
         <v>61</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="0"/>
@@ -10029,7 +10058,7 @@
         <v>61</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="0"/>
@@ -10092,7 +10121,7 @@
         <v>61</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="0"/>
@@ -10164,7 +10193,7 @@
         <v>34</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E51" s="14"/>
       <c r="G51" s="12"/>
@@ -10244,7 +10273,7 @@
         <v>61</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E59" s="14"/>
       <c r="G59" s="12"/>
@@ -10314,7 +10343,7 @@
         <v>61</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E66" s="14"/>
       <c r="G66" s="12"/>
@@ -10384,7 +10413,7 @@
         <v>61</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E73" s="14"/>
       <c r="G73" s="12"/>
@@ -10437,7 +10466,7 @@
         <v>61</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E78" s="12"/>
       <c r="G78" s="12"/>
@@ -10579,7 +10608,7 @@
         <v>61</v>
       </c>
       <c r="D82" s="20" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E82" s="12"/>
       <c r="G82" s="12"/>
@@ -10589,7 +10618,7 @@
         <v>61</v>
       </c>
       <c r="D83" s="20" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E83" s="12"/>
       <c r="G83" s="12"/>
@@ -10599,7 +10628,7 @@
         <v>61</v>
       </c>
       <c r="D84" s="20" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E84" s="12"/>
       <c r="G84" s="12"/>
@@ -10641,7 +10670,7 @@
         <v>61</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E88" s="12"/>
       <c r="F88" s="0"/>
@@ -10828,7 +10857,7 @@
         <v>61</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E91" s="12"/>
       <c r="G91" s="12"/>
@@ -11099,7 +11128,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="13" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D112" s="36" t="s">
         <v>150</v>
@@ -11109,7 +11138,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="13" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D113" s="36" t="s">
         <v>151</v>
@@ -11119,7 +11148,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="13" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D114" s="36" t="s">
         <v>152</v>
@@ -11184,7 +11213,7 @@
         <v>34</v>
       </c>
       <c r="D120" s="19" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="E120" s="12"/>
       <c r="G120" s="12"/>
@@ -11204,7 +11233,7 @@
         <v>61</v>
       </c>
       <c r="D122" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E122" s="12"/>
       <c r="G122" s="12"/>

</xml_diff>

<commit_message>
No real changes, just updating script to be WSL/DOcker compatible
</commit_message>
<xml_diff>
--- a/static/docs/src/CV.xlsx
+++ b/static/docs/src/CV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windo\Dropbox\z\www\mjbright.github.io\static\docs\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AD99F4-69D3-40EF-BF84-3EFA2EE14A81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D655BF2-2895-4B3C-963F-67655E3A1338}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="222">
   <si>
     <t>SECTION</t>
   </si>
@@ -712,6 +712,15 @@
   </si>
   <si>
     <t>+33 (0)652891534</t>
+  </si>
+  <si>
+    <t>06/2018</t>
+  </si>
+  <si>
+    <t>#COMMENT</t>
+  </si>
+  <si>
+    <t>2018-Nov: Community Security System</t>
   </si>
 </sst>
 </file>
@@ -1384,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1826,7 +1835,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" t="s">
@@ -1964,7 +1973,7 @@
     </row>
     <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C41" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>72</v>
@@ -2000,7 +2009,7 @@
     </row>
     <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C44" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>75</v>
@@ -2010,7 +2019,7 @@
     </row>
     <row r="45" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C45" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>76</v>
@@ -2108,7 +2117,7 @@
     </row>
     <row r="54" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C54" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D54" s="11" t="s">
         <v>83</v>
@@ -2128,7 +2137,7 @@
     </row>
     <row r="56" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C56" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>85</v>
@@ -2138,7 +2147,7 @@
     </row>
     <row r="57" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C57" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D57" s="19" t="s">
         <v>86</v>
@@ -2148,7 +2157,7 @@
     </row>
     <row r="58" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C58" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D58" s="19" t="s">
         <v>87</v>
@@ -2164,7 +2173,7 @@
     </row>
     <row r="59" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C59" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D59" s="19" t="s">
         <v>88</v>
@@ -2234,7 +2243,7 @@
     </row>
     <row r="66" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C66" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D66" s="11" t="s">
         <v>92</v>
@@ -2244,7 +2253,7 @@
     </row>
     <row r="67" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C67" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>93</v>
@@ -2264,7 +2273,7 @@
     </row>
     <row r="69" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C69" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D69" s="11" t="s">
         <v>95</v>
@@ -2274,7 +2283,7 @@
     </row>
     <row r="70" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C70" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D70" s="11" t="s">
         <v>96</v>
@@ -2876,7 +2885,7 @@
         <v>60</v>
       </c>
       <c r="D127" s="35" t="s">
-        <v>140</v>
+        <v>221</v>
       </c>
       <c r="E127" s="10"/>
       <c r="G127" s="10"/>

</xml_diff>

<commit_message>
Updated with current activities (Freelance Cloud Native: Training, Consulting, Conference Speaker) Added CKAD certif Added OpenShift demo Added Conuslting - Kubernetes Implementation
</commit_message>
<xml_diff>
--- a/static/docs/src/CV.xlsx
+++ b/static/docs/src/CV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windo\Dropbox\z\www\mjbright.github.io\static\docs\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D655BF2-2895-4B3C-963F-67655E3A1338}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F136610F-4D7A-43EE-B47A-D21DDCC768AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CV" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <definedName name="MONINT" localSheetId="2">#REF!</definedName>
     <definedName name="MONINT">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179017" iterateDelta="1E-4"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="227">
   <si>
     <t>SECTION</t>
   </si>
@@ -721,6 +721,21 @@
   </si>
   <si>
     <t>2018-Nov: Community Security System</t>
+  </si>
+  <si>
+    <t>CNCF Kubernetes CKA, CKAD, RedHat RHCE/RHCSA</t>
+  </si>
+  <si>
+    <t>Consulting - Kubernetes Implementation</t>
+  </si>
+  <si>
+    <t>Trainer, Consultant, Conference Speaker</t>
+  </si>
+  <si>
+    <t>Freelancing on Cloud Native - Docker, Kubernetes, Serverless</t>
+  </si>
+  <si>
+    <t>Creation of OpenShift Demo Platform</t>
   </si>
 </sst>
 </file>
@@ -1001,13 +1016,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1391,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M139"/>
+  <dimension ref="A1:M141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1412,20 +1427,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -1478,7 +1493,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>12</v>
+        <v>222</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="11" t="s">
@@ -1493,7 +1508,7 @@
       <c r="C5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="40" t="s">
         <v>218</v>
       </c>
       <c r="E5" s="12"/>
@@ -1566,7 +1581,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="11"/>
@@ -1594,7 +1609,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="11" t="s">
@@ -1742,8 +1757,8 @@
       <c r="C22" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>214</v>
+      <c r="D22" s="39" t="s">
+        <v>223</v>
       </c>
       <c r="E22" s="10"/>
       <c r="G22" s="10"/>
@@ -1753,117 +1768,114 @@
         <v>60</v>
       </c>
       <c r="D23" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C24" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" t="s">
+      <c r="E24" s="10"/>
+      <c r="F24" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-    </row>
-    <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+    </row>
+    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D26" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="8" t="s">
+      <c r="E26" s="10"/>
+      <c r="F26" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C26" s="8" t="s">
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C27" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="19" t="s">
+      <c r="E27" s="10"/>
+      <c r="F27" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D28" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="21" t="s">
+      <c r="E28" s="10"/>
+      <c r="F28" s="21" t="s">
         <v>53</v>
-      </c>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C28" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="10"/>
-      <c r="F28" t="s">
-        <v>56</v>
       </c>
       <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C29" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>219</v>
+        <v>54</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C30" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>219</v>
       </c>
       <c r="E30" s="10"/>
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
       <c r="G30" s="10"/>
     </row>
     <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C31" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>62</v>
+      <c r="D31" s="39" t="s">
+        <v>226</v>
       </c>
       <c r="E31" s="10"/>
-      <c r="F31" t="s">
-        <v>63</v>
-      </c>
       <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
@@ -1871,12 +1883,9 @@
         <v>60</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E32" s="10"/>
-      <c r="F32" t="s">
-        <v>65</v>
-      </c>
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
@@ -1884,67 +1893,71 @@
         <v>60</v>
       </c>
       <c r="D33" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C34" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C35" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="10"/>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
+      <c r="E35" s="10"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-    </row>
-    <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C35" s="11" t="s">
+      <c r="B36" s="23"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C37" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D37" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="E35" s="12"/>
-      <c r="G35" s="25"/>
-      <c r="I35" s="26"/>
-    </row>
-    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C36" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="12"/>
-      <c r="G36" s="25"/>
-      <c r="I36" s="26"/>
-    </row>
-    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C37" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="E37" s="12"/>
       <c r="G37" s="25"/>
       <c r="I37" s="26"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C38" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>55</v>
+      <c r="C38" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="E38" s="12"/>
       <c r="G38" s="25"/>
@@ -1952,175 +1965,177 @@
     </row>
     <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C39" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E39" s="12"/>
       <c r="G39" s="25"/>
       <c r="I39" s="26"/>
     </row>
-    <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C40" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="E40" s="12"/>
-      <c r="G40" s="10"/>
-    </row>
-    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="G40" s="25"/>
+      <c r="I40" s="26"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C41" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E41" s="12"/>
-      <c r="G41" s="10"/>
+      <c r="G41" s="25"/>
+      <c r="I41" s="26"/>
     </row>
     <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C42" s="21" t="s">
         <v>60</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E42" s="12"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="16"/>
-      <c r="M42" s="16"/>
     </row>
     <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C43" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E43" s="12"/>
       <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C44" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E44" s="12"/>
       <c r="G44" s="10"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
     </row>
     <row r="45" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C45" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E45" s="12"/>
       <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C46" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E46" s="12"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C47" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D47" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" s="12"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C48" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" s="12"/>
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C49" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E47" s="12"/>
-      <c r="G47" s="25"/>
-      <c r="I47" s="26"/>
-    </row>
-    <row r="48" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
+      <c r="E49" s="12"/>
+      <c r="G49" s="25"/>
+      <c r="I49" s="26"/>
+    </row>
+    <row r="50" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="10"/>
-    </row>
-    <row r="49" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C49" s="11" t="s">
+      <c r="B50" s="23"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C51" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D51" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="E49" s="12"/>
-      <c r="G49" s="10"/>
-    </row>
-    <row r="50" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C50" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E50" s="12"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
-      <c r="J50" s="16"/>
-      <c r="K50" s="16"/>
-      <c r="L50" s="16"/>
-      <c r="M50" s="16"/>
-    </row>
-    <row r="51" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C51" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51" s="27" t="s">
-        <v>81</v>
       </c>
       <c r="E51" s="12"/>
       <c r="G51" s="10"/>
     </row>
-    <row r="52" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C52" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>69</v>
+    <row r="52" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C52" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>80</v>
       </c>
       <c r="E52" s="12"/>
       <c r="G52" s="10"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
     </row>
     <row r="53" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C53" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>82</v>
+        <v>54</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>81</v>
       </c>
       <c r="E53" s="12"/>
       <c r="G53" s="10"/>
     </row>
     <row r="54" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C54" s="21" t="s">
-        <v>220</v>
+        <v>57</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E54" s="12"/>
       <c r="G54" s="10"/>
@@ -2130,7 +2145,7 @@
         <v>60</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E55" s="12"/>
       <c r="G55" s="10"/>
@@ -2139,18 +2154,18 @@
       <c r="C56" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="D56" s="19" t="s">
-        <v>85</v>
+      <c r="D56" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="E56" s="12"/>
       <c r="G56" s="10"/>
     </row>
     <row r="57" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C57" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="D57" s="19" t="s">
-        <v>86</v>
+        <v>60</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="E57" s="12"/>
       <c r="G57" s="10"/>
@@ -2160,113 +2175,113 @@
         <v>220</v>
       </c>
       <c r="D58" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E58" s="12"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9"/>
-      <c r="M58" s="9"/>
+      <c r="G58" s="10"/>
     </row>
     <row r="59" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C59" s="21" t="s">
         <v>220</v>
       </c>
       <c r="D59" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E59" s="12"/>
       <c r="G59" s="10"/>
     </row>
-    <row r="60" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="23"/>
+    <row r="60" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C60" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="E60" s="12"/>
-      <c r="G60" s="10"/>
-    </row>
-    <row r="61" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C61" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" s="18" t="s">
-        <v>89</v>
+      <c r="G60" s="14"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+    </row>
+    <row r="61" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C61" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="E61" s="12"/>
       <c r="G61" s="10"/>
     </row>
-    <row r="62" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C62" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>80</v>
-      </c>
+    <row r="62" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" s="23"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="23"/>
       <c r="E62" s="12"/>
       <c r="G62" s="10"/>
     </row>
-    <row r="63" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C63" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D63" s="27" t="s">
-        <v>90</v>
+    <row r="63" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C63" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="E63" s="12"/>
       <c r="G63" s="10"/>
     </row>
-    <row r="64" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C64" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>81</v>
+    <row r="64" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C64" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>80</v>
       </c>
       <c r="E64" s="12"/>
       <c r="G64" s="10"/>
     </row>
     <row r="65" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C65" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>91</v>
+        <v>54</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>90</v>
       </c>
       <c r="E65" s="12"/>
       <c r="G65" s="10"/>
     </row>
     <row r="66" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C66" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>92</v>
+        <v>57</v>
+      </c>
+      <c r="D66" s="27" t="s">
+        <v>81</v>
       </c>
       <c r="E66" s="12"/>
       <c r="G66" s="10"/>
     </row>
     <row r="67" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C67" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E67" s="12"/>
       <c r="G67" s="10"/>
     </row>
     <row r="68" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C68" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E68" s="12"/>
       <c r="G68" s="10"/>
@@ -2276,310 +2291,310 @@
         <v>220</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E69" s="12"/>
       <c r="G69" s="10"/>
     </row>
     <row r="70" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C70" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E70" s="12"/>
       <c r="G70" s="10"/>
     </row>
-    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B71" s="23"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="23"/>
+    <row r="71" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C71" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>95</v>
+      </c>
       <c r="E71" s="12"/>
       <c r="G71" s="10"/>
     </row>
-    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C72" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>97</v>
+    <row r="72" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C72" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="E72" s="12"/>
       <c r="G72" s="10"/>
     </row>
-    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C73" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>98</v>
-      </c>
+    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73" s="23"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="23"/>
       <c r="E73" s="12"/>
       <c r="G73" s="10"/>
     </row>
-    <row r="74" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C74" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D74" s="27" t="s">
-        <v>99</v>
+    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C74" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="E74" s="12"/>
       <c r="G74" s="10"/>
     </row>
-    <row r="75" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C75" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D75" s="27" t="s">
-        <v>90</v>
+    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C75" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="E75" s="12"/>
       <c r="G75" s="10"/>
     </row>
     <row r="76" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C76" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>100</v>
+        <v>54</v>
+      </c>
+      <c r="D76" s="27" t="s">
+        <v>99</v>
       </c>
       <c r="E76" s="12"/>
       <c r="G76" s="10"/>
     </row>
     <row r="77" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C77" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>101</v>
+        <v>57</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>90</v>
       </c>
       <c r="E77" s="12"/>
       <c r="G77" s="10"/>
     </row>
-    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B78" s="23"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="23"/>
+    <row r="78" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C78" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>100</v>
+      </c>
       <c r="E78" s="12"/>
       <c r="G78" s="10"/>
     </row>
-    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C79" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D79" s="18" t="s">
-        <v>102</v>
+    <row r="79" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C79" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="E79" s="12"/>
       <c r="G79" s="10"/>
     </row>
-    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C80" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D80" s="18" t="s">
-        <v>103</v>
-      </c>
+    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B80" s="23"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="23"/>
       <c r="E80" s="12"/>
       <c r="G80" s="10"/>
     </row>
-    <row r="81" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C81" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D81" s="27" t="s">
-        <v>104</v>
+    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C81" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="E81" s="12"/>
       <c r="G81" s="10"/>
     </row>
-    <row r="82" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C82" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D82" s="27" t="s">
-        <v>105</v>
+    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C82" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="E82" s="12"/>
       <c r="G82" s="10"/>
     </row>
-    <row r="83" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C83" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D83" s="19" t="s">
-        <v>106</v>
+        <v>54</v>
+      </c>
+      <c r="D83" s="27" t="s">
+        <v>104</v>
       </c>
       <c r="E83" s="12"/>
       <c r="G83" s="10"/>
     </row>
-    <row r="84" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B84" s="23"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="23"/>
+    <row r="84" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C84" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D84" s="27" t="s">
+        <v>105</v>
+      </c>
       <c r="E84" s="12"/>
       <c r="G84" s="10"/>
     </row>
-    <row r="85" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B85" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C85" s="29"/>
-      <c r="D85" s="28"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="14"/>
+    <row r="85" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C85" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D85" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E85" s="12"/>
       <c r="G85" s="10"/>
     </row>
-    <row r="86" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B86" s="23"/>
       <c r="C86" s="24"/>
       <c r="D86" s="23"/>
-      <c r="E86" s="10"/>
+      <c r="E86" s="12"/>
       <c r="G86" s="10"/>
     </row>
-    <row r="87" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C87" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D87" s="18" t="s">
-        <v>108</v>
-      </c>
+    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C87" s="29"/>
+      <c r="D87" s="28"/>
       <c r="E87" s="10"/>
+      <c r="F87" s="14"/>
       <c r="G87" s="10"/>
     </row>
-    <row r="88" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C88" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D88" s="19" t="s">
-        <v>109</v>
-      </c>
+    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B88" s="23"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="23"/>
       <c r="E88" s="10"/>
       <c r="G88" s="10"/>
     </row>
-    <row r="89" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="C89" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D89" s="19" t="s">
-        <v>110</v>
+        <v>34</v>
+      </c>
+      <c r="D89" s="18" t="s">
+        <v>108</v>
       </c>
       <c r="E89" s="10"/>
       <c r="G89" s="10"/>
     </row>
-    <row r="90" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C90" s="21" t="s">
         <v>60</v>
       </c>
       <c r="D90" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E90" s="10"/>
       <c r="G90" s="10"/>
     </row>
-    <row r="91" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B91" s="23"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="23"/>
+    <row r="91" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C91" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D91" s="19" t="s">
+        <v>110</v>
+      </c>
       <c r="E91" s="10"/>
       <c r="G91" s="10"/>
     </row>
-    <row r="92" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C92" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D92" s="18" t="s">
-        <v>112</v>
+        <v>60</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>111</v>
       </c>
       <c r="E92" s="10"/>
       <c r="G92" s="10"/>
     </row>
-    <row r="93" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C93" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D93" s="19" t="s">
-        <v>113</v>
-      </c>
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B93" s="23"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="23"/>
       <c r="E93" s="10"/>
       <c r="G93" s="10"/>
     </row>
-    <row r="94" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="C94" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D94" s="19" t="s">
-        <v>114</v>
+        <v>34</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>112</v>
       </c>
       <c r="E94" s="10"/>
       <c r="G94" s="10"/>
     </row>
-    <row r="95" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="22" t="s">
+    <row r="95" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C95" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E95" s="10"/>
+      <c r="G95" s="10"/>
+    </row>
+    <row r="96" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C96" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D96" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E96" s="10"/>
+      <c r="G96" s="10"/>
+    </row>
+    <row r="97" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B95" s="23"/>
-      <c r="C95" s="24"/>
-      <c r="D95" s="23"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="14"/>
-      <c r="H95" s="9"/>
-      <c r="I95" s="9"/>
-      <c r="J95" s="9"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="9"/>
-      <c r="M95" s="9"/>
-    </row>
-    <row r="96" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C96" s="21" t="s">
+      <c r="B97" s="23"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="9"/>
+      <c r="I97" s="9"/>
+      <c r="J97" s="9"/>
+      <c r="K97" s="9"/>
+      <c r="L97" s="9"/>
+      <c r="M97" s="9"/>
+    </row>
+    <row r="98" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C98" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D96" s="18" t="s">
+      <c r="D98" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="E96" s="10"/>
-      <c r="F96" s="16"/>
-      <c r="G96" s="10"/>
-    </row>
-    <row r="97" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C97" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D97" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E97" s="10"/>
-      <c r="G97" s="10"/>
-    </row>
-    <row r="98" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C98" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D98" s="19" t="s">
-        <v>117</v>
-      </c>
       <c r="E98" s="10"/>
+      <c r="F98" s="16"/>
       <c r="G98" s="10"/>
     </row>
     <row r="99" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
@@ -2587,110 +2602,106 @@
         <v>60</v>
       </c>
       <c r="D99" s="19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E99" s="10"/>
       <c r="G99" s="10"/>
     </row>
-    <row r="100" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B100" s="23"/>
-      <c r="C100" s="24"/>
-      <c r="D100" s="23"/>
+    <row r="100" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C100" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D100" s="19" t="s">
+        <v>117</v>
+      </c>
       <c r="E100" s="10"/>
       <c r="G100" s="10"/>
     </row>
-    <row r="101" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C101" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D101" s="18" t="s">
-        <v>119</v>
+        <v>60</v>
+      </c>
+      <c r="D101" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="E101" s="10"/>
       <c r="G101" s="10"/>
     </row>
-    <row r="102" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C102" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D102" s="19" t="s">
-        <v>120</v>
-      </c>
+    <row r="102" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B102" s="23"/>
+      <c r="C102" s="24"/>
+      <c r="D102" s="23"/>
       <c r="E102" s="10"/>
       <c r="G102" s="10"/>
     </row>
-    <row r="103" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="C103" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D103" s="19" t="s">
-        <v>121</v>
+        <v>34</v>
+      </c>
+      <c r="D103" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="E103" s="10"/>
       <c r="G103" s="10"/>
     </row>
-    <row r="104" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B104" s="23"/>
-      <c r="C104" s="24"/>
-      <c r="D104" s="23"/>
+    <row r="104" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C104" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D104" s="19" t="s">
+        <v>120</v>
+      </c>
       <c r="E104" s="10"/>
-      <c r="F104" s="10"/>
-      <c r="G104" s="14"/>
-      <c r="H104" s="9"/>
-      <c r="I104" s="9"/>
-      <c r="J104" s="9"/>
-      <c r="K104" s="9"/>
-      <c r="L104" s="9"/>
-      <c r="M104" s="9"/>
-    </row>
-    <row r="105" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C105" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D105" s="18" t="s">
-        <v>122</v>
+      <c r="G104" s="10"/>
+    </row>
+    <row r="105" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C105" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D105" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="E105" s="10"/>
       <c r="G105" s="10"/>
     </row>
-    <row r="106" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C106" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D106" s="19" t="s">
+    <row r="106" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B106" s="23"/>
+      <c r="C106" s="24"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="9"/>
+      <c r="I106" s="9"/>
+      <c r="J106" s="9"/>
+      <c r="K106" s="9"/>
+      <c r="L106" s="9"/>
+      <c r="M106" s="9"/>
+    </row>
+    <row r="107" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C107" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D107" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E107" s="10"/>
+      <c r="G107" s="10"/>
+    </row>
+    <row r="108" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C108" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D108" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="E106" s="10"/>
-      <c r="G106" s="10"/>
-    </row>
-    <row r="107" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B107" s="23"/>
-      <c r="C107" s="24"/>
-      <c r="D107" s="23"/>
-      <c r="E107" s="10"/>
-      <c r="F107" s="23"/>
-      <c r="G107" s="10"/>
-    </row>
-    <row r="108" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B108" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="C108" s="29"/>
-      <c r="D108" s="28"/>
       <c r="E108" s="10"/>
-      <c r="F108" s="28"/>
       <c r="G108" s="10"/>
     </row>
     <row r="109" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -2704,88 +2715,88 @@
       <c r="F109" s="23"/>
       <c r="G109" s="10"/>
     </row>
-    <row r="110" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C110" s="11" t="s">
+    <row r="110" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C110" s="29"/>
+      <c r="D110" s="28"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="28"/>
+      <c r="G110" s="10"/>
+    </row>
+    <row r="111" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B111" s="23"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="23"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="23"/>
+      <c r="G111" s="10"/>
+    </row>
+    <row r="112" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C112" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D110" s="18" t="s">
+      <c r="D112" s="18" t="s">
         <v>125</v>
-      </c>
-      <c r="E110" s="10"/>
-      <c r="G110" s="10"/>
-    </row>
-    <row r="111" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C111" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="D111" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="E111" s="10"/>
-      <c r="G111" s="10"/>
-    </row>
-    <row r="112" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C112" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D112" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="E112" s="10"/>
       <c r="G112" s="10"/>
     </row>
-    <row r="113" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C113" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D113" s="11" t="s">
-        <v>129</v>
+    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C113" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D113" s="18" t="s">
+        <v>127</v>
       </c>
       <c r="E113" s="10"/>
       <c r="G113" s="10"/>
     </row>
     <row r="114" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C114" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D114" s="19" t="s">
-        <v>130</v>
+        <v>54</v>
+      </c>
+      <c r="D114" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="E114" s="10"/>
       <c r="G114" s="10"/>
     </row>
     <row r="115" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C115" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D115" s="19" t="s">
-        <v>131</v>
+        <v>57</v>
+      </c>
+      <c r="D115" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="E115" s="10"/>
       <c r="G115" s="10"/>
     </row>
-    <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A116" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B116" s="23"/>
-      <c r="C116" s="24"/>
-      <c r="D116" s="23"/>
+    <row r="116" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C116" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D116" s="19" t="s">
+        <v>130</v>
+      </c>
       <c r="E116" s="10"/>
-      <c r="F116" s="23"/>
       <c r="G116" s="10"/>
     </row>
-    <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A117" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B117" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="C117" s="30"/>
-      <c r="D117" s="28"/>
+    <row r="117" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C117" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D117" s="19" t="s">
+        <v>131</v>
+      </c>
       <c r="E117" s="10"/>
-      <c r="F117" s="28"/>
       <c r="G117" s="10"/>
     </row>
     <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -2800,31 +2811,35 @@
       <c r="G118" s="10"/>
     </row>
     <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="C119" s="21" t="s">
+      <c r="A119" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C119" s="30"/>
+      <c r="D119" s="28"/>
+      <c r="E119" s="10"/>
+      <c r="F119" s="28"/>
+      <c r="G119" s="10"/>
+    </row>
+    <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B120" s="23"/>
+      <c r="C120" s="24"/>
+      <c r="D120" s="23"/>
+      <c r="E120" s="10"/>
+      <c r="F120" s="23"/>
+      <c r="G120" s="10"/>
+    </row>
+    <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="C121" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D119" s="31" t="s">
+      <c r="D121" s="31" t="s">
         <v>133</v>
-      </c>
-      <c r="E119" s="10"/>
-      <c r="G119" s="10"/>
-    </row>
-    <row r="120" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C120" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D120" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="E120" s="10"/>
-      <c r="G120" s="10"/>
-    </row>
-    <row r="121" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C121" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D121" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="E121" s="10"/>
       <c r="G121" s="10"/>
@@ -2833,110 +2848,110 @@
       <c r="C122" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D122" s="11" t="s">
-        <v>136</v>
+      <c r="D122" s="37" t="s">
+        <v>134</v>
       </c>
       <c r="E122" s="10"/>
       <c r="G122" s="10"/>
     </row>
     <row r="123" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C123" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D123" s="34" t="s">
-        <v>137</v>
+      <c r="C123" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D123" s="33" t="s">
+        <v>216</v>
       </c>
       <c r="E123" s="10"/>
       <c r="G123" s="10"/>
     </row>
     <row r="124" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C124" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D124" s="34" t="s">
-        <v>138</v>
+      <c r="C124" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D124" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="E124" s="10"/>
       <c r="G124" s="10"/>
     </row>
-    <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A125" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B125" s="23"/>
-      <c r="C125" s="24"/>
-      <c r="D125" s="23"/>
+    <row r="125" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C125" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D125" s="34" t="s">
+        <v>137</v>
+      </c>
       <c r="E125" s="10"/>
-      <c r="F125" s="23"/>
       <c r="G125" s="10"/>
     </row>
-    <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C126" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D126" s="18" t="s">
-        <v>139</v>
+        <v>60</v>
+      </c>
+      <c r="D126" s="34" t="s">
+        <v>138</v>
       </c>
       <c r="E126" s="10"/>
       <c r="G126" s="10"/>
     </row>
-    <row r="127" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C127" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D127" s="35" t="s">
-        <v>221</v>
-      </c>
+    <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B127" s="23"/>
+      <c r="C127" s="24"/>
+      <c r="D127" s="23"/>
       <c r="E127" s="10"/>
+      <c r="F127" s="23"/>
       <c r="G127" s="10"/>
     </row>
-    <row r="128" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="C128" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D128" s="35" t="s">
-        <v>141</v>
+        <v>34</v>
+      </c>
+      <c r="D128" s="18" t="s">
+        <v>139</v>
       </c>
       <c r="E128" s="10"/>
       <c r="G128" s="10"/>
     </row>
-    <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A129" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B129" s="23"/>
-      <c r="C129" s="24"/>
-      <c r="D129" s="23"/>
+    <row r="129" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C129" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D129" s="35" t="s">
+        <v>221</v>
+      </c>
       <c r="E129" s="10"/>
-      <c r="F129" s="23"/>
       <c r="G129" s="10"/>
     </row>
-    <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C130" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D130" s="18" t="s">
-        <v>142</v>
+        <v>60</v>
+      </c>
+      <c r="D130" s="35" t="s">
+        <v>141</v>
       </c>
       <c r="E130" s="10"/>
       <c r="G130" s="10"/>
     </row>
-    <row r="131" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C131" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D131" s="19" t="s">
-        <v>143</v>
-      </c>
+    <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B131" s="23"/>
+      <c r="C131" s="24"/>
+      <c r="D131" s="23"/>
       <c r="E131" s="10"/>
+      <c r="F131" s="23"/>
       <c r="G131" s="10"/>
     </row>
-    <row r="132" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C132" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D132" s="19" t="s">
-        <v>144</v>
+    <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C132" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D132" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="E132" s="10"/>
       <c r="G132" s="10"/>
@@ -2946,48 +2961,48 @@
         <v>60</v>
       </c>
       <c r="D133" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E133" s="10"/>
       <c r="G133" s="10"/>
     </row>
-    <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A134" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B134" s="23"/>
-      <c r="C134" s="24"/>
-      <c r="D134" s="23"/>
+    <row r="134" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C134" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D134" s="19" t="s">
+        <v>144</v>
+      </c>
       <c r="E134" s="10"/>
-      <c r="F134" s="23"/>
       <c r="G134" s="10"/>
     </row>
-    <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C135" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D135" s="18" t="s">
-        <v>146</v>
+    <row r="135" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C135" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D135" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="E135" s="10"/>
       <c r="G135" s="10"/>
     </row>
-    <row r="136" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C136" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D136" s="19" t="s">
-        <v>147</v>
-      </c>
+    <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B136" s="23"/>
+      <c r="C136" s="24"/>
+      <c r="D136" s="23"/>
       <c r="E136" s="10"/>
+      <c r="F136" s="23"/>
       <c r="G136" s="10"/>
     </row>
-    <row r="137" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C137" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D137" s="19" t="s">
-        <v>148</v>
+    <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C137" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D137" s="18" t="s">
+        <v>146</v>
       </c>
       <c r="E137" s="10"/>
       <c r="G137" s="10"/>
@@ -2997,20 +3012,40 @@
         <v>60</v>
       </c>
       <c r="D138" s="19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E138" s="10"/>
       <c r="G138" s="10"/>
     </row>
-    <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A139" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="24"/>
-      <c r="D139" s="23"/>
+    <row r="139" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C139" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D139" s="19" t="s">
+        <v>148</v>
+      </c>
       <c r="E139" s="10"/>
       <c r="G139" s="10"/>
+    </row>
+    <row r="140" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C140" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D140" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E140" s="10"/>
+      <c r="G140" s="10"/>
+    </row>
+    <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A141" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B141" s="23"/>
+      <c r="C141" s="24"/>
+      <c r="D141" s="23"/>
+      <c r="E141" s="10"/>
+      <c r="G141" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3022,7 +3057,7 @@
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{FECD6F66-D8B7-46BD-B870-678E17186243}"/>
     <hyperlink ref="D8" r:id="rId2" xr:uid="{E06E48E3-0BBE-425D-B2FE-65C4D9CF6DA0}"/>
-    <hyperlink ref="D120" r:id="rId3" xr:uid="{22FECDD5-2CC5-40AB-B1F4-9F8C8C9CB1EE}"/>
+    <hyperlink ref="D122" r:id="rId3" xr:uid="{22FECDD5-2CC5-40AB-B1F4-9F8C8C9CB1EE}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3050,20 +3085,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -4688,20 +4723,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -6218,20 +6253,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -8201,20 +8236,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -10146,20 +10181,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>

</xml_diff>

<commit_message>
First complete CV in English/French ...
</commit_message>
<xml_diff>
--- a/static/docs/src/CV.xlsx
+++ b/static/docs/src/CV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windo\Dropbox\z\www\mjbright.github.io\static\docs\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC116EB0-5CC1-4B30-9E8B-51D9CB662D7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4C52C9-7020-4737-AD4F-7124855C7B65}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,8 +64,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={C2399582-17ED-4EE8-991C-1B13371D64F0}</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{C2399582-17ED-4EE8-991C-1B13371D64F0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NEW variables must be taken care of in csv2yaml.py, in csv_tex.py and in templates/*.tex ... and elsewhere?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="280">
   <si>
     <t>SECTION</t>
   </si>
@@ -754,12 +772,6 @@
     <t>https://www.mjbright.net</t>
   </si>
   <si>
-    <t>Freelance - formation/consulting sur Cloud Natif</t>
-  </si>
-  <si>
-    <t>Formateur/Consultant Cloud Natif</t>
-  </si>
-  <si>
     <t>Formateur Cloud Natif</t>
   </si>
   <si>
@@ -775,12 +787,6 @@
     <t>Conferencier</t>
   </si>
   <si>
-    <t>Creations de demos OpenShift</t>
-  </si>
-  <si>
-    <t>Presentations clients Cloud Natifs (PaaS, Serverless, DevOps)</t>
-  </si>
-  <si>
     <t>Animation de Labs Container Orchestration (Swarm, Kubernetes, Mesos)</t>
   </si>
   <si>
@@ -790,35 +796,140 @@
     <t>Brevet EU pour "Prepaid data charging" [EP1720335A1]</t>
   </si>
   <si>
-    <t>Installations automises d'AP4SaaS/IaaS pour Telecom</t>
-  </si>
-  <si>
     <t>- Transfert vers equipes de development en Inde et Chine</t>
   </si>
   <si>
-    <t>Frameworks de test automatises pour IaaS</t>
-  </si>
-  <si>
-    <t>Development agile d'un plateforme d'analyses de donnees</t>
-  </si>
-  <si>
     <t>--  Equipe Agile(SCRUM, TDD, Integration Continu)</t>
   </si>
   <si>
     <t>--  Development logiciel, tests unitaire et functionel pourr SOAP et REST.</t>
   </si>
   <si>
-    <t>Propose et implemente creation de dialog VoiceXML pour MWC PoC</t>
-  </si>
-  <si>
     <t>MOOCs en BigData, SDN, DBs</t>
+  </si>
+  <si>
+    <t>TALKS</t>
+  </si>
+  <si>
+    <t>Cloud Native - Docker, Kubernetes, Serverless</t>
+  </si>
+  <si>
+    <t>Freelance Trainer, Consultant, Conference Speaker</t>
+  </si>
+  <si>
+    <t>Freelance Formateur, Consultant, Conferencier</t>
+  </si>
+  <si>
+    <t>Cloud Natif - Docker, Kubernetes, Serverless</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @mjbright Consulting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $@$mjbright Consulting</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>OpenShift PoC Management</t>
+  </si>
+  <si>
+    <t>Gestion d'un PoC OpenShift</t>
+  </si>
+  <si>
+    <t>Development agile d'un plateforme d'analyses de donnees, profile utilisateur</t>
+  </si>
+  <si>
+    <t>Pr\'esentations clients Cloud Natifs (PaaS, Serverless, DevOps)</t>
+  </si>
+  <si>
+    <t>Frameworks de test automatis\'es pour IaaS</t>
+  </si>
+  <si>
+    <t>Installations automis\'es d'AP4SaaS/IaaS pour Telecom</t>
+  </si>
+  <si>
+    <t>Propos\'e et implement\'e cr\'eation de dialog VoiceXML pour MWC PoC</t>
+  </si>
+  <si>
+    <t>Conseil technique en avant-vente sur produits OpenCall et PoCs</t>
+  </si>
+  <si>
+    <t>Atelier ITSM  en avant-vente, clients et partenaire</t>
+  </si>
+  <si>
+    <t>Technical Lead sur prodiuts Telecom IN</t>
+  </si>
+  <si>
+    <t>Ingenieur Logiciel</t>
+  </si>
+  <si>
+    <t>Chercheur</t>
+  </si>
+  <si>
+    <t>Recherche modelizations de reseaux donnees/signalisation (X.25, Ethernet, SS7)</t>
+  </si>
+  <si>
+    <t>Recherche traitement en Parallele, IA/Raisonnement Qualitatif</t>
+  </si>
+  <si>
+    <t>Chercheur - Stagiaire</t>
+  </si>
+  <si>
+    <t>Conception Z-filter, bit-slice proc., tests de perception utilisateur NICAM audio numerique</t>
+  </si>
+  <si>
+    <t>Langages Scripte (Python/Perl/Ruby/PHP), C++/C, Java, Scala, JavaScript, JQuery, FP</t>
+  </si>
+  <si>
+    <t>Noyau Linux Embarqu\'e, Android, Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Outils</t>
+  </si>
+  <si>
+    <t>Langues Etrangeres</t>
+  </si>
+  <si>
+    <t>Fluent en Anglais, Francais, notions d'Italien, Espagnol.</t>
+  </si>
+  <si>
+    <t>University Of Hull,  UK</t>
+  </si>
+  <si>
+    <t>Prix 'Walter Firth' pour electronique</t>
+  </si>
+  <si>
+    <t>Placement d'un an aux Laboratoires de Recherche de la BBC</t>
+  </si>
+  <si>
+    <t>Course a pied, velo, roller</t>
+  </si>
+  <si>
+    <t>Rock, Argentinian Tango, Salsa, Musique, Cinema</t>
+  </si>
+  <si>
+    <t>Voluntaire au Supermarch\'e eco-responsable L'elefan</t>
+  </si>
+  <si>
+    <t>Technologie</t>
+  </si>
+  <si>
+    <t>Organisateur du Grenoble Python User Group</t>
+  </si>
+  <si>
+    <t>Organisateur du Grenoble Docker User Group</t>
+  </si>
+  <si>
+    <t>Apprentissage continu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -882,8 +993,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -924,6 +1041,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC6D9F1"/>
         <bgColor rgb="FFD6DCE5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1015,7 +1138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1101,6 +1224,13 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1185,6 +1315,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Michael Bright" id="{34E52A3D-0500-47DA-ABCA-415301F9748D}" userId="1851055a07bfd4d4" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1482,12 +1618,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B3" dT="2019-05-12T18:19:34.42" personId="{34E52A3D-0500-47DA-ABCA-415301F9748D}" id="{C2399582-17ED-4EE8-991C-1B13371D64F0}">
+    <text>NEW variables must be taken care of in csv2yaml.py, in csv_tex.py and in templates/*.tex ... and elsewhere?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M142"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" topLeftCell="B111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1568,311 +1712,315 @@
       <c r="E3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="11" t="s">
-        <v>14</v>
-      </c>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>218</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>222</v>
       </c>
       <c r="E5" s="12"/>
-      <c r="F5" s="13" t="str">
-        <f>D5</f>
-        <v>+33 (0)652891534</v>
+      <c r="F5" s="11" t="s">
+        <v>222</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="11" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>199</v>
+        <v>15</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>218</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="43" t="str">
         <f>D6</f>
-        <v>training@mjbright.net</v>
+        <v>+33 (0)652891534</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C7" s="11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="F7" s="43" t="str">
+      <c r="F7" s="45" t="str">
         <f>D7</f>
-        <v>https://www.mjbright.net</v>
+        <v>training@mjbright.net</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="11" t="s">
-        <v>26</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C8" s="11" t="s">
-        <v>209</v>
+        <v>23</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="43" t="str">
+      <c r="F8" s="45" t="str">
         <f>D8</f>
-        <v>https://github.com/mjbright</v>
+        <v>https://www.mjbright.net</v>
       </c>
       <c r="G8" s="12"/>
-      <c r="H8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>28</v>
+        <v>241</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>134</v>
       </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="43" t="str">
+      <c r="F9" s="45" t="str">
         <f>D9</f>
-        <v>https://www.linkedin.com/in/mjbright</v>
+        <v>https://mjbright.github.io/Talks</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>225</v>
+        <v>209</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>210</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="11" t="s">
-        <v>229</v>
+      <c r="F10" s="45" t="str">
+        <f>D10</f>
+        <v>https://github.com/mjbright</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C11" s="11" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="13" t="str">
+      <c r="F11" s="45" t="str">
         <f>D11</f>
-        <v>Michael Bright</v>
+        <v>https://www.linkedin.com/in/mjbright</v>
       </c>
       <c r="G11" s="12"/>
-      <c r="H11" s="11" t="s">
-        <v>33</v>
-      </c>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C12" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="11" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="G12" s="12"/>
-      <c r="H12" s="11" t="s">
-        <v>207</v>
-      </c>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C13" s="11" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="13" t="str">
+      <c r="F13" s="45" t="str">
         <f>D13</f>
-        <v>Grenoble, France</v>
+        <v>Michael Bright</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="11" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>217</v>
+        <v>34</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>243</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="F14" s="13" t="str">
-        <f>D14</f>
-        <v>mjbright Consulting</v>
+      <c r="F14" s="11" t="s">
+        <v>244</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="45" t="str">
+        <f>D15</f>
+        <v>Grenoble, France</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="45" t="str">
+        <f>D16</f>
+        <v xml:space="preserve"> @mjbright Consulting</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-    </row>
-    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>217</v>
-      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="19" t="str">
-        <f>D18</f>
-        <v>mjbright Consulting</v>
-      </c>
+      <c r="F18" s="16"/>
       <c r="G18" s="10"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>212</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C20" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>211</v>
+      <c r="C20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>247</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="19" t="str">
+      <c r="F20" s="46" t="str">
         <f>D20</f>
-        <v>07/2018</v>
+        <v xml:space="preserve"> $@$mjbright Consulting</v>
       </c>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C21" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>58</v>
+    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>212</v>
       </c>
       <c r="E21" s="10"/>
-      <c r="F21" s="19" t="str">
-        <f>D21</f>
-        <v>Present</v>
+      <c r="F21" s="8" t="s">
+        <v>229</v>
       </c>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C22" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="E22" s="10"/>
-      <c r="F22" t="s">
-        <v>232</v>
+      <c r="F22" s="46" t="str">
+        <f>D22</f>
+        <v>07/2018</v>
       </c>
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C23" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>227</v>
+        <v>58</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" t="s">
-        <v>233</v>
+      <c r="F23" s="46" t="str">
+        <f>D23</f>
+        <v>Present</v>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -1880,12 +2028,12 @@
       <c r="C24" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>214</v>
+      <c r="D24" s="39" t="s">
+        <v>223</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G24" s="10"/>
     </row>
@@ -1893,125 +2041,125 @@
       <c r="C25" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>215</v>
+      <c r="D25" s="39" t="s">
+        <v>227</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
+    <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C26" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" t="s">
+        <v>232</v>
+      </c>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C27" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" t="s">
+        <v>233</v>
+      </c>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="8" t="str">
-        <f>D27</f>
-        <v>Cloud Native Solution Architect</v>
-      </c>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C28" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="16"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="8" t="str">
-        <f>D28</f>
-        <v>HPE Customer Innovation Center - Grenoble France</v>
-      </c>
+      <c r="F28" s="16"/>
       <c r="G28" s="10"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
     </row>
     <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="47" t="str">
+        <f>D29</f>
+        <v>Cloud Native Solution Architect</v>
+      </c>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C30" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="47" t="str">
+        <f>D30</f>
+        <v>HPE Customer Innovation Center - Grenoble France</v>
+      </c>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D31" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="8" t="str">
-        <f>D29</f>
+      <c r="E31" s="10"/>
+      <c r="F31" s="47" t="str">
+        <f>D31</f>
         <v>Cloud Native Solution Architect, HPE EG presales</v>
-      </c>
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C30" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="8" t="str">
-        <f>D30</f>
-        <v>09/2013</v>
-      </c>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C31" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="39" t="s">
-        <v>219</v>
-      </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="8" t="str">
-        <f>D31</f>
-        <v>06/2018</v>
       </c>
       <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C32" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="39" t="s">
-        <v>226</v>
+        <v>54</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="E32" s="10"/>
-      <c r="F32" t="s">
-        <v>236</v>
+      <c r="F32" s="47" t="str">
+        <f>D32</f>
+        <v>09/2013</v>
       </c>
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C33" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>219</v>
       </c>
       <c r="E33" s="10"/>
-      <c r="F33" t="s">
-        <v>237</v>
+      <c r="F33" s="47" t="str">
+        <f>D33</f>
+        <v>06/2018</v>
       </c>
       <c r="G33" s="10"/>
     </row>
@@ -2019,12 +2167,12 @@
       <c r="C34" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>62</v>
+      <c r="D34" s="39" t="s">
+        <v>249</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="G34" s="10"/>
     </row>
@@ -2033,11 +2181,11 @@
         <v>60</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="G35" s="10"/>
     </row>
@@ -2046,308 +2194,314 @@
         <v>60</v>
       </c>
       <c r="D36" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" t="s">
+        <v>234</v>
+      </c>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C37" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" t="s">
+        <v>235</v>
+      </c>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C38" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="10"/>
-      <c r="F36" t="str">
-        <f>D36</f>
+      <c r="E38" s="10"/>
+      <c r="F38" t="str">
+        <f>D38</f>
         <v>Cloud Automation (DigitalO, GCE, Azure, AWS, Terraform, Heat, Ansible, Vagrant)</v>
       </c>
-      <c r="G36" s="10"/>
-    </row>
-    <row r="37" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16"/>
-    </row>
-    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C38" s="11" t="s">
+      <c r="B39" s="23"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C40" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D40" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="12"/>
-      <c r="F38" t="str">
-        <f t="shared" ref="F38:F50" si="0">D38</f>
+      <c r="E40" s="12"/>
+      <c r="F40" s="48" t="str">
+        <f t="shared" ref="F40:F43" si="0">D40</f>
         <v>Cloud Engineer</v>
       </c>
-      <c r="G38" s="25"/>
-      <c r="I38" s="26"/>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C39" s="11" t="s">
+      <c r="G40" s="25"/>
+      <c r="I40" s="26"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C41" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D41" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="12"/>
-      <c r="F39" t="str">
+      <c r="E41" s="12"/>
+      <c r="F41" s="48" t="str">
         <f t="shared" si="0"/>
         <v>HP CMS - Grenoble France</v>
       </c>
-      <c r="G39" s="25"/>
-      <c r="I39" s="26"/>
-    </row>
-    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C40" s="21" t="s">
+      <c r="G41" s="25"/>
+      <c r="I41" s="26"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C42" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="12"/>
-      <c r="F40" t="str">
+      <c r="E42" s="12"/>
+      <c r="F42" s="48" t="str">
         <f t="shared" si="0"/>
         <v>09/2005</v>
       </c>
-      <c r="G40" s="25"/>
-      <c r="I40" s="26"/>
-    </row>
-    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C41" s="21" t="s">
+      <c r="G42" s="25"/>
+      <c r="I42" s="26"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C43" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="12"/>
-      <c r="F41" t="str">
+      <c r="E43" s="12"/>
+      <c r="F43" s="48" t="str">
         <f t="shared" si="0"/>
         <v>09/2013</v>
       </c>
-      <c r="G41" s="25"/>
-      <c r="I41" s="26"/>
-    </row>
-    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C42" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D42" s="11" t="s">
+      <c r="G43" s="25"/>
+      <c r="I43" s="26"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C44" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="12"/>
-      <c r="F42" t="s">
-        <v>240</v>
-      </c>
-      <c r="G42" s="25"/>
-      <c r="I42" s="26"/>
-    </row>
-    <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C43" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E43" s="12"/>
-      <c r="F43" t="s">
-        <v>241</v>
-      </c>
-      <c r="G43" s="10"/>
-    </row>
-    <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C44" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="E44" s="12"/>
-      <c r="F44" s="44" t="s">
-        <v>242</v>
-      </c>
-      <c r="G44" s="10"/>
+      <c r="F44" t="s">
+        <v>236</v>
+      </c>
+      <c r="G44" s="25"/>
+      <c r="I44" s="26"/>
     </row>
     <row r="45" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C45" s="21" t="s">
         <v>60</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="G45" s="10"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
-      <c r="J45" s="16"/>
-      <c r="K45" s="16"/>
-      <c r="L45" s="16"/>
-      <c r="M45" s="16"/>
     </row>
     <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C46" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E46" s="12"/>
-      <c r="F46" t="s">
-        <v>244</v>
+      <c r="F46" s="44" t="s">
+        <v>237</v>
       </c>
       <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C47" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E47" s="12"/>
-      <c r="F47" s="38" t="s">
-        <v>245</v>
+      <c r="F47" t="s">
+        <v>253</v>
       </c>
       <c r="G47" s="10"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
     </row>
     <row r="48" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C48" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E48" s="12"/>
-      <c r="F48" s="38" t="s">
-        <v>246</v>
+      <c r="F48" t="s">
+        <v>251</v>
       </c>
       <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C49" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D49" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E49" s="12"/>
+      <c r="F49" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C50" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" s="12"/>
+      <c r="F50" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C51" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E49" s="12"/>
-      <c r="F49" t="s">
-        <v>247</v>
-      </c>
-      <c r="G49" s="10"/>
-    </row>
-    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C50" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="11" t="s">
+      <c r="E51" s="12"/>
+      <c r="F51" t="s">
+        <v>255</v>
+      </c>
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C52" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E50" s="12"/>
-      <c r="F50" t="s">
-        <v>248</v>
-      </c>
-      <c r="G50" s="25"/>
-      <c r="I50" s="26"/>
-    </row>
-    <row r="51" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
+      <c r="E52" s="12"/>
+      <c r="F52" t="s">
+        <v>240</v>
+      </c>
+      <c r="G52" s="25"/>
+      <c r="I52" s="26"/>
+    </row>
+    <row r="53" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="10"/>
-    </row>
-    <row r="52" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C52" s="11" t="s">
+      <c r="B53" s="23"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C54" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D54" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E52" s="12"/>
-      <c r="F52" t="str">
-        <f>D52</f>
+      <c r="E54" s="12"/>
+      <c r="F54" s="48" t="str">
+        <f>D54</f>
         <v>Solution Architect/Consultant</v>
       </c>
-      <c r="G52" s="10"/>
-    </row>
-    <row r="53" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C53" s="11" t="s">
+      <c r="G54" s="10"/>
+    </row>
+    <row r="55" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C55" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D53" s="18" t="s">
+      <c r="D55" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E53" s="12"/>
-      <c r="F53" t="str">
-        <f t="shared" ref="F53:F55" si="1">D53</f>
+      <c r="E55" s="12"/>
+      <c r="F55" s="48" t="str">
+        <f t="shared" ref="F55:F57" si="1">D55</f>
         <v>HP OCBU - Grenoble France</v>
       </c>
-      <c r="G53" s="10"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="16"/>
-      <c r="J53" s="16"/>
-      <c r="K53" s="16"/>
-      <c r="L53" s="16"/>
-      <c r="M53" s="16"/>
-    </row>
-    <row r="54" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C54" s="21" t="s">
+      <c r="G55" s="10"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+    </row>
+    <row r="56" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C56" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="27" t="s">
+      <c r="D56" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="E54" s="12"/>
-      <c r="F54" t="str">
+      <c r="E56" s="12"/>
+      <c r="F56" s="48" t="str">
         <f t="shared" si="1"/>
         <v>02/1998</v>
       </c>
-      <c r="G54" s="10"/>
-    </row>
-    <row r="55" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C55" s="21" t="s">
+      <c r="G56" s="10"/>
+    </row>
+    <row r="57" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C57" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D57" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="12"/>
-      <c r="F55" t="str">
+      <c r="E57" s="12"/>
+      <c r="F57" s="48" t="str">
         <f t="shared" si="1"/>
         <v>09/2005</v>
       </c>
-      <c r="G55" s="10"/>
-    </row>
-    <row r="56" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C56" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E56" s="12"/>
-      <c r="G56" s="10"/>
-    </row>
-    <row r="57" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C57" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E57" s="12"/>
       <c r="G57" s="10"/>
     </row>
     <row r="58" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
@@ -2355,29 +2509,38 @@
         <v>60</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E58" s="12"/>
+      <c r="F58" s="11" t="s">
+        <v>256</v>
+      </c>
       <c r="G58" s="10"/>
     </row>
     <row r="59" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C59" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="D59" s="19" t="s">
-        <v>85</v>
+      <c r="D59" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="E59" s="12"/>
+      <c r="F59" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="G59" s="10"/>
     </row>
     <row r="60" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C60" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="D60" s="19" t="s">
-        <v>86</v>
+        <v>60</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="E60" s="12"/>
+      <c r="F60" s="11" t="s">
+        <v>257</v>
+      </c>
       <c r="G60" s="10"/>
     </row>
     <row r="61" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
@@ -2385,132 +2548,150 @@
         <v>220</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E61" s="12"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
-      <c r="L61" s="9"/>
-      <c r="M61" s="9"/>
+      <c r="F61" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G61" s="10"/>
     </row>
     <row r="62" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C62" s="21" t="s">
         <v>220</v>
       </c>
       <c r="D62" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E62" s="12"/>
+      <c r="F62" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G62" s="10"/>
+    </row>
+    <row r="63" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C63" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63" s="12"/>
+      <c r="F63" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G63" s="14"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+    </row>
+    <row r="64" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C64" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D64" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E62" s="12"/>
-      <c r="G62" s="10"/>
-    </row>
-    <row r="63" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
+      <c r="E64" s="12"/>
+      <c r="F64" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G64" s="10"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="10"/>
-    </row>
-    <row r="64" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C64" s="11" t="s">
+      <c r="B65" s="23"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="10"/>
+    </row>
+    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C66" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D64" s="18" t="s">
+      <c r="D66" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="E64" s="12"/>
-      <c r="F64" t="str">
-        <f>D64</f>
+      <c r="E66" s="12"/>
+      <c r="F66" s="48" t="str">
+        <f>D66</f>
         <v>Technical Lead/Software Engineer</v>
       </c>
-      <c r="G64" s="10"/>
-    </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C65" s="11" t="s">
+      <c r="G66" s="10"/>
+    </row>
+    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C67" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D65" s="18" t="s">
+      <c r="D67" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E65" s="12"/>
-      <c r="F65" t="str">
-        <f t="shared" ref="F65:F67" si="2">D65</f>
+      <c r="E67" s="12"/>
+      <c r="F67" s="48" t="str">
+        <f t="shared" ref="F67:F69" si="2">D67</f>
         <v>HP OCBU - Grenoble France</v>
       </c>
-      <c r="G65" s="10"/>
-    </row>
-    <row r="66" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C66" s="21" t="s">
+      <c r="G67" s="10"/>
+    </row>
+    <row r="68" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C68" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D66" s="27" t="s">
+      <c r="D68" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E66" s="12"/>
-      <c r="F66" t="str">
+      <c r="E68" s="12"/>
+      <c r="F68" s="48" t="str">
         <f t="shared" si="2"/>
         <v>05/1992</v>
       </c>
-      <c r="G66" s="10"/>
-    </row>
-    <row r="67" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C67" s="21" t="s">
+      <c r="G68" s="10"/>
+    </row>
+    <row r="69" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C69" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D67" s="27" t="s">
+      <c r="D69" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="E67" s="12"/>
-      <c r="F67" t="str">
+      <c r="E69" s="12"/>
+      <c r="F69" s="48" t="str">
         <f t="shared" si="2"/>
         <v>02/1998</v>
       </c>
-      <c r="G67" s="10"/>
-    </row>
-    <row r="68" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C68" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E68" s="12"/>
-      <c r="G68" s="10"/>
-    </row>
-    <row r="69" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C69" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E69" s="12"/>
       <c r="G69" s="10"/>
     </row>
     <row r="70" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C70" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E70" s="12"/>
+      <c r="F70" s="11" t="s">
+        <v>258</v>
+      </c>
       <c r="G70" s="10"/>
     </row>
     <row r="71" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C71" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E71" s="12"/>
+      <c r="F71" s="11" t="s">
+        <v>92</v>
+      </c>
       <c r="G71" s="10"/>
     </row>
     <row r="72" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
@@ -2518,207 +2699,222 @@
         <v>220</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E72" s="12"/>
+      <c r="F72" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="G72" s="10"/>
     </row>
     <row r="73" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C73" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E73" s="12"/>
+      <c r="F73" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="G73" s="10"/>
+    </row>
+    <row r="74" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C74" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="D73" s="11" t="s">
+      <c r="D74" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E74" s="12"/>
+      <c r="F74" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G74" s="10"/>
+    </row>
+    <row r="75" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C75" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D75" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E73" s="12"/>
-      <c r="G73" s="10"/>
-    </row>
-    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="22" t="s">
+      <c r="E75" s="12"/>
+      <c r="F75" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G75" s="10"/>
+    </row>
+    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B74" s="23"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="10"/>
-    </row>
-    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C75" s="11" t="s">
+      <c r="B76" s="23"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="10"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C77" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D75" s="18" t="s">
+      <c r="D77" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="E75" s="12"/>
-      <c r="F75" t="str">
-        <f>D75</f>
-        <v>Member of Technical Staff</v>
-      </c>
-      <c r="G75" s="10"/>
-    </row>
-    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C76" s="11" t="s">
+      <c r="E77" s="12"/>
+      <c r="F77" s="49" t="s">
+        <v>260</v>
+      </c>
+      <c r="G77" s="10"/>
+    </row>
+    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C78" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D76" s="18" t="s">
+      <c r="D78" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E76" s="12"/>
-      <c r="F76" t="str">
-        <f t="shared" ref="F76:F78" si="3">D76</f>
+      <c r="E78" s="12"/>
+      <c r="F78" s="48" t="str">
+        <f t="shared" ref="F78:F80" si="3">D78</f>
         <v>HP Research Labs - Bristol UK</v>
       </c>
-      <c r="G76" s="10"/>
-    </row>
-    <row r="77" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C77" s="21" t="s">
+      <c r="G78" s="10"/>
+    </row>
+    <row r="79" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C79" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D77" s="27" t="s">
+      <c r="D79" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="E77" s="12"/>
-      <c r="F77" t="str">
+      <c r="E79" s="12"/>
+      <c r="F79" s="48" t="str">
         <f t="shared" si="3"/>
         <v>08/1985</v>
       </c>
-      <c r="G77" s="10"/>
-    </row>
-    <row r="78" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C78" s="21" t="s">
+      <c r="G79" s="10"/>
+    </row>
+    <row r="80" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C80" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D78" s="27" t="s">
+      <c r="D80" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E78" s="12"/>
-      <c r="F78" t="str">
+      <c r="E80" s="12"/>
+      <c r="F80" s="48" t="str">
         <f t="shared" si="3"/>
         <v>05/1992</v>
       </c>
-      <c r="G78" s="10"/>
-    </row>
-    <row r="79" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C79" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D79" s="19" t="s">
+      <c r="G80" s="10"/>
+    </row>
+    <row r="81" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C81" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D81" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E79" s="12"/>
-      <c r="G79" s="10"/>
-    </row>
-    <row r="80" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C80" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D80" s="19" t="s">
+      <c r="E81" s="12"/>
+      <c r="F81" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="G81" s="10"/>
+    </row>
+    <row r="82" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C82" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D82" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E80" s="12"/>
-      <c r="G80" s="10"/>
-    </row>
-    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="22" t="s">
+      <c r="E82" s="12"/>
+      <c r="F82" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="G82" s="10"/>
+    </row>
+    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B81" s="23"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="23"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="10"/>
-    </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C82" s="11" t="s">
+      <c r="B83" s="23"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="10"/>
+    </row>
+    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C84" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D82" s="18" t="s">
+      <c r="D84" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E82" s="12"/>
-      <c r="F82" t="str">
-        <f>D82</f>
-        <v>Research Trainee</v>
-      </c>
-      <c r="G82" s="10"/>
-    </row>
-    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C83" s="11" t="s">
+      <c r="E84" s="12"/>
+      <c r="F84" s="49" t="s">
+        <v>263</v>
+      </c>
+      <c r="G84" s="10"/>
+    </row>
+    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C85" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D83" s="18" t="s">
+      <c r="D85" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E83" s="12"/>
-      <c r="F83" t="str">
-        <f t="shared" ref="F83:F85" si="4">D83</f>
+      <c r="E85" s="12"/>
+      <c r="F85" s="48" t="str">
+        <f t="shared" ref="F85:F87" si="4">D85</f>
         <v>BBC Research Labs - UK</v>
       </c>
-      <c r="G83" s="10"/>
-    </row>
-    <row r="84" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C84" s="21" t="s">
+      <c r="G85" s="10"/>
+    </row>
+    <row r="86" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C86" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D84" s="27" t="s">
+      <c r="D86" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="E84" s="12"/>
-      <c r="F84" t="str">
+      <c r="E86" s="12"/>
+      <c r="F86" s="48" t="str">
         <f t="shared" si="4"/>
         <v>09/1983</v>
       </c>
-      <c r="G84" s="10"/>
-    </row>
-    <row r="85" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C85" s="21" t="s">
+      <c r="G86" s="10"/>
+    </row>
+    <row r="87" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C87" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D85" s="27" t="s">
+      <c r="D87" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="E85" s="12"/>
-      <c r="F85" t="str">
+      <c r="E87" s="12"/>
+      <c r="F87" s="48" t="str">
         <f t="shared" si="4"/>
         <v>08/1984</v>
       </c>
-      <c r="G85" s="10"/>
-    </row>
-    <row r="86" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C86" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D86" s="19" t="s">
+      <c r="G87" s="10"/>
+    </row>
+    <row r="88" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C88" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D88" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="E86" s="12"/>
-      <c r="G86" s="10"/>
-    </row>
-    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B87" s="23"/>
-      <c r="C87" s="24"/>
-      <c r="D87" s="23"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="23"/>
-      <c r="G87" s="10"/>
-    </row>
-    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B88" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C88" s="29"/>
-      <c r="D88" s="28"/>
-      <c r="E88" s="10"/>
-      <c r="F88" s="14"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="19" t="s">
+        <v>264</v>
+      </c>
       <c r="G88" s="10"/>
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -2728,38 +2924,46 @@
       <c r="B89" s="23"/>
       <c r="C89" s="24"/>
       <c r="D89" s="23"/>
-      <c r="E89" s="10"/>
+      <c r="E89" s="12"/>
       <c r="F89" s="23"/>
       <c r="G89" s="10"/>
     </row>
-    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C90" s="21" t="s">
+    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C90" s="29"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="10"/>
+    </row>
+    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B91" s="23"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="10"/>
+    </row>
+    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C92" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D90" s="18" t="s">
+      <c r="D92" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="E90" s="10"/>
-      <c r="G90" s="10"/>
-    </row>
-    <row r="91" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C91" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D91" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E91" s="10"/>
-      <c r="G91" s="10"/>
-    </row>
-    <row r="92" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C92" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D92" s="19" t="s">
-        <v>110</v>
-      </c>
       <c r="E92" s="10"/>
+      <c r="F92" s="48" t="str">
+        <f>D92</f>
+        <v>Certifications</v>
+      </c>
       <c r="G92" s="10"/>
     </row>
     <row r="93" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
@@ -2767,97 +2971,125 @@
         <v>60</v>
       </c>
       <c r="D93" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E93" s="10"/>
+      <c r="F93" s="48" t="str">
+        <f t="shared" ref="F93:F95" si="5">D93</f>
+        <v xml:space="preserve">Sep 2017 CNCF Kubernetes Administration (CKA) </v>
+      </c>
+      <c r="G93" s="10"/>
+    </row>
+    <row r="94" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C94" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D94" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E94" s="10"/>
+      <c r="F94" s="48" t="str">
+        <f t="shared" si="5"/>
+        <v>May 2015 HPE Expert One, SDN Apps (HP0-Y48)</v>
+      </c>
+      <c r="G94" s="10"/>
+    </row>
+    <row r="95" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C95" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E93" s="10"/>
-      <c r="G93" s="10"/>
-    </row>
-    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="22" t="s">
+      <c r="E95" s="10"/>
+      <c r="F95" s="48" t="str">
+        <f t="shared" si="5"/>
+        <v>Nov 2013 RedHat RHCE/RHCSA</v>
+      </c>
+      <c r="G95" s="10"/>
+    </row>
+    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B94" s="23"/>
-      <c r="C94" s="24"/>
-      <c r="D94" s="23"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="23"/>
-      <c r="G94" s="10"/>
-    </row>
-    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C95" s="21" t="s">
+      <c r="B96" s="23"/>
+      <c r="C96" s="24"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="10"/>
+    </row>
+    <row r="97" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C97" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D95" s="18" t="s">
+      <c r="D97" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E95" s="10"/>
-      <c r="G95" s="10"/>
-    </row>
-    <row r="96" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C96" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D96" s="19" t="s">
+      <c r="E97" s="10"/>
+      <c r="F97" s="48" t="str">
+        <f>D97</f>
+        <v>Cloud</v>
+      </c>
+      <c r="G97" s="10"/>
+    </row>
+    <row r="98" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C98" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D98" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E96" s="10"/>
-      <c r="G96" s="10"/>
-    </row>
-    <row r="97" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C97" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D97" s="19" t="s">
+      <c r="E98" s="10"/>
+      <c r="F98" s="48" t="str">
+        <f t="shared" ref="F98:F99" si="6">D98</f>
+        <v>PaaS OpenShift, Google App Engine, Heroku</v>
+      </c>
+      <c r="G98" s="10"/>
+    </row>
+    <row r="99" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C99" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D99" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E97" s="10"/>
-      <c r="G97" s="10"/>
-    </row>
-    <row r="98" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="22" t="s">
+      <c r="E99" s="10"/>
+      <c r="F99" s="48" t="str">
+        <f t="shared" si="6"/>
+        <v>IaaS Azure, AWS, OpenStack, CloudStack, SDN (OpenDaylight), Docker</v>
+      </c>
+      <c r="G99" s="10"/>
+    </row>
+    <row r="100" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B98" s="23"/>
-      <c r="C98" s="24"/>
-      <c r="D98" s="23"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="23"/>
-      <c r="G98" s="14"/>
-      <c r="H98" s="9"/>
-      <c r="I98" s="9"/>
-      <c r="J98" s="9"/>
-      <c r="K98" s="9"/>
-      <c r="L98" s="9"/>
-      <c r="M98" s="9"/>
-    </row>
-    <row r="99" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C99" s="21" t="s">
+      <c r="B100" s="23"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="23"/>
+      <c r="G100" s="14"/>
+      <c r="H100" s="9"/>
+      <c r="I100" s="9"/>
+      <c r="J100" s="9"/>
+      <c r="K100" s="9"/>
+      <c r="L100" s="9"/>
+      <c r="M100" s="9"/>
+    </row>
+    <row r="101" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C101" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D99" s="18" t="s">
+      <c r="D101" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="E99" s="10"/>
-      <c r="G99" s="10"/>
-    </row>
-    <row r="100" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C100" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D100" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E100" s="10"/>
-      <c r="G100" s="10"/>
-    </row>
-    <row r="101" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C101" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D101" s="19" t="s">
-        <v>117</v>
-      </c>
       <c r="E101" s="10"/>
+      <c r="F101" s="48" t="str">
+        <f t="shared" ref="F101:F104" si="7">D101</f>
+        <v>Languages and Paradigms</v>
+      </c>
       <c r="G101" s="10"/>
     </row>
     <row r="102" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
@@ -2865,111 +3097,134 @@
         <v>60</v>
       </c>
       <c r="D102" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E102" s="10"/>
+      <c r="F102" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="G102" s="10"/>
+    </row>
+    <row r="103" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C103" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D103" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E103" s="10"/>
+      <c r="F103" s="48" t="str">
+        <f t="shared" si="7"/>
+        <v>SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</v>
+      </c>
+      <c r="G103" s="10"/>
+    </row>
+    <row r="104" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C104" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D104" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="E102" s="10"/>
-      <c r="G102" s="10"/>
-    </row>
-    <row r="103" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A103" s="22" t="s">
+      <c r="E104" s="10"/>
+      <c r="F104" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="G104" s="10"/>
+    </row>
+    <row r="105" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B103" s="23"/>
-      <c r="C103" s="24"/>
-      <c r="D103" s="23"/>
-      <c r="E103" s="10"/>
-      <c r="F103" s="23"/>
-      <c r="G103" s="10"/>
-    </row>
-    <row r="104" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C104" s="21" t="s">
+      <c r="B105" s="23"/>
+      <c r="C105" s="24"/>
+      <c r="D105" s="23"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="23"/>
+      <c r="G105" s="10"/>
+    </row>
+    <row r="106" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C106" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D104" s="18" t="s">
+      <c r="D106" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="E104" s="10"/>
-      <c r="G104" s="10"/>
-    </row>
-    <row r="105" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C105" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D105" s="19" t="s">
+      <c r="E106" s="10"/>
+      <c r="F106" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="G106" s="10"/>
+    </row>
+    <row r="107" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C107" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D107" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="E105" s="10"/>
-      <c r="G105" s="10"/>
-    </row>
-    <row r="106" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C106" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D106" s="19" t="s">
+      <c r="E107" s="10"/>
+      <c r="F107" s="48" t="str">
+        <f t="shared" ref="F106:F108" si="8">D107</f>
+        <v>Eclipse, Git, svn, vim, maven, Jenkins, gdb</v>
+      </c>
+      <c r="G107" s="10"/>
+    </row>
+    <row r="108" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C108" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D108" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="E106" s="10"/>
-      <c r="G106" s="10"/>
-    </row>
-    <row r="107" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="22" t="s">
+      <c r="E108" s="10"/>
+      <c r="F108" s="48" t="str">
+        <f t="shared" si="8"/>
+        <v>Virtualization (vSphere/Pyvmomi, KVM-Qemu, VirtualBox)</v>
+      </c>
+      <c r="G108" s="10"/>
+    </row>
+    <row r="109" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B107" s="23"/>
-      <c r="C107" s="24"/>
-      <c r="D107" s="23"/>
-      <c r="E107" s="10"/>
-      <c r="F107" s="23"/>
-      <c r="G107" s="14"/>
-      <c r="H107" s="9"/>
-      <c r="I107" s="9"/>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
-      <c r="L107" s="9"/>
-      <c r="M107" s="9"/>
-    </row>
-    <row r="108" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C108" s="11" t="s">
+      <c r="B109" s="23"/>
+      <c r="C109" s="24"/>
+      <c r="D109" s="23"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="14"/>
+      <c r="H109" s="9"/>
+      <c r="I109" s="9"/>
+      <c r="J109" s="9"/>
+      <c r="K109" s="9"/>
+      <c r="L109" s="9"/>
+      <c r="M109" s="9"/>
+    </row>
+    <row r="110" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C110" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D108" s="18" t="s">
+      <c r="D110" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="E108" s="10"/>
-      <c r="G108" s="10"/>
-    </row>
-    <row r="109" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C109" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D109" s="19" t="s">
+      <c r="E110" s="10"/>
+      <c r="F110" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="G110" s="10"/>
+    </row>
+    <row r="111" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C111" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D111" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="E109" s="10"/>
-      <c r="G109" s="10"/>
-    </row>
-    <row r="110" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B110" s="23"/>
-      <c r="C110" s="24"/>
-      <c r="D110" s="23"/>
-      <c r="E110" s="10"/>
-      <c r="F110" s="23"/>
-      <c r="G110" s="10"/>
-    </row>
-    <row r="111" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B111" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="C111" s="29"/>
-      <c r="D111" s="28"/>
       <c r="E111" s="10"/>
-      <c r="F111" s="28"/>
+      <c r="F111" s="19" t="s">
+        <v>269</v>
+      </c>
       <c r="G111" s="10"/>
     </row>
     <row r="112" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -2983,88 +3238,110 @@
       <c r="F112" s="23"/>
       <c r="G112" s="10"/>
     </row>
-    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C113" s="11" t="s">
+    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C113" s="29"/>
+      <c r="D113" s="28"/>
+      <c r="E113" s="10"/>
+      <c r="F113" s="28"/>
+      <c r="G113" s="10"/>
+    </row>
+    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B114" s="23"/>
+      <c r="C114" s="24"/>
+      <c r="D114" s="23"/>
+      <c r="E114" s="10"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="10"/>
+    </row>
+    <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C115" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D113" s="18" t="s">
+      <c r="D115" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="E113" s="10"/>
-      <c r="G113" s="10"/>
-    </row>
-    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C114" s="11" t="s">
+      <c r="E115" s="10"/>
+      <c r="F115" s="48" t="str">
+        <f t="shared" ref="F115:F120" si="9">D115</f>
+        <v>B.Sc/Dip.Eng in  Electronic Control and Robotics</v>
+      </c>
+      <c r="G115" s="10"/>
+    </row>
+    <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C116" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D114" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="E114" s="10"/>
-      <c r="G114" s="10"/>
-    </row>
-    <row r="115" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C115" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D115" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="E115" s="10"/>
-      <c r="G115" s="10"/>
-    </row>
-    <row r="116" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C116" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D116" s="11" t="s">
-        <v>129</v>
+      <c r="D116" s="18" t="s">
+        <v>270</v>
       </c>
       <c r="E116" s="10"/>
+      <c r="F116" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v>University Of Hull,  UK</v>
+      </c>
       <c r="G116" s="10"/>
     </row>
     <row r="117" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C117" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D117" s="19" t="s">
-        <v>130</v>
+        <v>54</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="E117" s="10"/>
+      <c r="F117" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v>10/1980</v>
+      </c>
       <c r="G117" s="10"/>
     </row>
     <row r="118" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C118" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D118" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D118" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E118" s="10"/>
+      <c r="F118" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v>07/1985</v>
+      </c>
+      <c r="G118" s="10"/>
+    </row>
+    <row r="119" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C119" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D119" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="E119" s="10"/>
+      <c r="F119" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="G119" s="10"/>
+    </row>
+    <row r="120" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C120" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D120" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="E118" s="10"/>
-      <c r="G118" s="10"/>
-    </row>
-    <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A119" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B119" s="23"/>
-      <c r="C119" s="24"/>
-      <c r="D119" s="23"/>
-      <c r="E119" s="10"/>
-      <c r="F119" s="23"/>
-      <c r="G119" s="10"/>
-    </row>
-    <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A120" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B120" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="C120" s="30"/>
-      <c r="D120" s="28"/>
       <c r="E120" s="10"/>
-      <c r="F120" s="28"/>
+      <c r="F120" s="19" t="s">
+        <v>272</v>
+      </c>
       <c r="G120" s="10"/>
     </row>
     <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -3079,148 +3356,189 @@
       <c r="G121" s="10"/>
     </row>
     <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="C122" s="21" t="s">
+      <c r="A122" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C122" s="30"/>
+      <c r="D122" s="28"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="28"/>
+      <c r="G122" s="10"/>
+    </row>
+    <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B123" s="23"/>
+      <c r="C123" s="24"/>
+      <c r="D123" s="23"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="23"/>
+      <c r="G123" s="10"/>
+    </row>
+    <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="C124" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D122" s="31" t="s">
+      <c r="D124" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="E122" s="10"/>
-      <c r="G122" s="10"/>
-    </row>
-    <row r="123" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C123" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D123" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="E123" s="10"/>
-      <c r="F123" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="G123" s="10"/>
-    </row>
-    <row r="124" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C124" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D124" s="33" t="s">
-        <v>216</v>
-      </c>
       <c r="E124" s="10"/>
+      <c r="F124" s="48" t="str">
+        <f t="shared" ref="F124:F129" si="10">D124</f>
+        <v>Conference Talks</v>
+      </c>
       <c r="G124" s="10"/>
     </row>
     <row r="125" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C125" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D125" s="11" t="s">
+      <c r="D125" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="E125" s="10"/>
+      <c r="F125" s="48" t="str">
+        <f t="shared" si="10"/>
+        <v>https://mjbright.github.io/Talks</v>
+      </c>
+      <c r="G125" s="10"/>
+    </row>
+    <row r="126" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C126" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D126" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="E126" s="10"/>
+      <c r="F126" s="48" t="str">
+        <f t="shared" si="10"/>
+        <v>2018 FOSSCon (Pres+Lab), FOSS Asia (Pres+Lab), Code Europe, PyConfr</v>
+      </c>
+      <c r="G126" s="10"/>
+    </row>
+    <row r="127" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C127" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D127" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="E125" s="10"/>
-      <c r="G125" s="10"/>
-    </row>
-    <row r="126" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C126" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D126" s="34" t="s">
+      <c r="E127" s="10"/>
+      <c r="F127" s="48" t="str">
+        <f t="shared" si="10"/>
+        <v>2017 Devconf.cz, Snowcamp.io, HPE TSS, HPE TES, DockerConUS, RMLL, OSS EU (Pres+Lab)</v>
+      </c>
+      <c r="G127" s="10"/>
+    </row>
+    <row r="128" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C128" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D128" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E126" s="10"/>
-      <c r="G126" s="10"/>
-    </row>
-    <row r="127" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C127" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D127" s="34" t="s">
+      <c r="E128" s="10"/>
+      <c r="F128" s="48" t="str">
+        <f t="shared" si="10"/>
+        <v>2016 Europython (Pres+Lab), ContainerCon Europe (Pres+Lab)</v>
+      </c>
+      <c r="G128" s="10"/>
+    </row>
+    <row r="129" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C129" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D129" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="E127" s="10"/>
-      <c r="G127" s="10"/>
-    </row>
-    <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A128" s="22" t="s">
+      <c r="E129" s="10"/>
+      <c r="F129" s="48" t="str">
+        <f t="shared" si="10"/>
+        <v>2015 Pyconfr, Ipython vers Jupyter</v>
+      </c>
+      <c r="G129" s="10"/>
+    </row>
+    <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B128" s="23"/>
-      <c r="C128" s="24"/>
-      <c r="D128" s="23"/>
-      <c r="E128" s="10"/>
-      <c r="F128" s="23"/>
-      <c r="G128" s="10"/>
-    </row>
-    <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C129" s="11" t="s">
+      <c r="B130" s="23"/>
+      <c r="C130" s="24"/>
+      <c r="D130" s="23"/>
+      <c r="E130" s="10"/>
+      <c r="F130" s="23"/>
+      <c r="G130" s="10"/>
+    </row>
+    <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C131" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D129" s="18" t="s">
+      <c r="D131" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="E129" s="10"/>
-      <c r="G129" s="10"/>
-    </row>
-    <row r="130" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C130" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D130" s="35" t="s">
+      <c r="E131" s="10"/>
+      <c r="F131" s="18" t="str">
+        <f t="shared" ref="F131:F133" si="11">D131</f>
+        <v>Startup Weekend</v>
+      </c>
+      <c r="G131" s="10"/>
+    </row>
+    <row r="132" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C132" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D132" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="E130" s="10"/>
-      <c r="G130" s="10"/>
-    </row>
-    <row r="131" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C131" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D131" s="35" t="s">
+      <c r="E132" s="10"/>
+      <c r="F132" s="48" t="str">
+        <f t="shared" si="11"/>
+        <v>2018-Nov: Community Security System</v>
+      </c>
+      <c r="G132" s="10"/>
+    </row>
+    <row r="133" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C133" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D133" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="E131" s="10"/>
-      <c r="G131" s="10"/>
-    </row>
-    <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A132" s="22" t="s">
+      <c r="E133" s="10"/>
+      <c r="F133" s="48" t="str">
+        <f t="shared" si="11"/>
+        <v>2012-Nov 2nd place: https://www.archionline.com/</v>
+      </c>
+      <c r="G133" s="10"/>
+    </row>
+    <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B132" s="23"/>
-      <c r="C132" s="24"/>
-      <c r="D132" s="23"/>
-      <c r="E132" s="10"/>
-      <c r="F132" s="23"/>
-      <c r="G132" s="10"/>
-    </row>
-    <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C133" s="11" t="s">
+      <c r="B134" s="23"/>
+      <c r="C134" s="24"/>
+      <c r="D134" s="23"/>
+      <c r="E134" s="10"/>
+      <c r="F134" s="23"/>
+      <c r="G134" s="10"/>
+    </row>
+    <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C135" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D133" s="18" t="s">
+      <c r="D135" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="E133" s="10"/>
-      <c r="G133" s="10"/>
-    </row>
-    <row r="134" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C134" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D134" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E134" s="10"/>
-      <c r="G134" s="10"/>
-    </row>
-    <row r="135" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C135" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D135" s="19" t="s">
-        <v>144</v>
-      </c>
       <c r="E135" s="10"/>
+      <c r="F135" s="18" t="str">
+        <f t="shared" ref="F135:F138" si="12">D135</f>
+        <v>Miscellaneous</v>
+      </c>
       <c r="G135" s="10"/>
     </row>
     <row r="136" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
@@ -3228,50 +3546,62 @@
         <v>60</v>
       </c>
       <c r="D136" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E136" s="10"/>
+      <c r="F136" s="49" t="s">
+        <v>273</v>
+      </c>
+      <c r="G136" s="10"/>
+    </row>
+    <row r="137" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C137" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D137" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="E137" s="10"/>
+      <c r="F137" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="G137" s="10"/>
+    </row>
+    <row r="138" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C138" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D138" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="E136" s="10"/>
-      <c r="G136" s="10"/>
-    </row>
-    <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A137" s="22" t="s">
+      <c r="E138" s="10"/>
+      <c r="F138" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="G138" s="10"/>
+    </row>
+    <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B137" s="23"/>
-      <c r="C137" s="24"/>
-      <c r="D137" s="23"/>
-      <c r="E137" s="10"/>
-      <c r="F137" s="23"/>
-      <c r="G137" s="10"/>
-    </row>
-    <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C138" s="11" t="s">
+      <c r="B139" s="23"/>
+      <c r="C139" s="24"/>
+      <c r="D139" s="23"/>
+      <c r="E139" s="10"/>
+      <c r="F139" s="23"/>
+      <c r="G139" s="10"/>
+    </row>
+    <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C140" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D138" s="18" t="s">
+      <c r="D140" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="E138" s="10"/>
-      <c r="G138" s="10"/>
-    </row>
-    <row r="139" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C139" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D139" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="E139" s="10"/>
-      <c r="G139" s="10"/>
-    </row>
-    <row r="140" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C140" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D140" s="19" t="s">
-        <v>148</v>
-      </c>
       <c r="E140" s="10"/>
+      <c r="F140" s="18" t="s">
+        <v>276</v>
+      </c>
       <c r="G140" s="10"/>
     </row>
     <row r="141" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
@@ -3279,21 +3609,50 @@
         <v>60</v>
       </c>
       <c r="D141" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E141" s="10"/>
+      <c r="F141" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="G141" s="10"/>
+    </row>
+    <row r="142" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C142" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D142" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E142" s="10"/>
+      <c r="F142" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="G142" s="10"/>
+    </row>
+    <row r="143" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C143" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D143" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="E141" s="10"/>
-      <c r="G141" s="10"/>
-    </row>
-    <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A142" s="22" t="s">
+      <c r="E143" s="10"/>
+      <c r="F143" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="G143" s="10"/>
+    </row>
+    <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A144" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B142" s="23"/>
-      <c r="C142" s="24"/>
-      <c r="D142" s="23"/>
-      <c r="E142" s="10"/>
-      <c r="F142" s="23"/>
-      <c r="G142" s="10"/>
+      <c r="B144" s="23"/>
+      <c r="C144" s="24"/>
+      <c r="D144" s="23"/>
+      <c r="E144" s="10"/>
+      <c r="F144" s="23"/>
+      <c r="G144" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3303,11 +3662,11 @@
     <mergeCell ref="I1:J1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{FECD6F66-D8B7-46BD-B870-678E17186243}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{E06E48E3-0BBE-425D-B2FE-65C4D9CF6DA0}"/>
-    <hyperlink ref="D123" r:id="rId3" xr:uid="{22FECDD5-2CC5-40AB-B1F4-9F8C8C9CB1EE}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{22A5A641-F2FA-46B6-93D1-F6ED2F1D0FE2}"/>
-    <hyperlink ref="F123" r:id="rId5" xr:uid="{2C4A759C-CD44-4E43-885C-10D7456A57A2}"/>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{FECD6F66-D8B7-46BD-B870-678E17186243}"/>
+    <hyperlink ref="D10" r:id="rId2" xr:uid="{E06E48E3-0BBE-425D-B2FE-65C4D9CF6DA0}"/>
+    <hyperlink ref="D125" r:id="rId3" xr:uid="{22FECDD5-2CC5-40AB-B1F4-9F8C8C9CB1EE}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{22A5A641-F2FA-46B6-93D1-F6ED2F1D0FE2}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{959B1FAB-C5B5-43D2-84B9-DE8D37B08A6A}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3315,6 +3674,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated English CV with Training experience
</commit_message>
<xml_diff>
--- a/static/docs/src/CV.xlsx
+++ b/static/docs/src/CV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windo\Dropbox\z\www\mjbright.github.io\static\docs\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7567B5-5C3F-4D72-98D6-DA28D0E4FFE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21FE4B3-68EF-4043-9CF4-CA05606FDA40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
     <definedName name="MONINT" localSheetId="1">#REF!</definedName>
     <definedName name="MONINT">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2368" uniqueCount="286">
   <si>
     <t>SECTION</t>
   </si>
@@ -945,13 +945,31 @@
   </si>
   <si>
     <t>Apprentissage continu</t>
+  </si>
+  <si>
+    <t>Technical Trainer, Consultant</t>
+  </si>
+  <si>
+    <t>Formateur, Consultant Technique</t>
+  </si>
+  <si>
+    <t>Kubernetes Instructor for LinuxFoundation, Controlplane.io</t>
+  </si>
+  <si>
+    <t>Consulting - Kubernetes Air-gapped Implementation</t>
+  </si>
+  <si>
+    <t>Creation, delivery of Docker, Kubernetes, Terraform trainings</t>
+  </si>
+  <si>
+    <t>Creation Ansible, Serverless trainings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1013,12 +1031,6 @@
       <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1238,12 +1250,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1253,6 +1259,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1681,20 +1693,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -1781,8 +1793,8 @@
         <v>218</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="F6" s="43" t="str">
-        <f>D6</f>
+      <c r="F6" s="41" t="str">
+        <f t="shared" ref="F6:F11" si="0">D6</f>
         <v>+33 (0)652891534</v>
       </c>
       <c r="G6" s="12"/>
@@ -1798,8 +1810,8 @@
         <v>199</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="F7" s="45" t="str">
-        <f>D7</f>
+      <c r="F7" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>training@mjbright.net</v>
       </c>
       <c r="G7" s="12"/>
@@ -1815,8 +1827,8 @@
         <v>228</v>
       </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="45" t="str">
-        <f>D8</f>
+      <c r="F8" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>https://www.mjbright.net</v>
       </c>
       <c r="G8" s="12"/>
@@ -1832,8 +1844,8 @@
         <v>134</v>
       </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="45" t="str">
-        <f>D9</f>
+      <c r="F9" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>https://mjbright.github.io/Talks</v>
       </c>
       <c r="G9" s="12"/>
@@ -1847,8 +1859,8 @@
         <v>210</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="45" t="str">
-        <f>D10</f>
+      <c r="F10" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>https://github.com/mjbright</v>
       </c>
       <c r="G10" s="12"/>
@@ -1862,8 +1874,8 @@
         <v>28</v>
       </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="45" t="str">
-        <f>D11</f>
+      <c r="F11" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>https://www.linkedin.com/in/mjbright</v>
       </c>
       <c r="G11" s="12"/>
@@ -1891,7 +1903,7 @@
         <v>31</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="45" t="str">
+      <c r="F13" s="43" t="str">
         <f>D13</f>
         <v>Michael Bright</v>
       </c>
@@ -1924,7 +1936,7 @@
         <v>39</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="45" t="str">
+      <c r="F15" s="43" t="str">
         <f>D15</f>
         <v>Grenoble, France</v>
       </c>
@@ -1941,7 +1953,7 @@
         <v>246</v>
       </c>
       <c r="E16" s="12"/>
-      <c r="F16" s="45" t="str">
+      <c r="F16" s="43" t="str">
         <f>D16</f>
         <v xml:space="preserve"> @mjbright Consulting</v>
       </c>
@@ -2007,7 +2019,7 @@
         <v>247</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="46" t="str">
+      <c r="F20" s="44" t="str">
         <f>D20</f>
         <v xml:space="preserve"> $@$mjbright Consulting</v>
       </c>
@@ -2034,7 +2046,7 @@
         <v>211</v>
       </c>
       <c r="E22" s="10"/>
-      <c r="F22" s="46" t="str">
+      <c r="F22" s="44" t="str">
         <f>D22</f>
         <v>07/2018</v>
       </c>
@@ -2048,7 +2060,7 @@
         <v>58</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="46" t="str">
+      <c r="F23" s="44" t="str">
         <f>D23</f>
         <v>Present</v>
       </c>
@@ -2131,7 +2143,7 @@
         <v>35</v>
       </c>
       <c r="E29" s="10"/>
-      <c r="F29" s="47" t="str">
+      <c r="F29" s="45" t="str">
         <f>D29</f>
         <v>Cloud Native Solution Architect</v>
       </c>
@@ -2145,7 +2157,7 @@
         <v>49</v>
       </c>
       <c r="E30" s="10"/>
-      <c r="F30" s="47" t="str">
+      <c r="F30" s="45" t="str">
         <f>D30</f>
         <v>HPE Customer Innovation Center - Grenoble France</v>
       </c>
@@ -2159,7 +2171,7 @@
         <v>52</v>
       </c>
       <c r="E31" s="10"/>
-      <c r="F31" s="47" t="str">
+      <c r="F31" s="45" t="str">
         <f>D31</f>
         <v>Cloud Native Solution Architect, HPE EG presales</v>
       </c>
@@ -2173,7 +2185,7 @@
         <v>55</v>
       </c>
       <c r="E32" s="10"/>
-      <c r="F32" s="47" t="str">
+      <c r="F32" s="45" t="str">
         <f>D32</f>
         <v>09/2013</v>
       </c>
@@ -2187,7 +2199,7 @@
         <v>219</v>
       </c>
       <c r="E33" s="10"/>
-      <c r="F33" s="47" t="str">
+      <c r="F33" s="45" t="str">
         <f>D33</f>
         <v>06/2018</v>
       </c>
@@ -2284,8 +2296,8 @@
         <v>67</v>
       </c>
       <c r="E40" s="12"/>
-      <c r="F40" s="48" t="str">
-        <f t="shared" ref="F40:F43" si="0">D40</f>
+      <c r="F40" s="46" t="str">
+        <f t="shared" ref="F40:F43" si="1">D40</f>
         <v>Cloud Engineer</v>
       </c>
       <c r="G40" s="25"/>
@@ -2299,8 +2311,8 @@
         <v>68</v>
       </c>
       <c r="E41" s="12"/>
-      <c r="F41" s="48" t="str">
-        <f t="shared" si="0"/>
+      <c r="F41" s="46" t="str">
+        <f t="shared" si="1"/>
         <v>HP CMS - Grenoble France</v>
       </c>
       <c r="G41" s="25"/>
@@ -2314,8 +2326,8 @@
         <v>69</v>
       </c>
       <c r="E42" s="12"/>
-      <c r="F42" s="48" t="str">
-        <f t="shared" si="0"/>
+      <c r="F42" s="46" t="str">
+        <f t="shared" si="1"/>
         <v>09/2005</v>
       </c>
       <c r="G42" s="25"/>
@@ -2329,8 +2341,8 @@
         <v>55</v>
       </c>
       <c r="E43" s="12"/>
-      <c r="F43" s="48" t="str">
-        <f t="shared" si="0"/>
+      <c r="F43" s="46" t="str">
+        <f t="shared" si="1"/>
         <v>09/2013</v>
       </c>
       <c r="G43" s="25"/>
@@ -2371,7 +2383,7 @@
         <v>72</v>
       </c>
       <c r="E46" s="12"/>
-      <c r="F46" s="44" t="s">
+      <c r="F46" s="42" t="s">
         <v>237</v>
       </c>
       <c r="G46" s="10"/>
@@ -2480,7 +2492,7 @@
         <v>79</v>
       </c>
       <c r="E54" s="12"/>
-      <c r="F54" s="48" t="str">
+      <c r="F54" s="46" t="str">
         <f>D54</f>
         <v>Solution Architect/Consultant</v>
       </c>
@@ -2494,8 +2506,8 @@
         <v>80</v>
       </c>
       <c r="E55" s="12"/>
-      <c r="F55" s="48" t="str">
-        <f t="shared" ref="F55:F57" si="1">D55</f>
+      <c r="F55" s="46" t="str">
+        <f t="shared" ref="F55:F57" si="2">D55</f>
         <v>HP OCBU - Grenoble France</v>
       </c>
       <c r="G55" s="10"/>
@@ -2514,8 +2526,8 @@
         <v>81</v>
       </c>
       <c r="E56" s="12"/>
-      <c r="F56" s="48" t="str">
-        <f t="shared" si="1"/>
+      <c r="F56" s="46" t="str">
+        <f t="shared" si="2"/>
         <v>02/1998</v>
       </c>
       <c r="G56" s="10"/>
@@ -2528,8 +2540,8 @@
         <v>69</v>
       </c>
       <c r="E57" s="12"/>
-      <c r="F57" s="48" t="str">
-        <f t="shared" si="1"/>
+      <c r="F57" s="46" t="str">
+        <f t="shared" si="2"/>
         <v>09/2005</v>
       </c>
       <c r="G57" s="10"/>
@@ -2650,7 +2662,7 @@
         <v>89</v>
       </c>
       <c r="E66" s="12"/>
-      <c r="F66" s="48" t="str">
+      <c r="F66" s="46" t="str">
         <f>D66</f>
         <v>Technical Lead/Software Engineer</v>
       </c>
@@ -2664,8 +2676,8 @@
         <v>80</v>
       </c>
       <c r="E67" s="12"/>
-      <c r="F67" s="48" t="str">
-        <f t="shared" ref="F67:F69" si="2">D67</f>
+      <c r="F67" s="46" t="str">
+        <f t="shared" ref="F67:F69" si="3">D67</f>
         <v>HP OCBU - Grenoble France</v>
       </c>
       <c r="G67" s="10"/>
@@ -2678,8 +2690,8 @@
         <v>90</v>
       </c>
       <c r="E68" s="12"/>
-      <c r="F68" s="48" t="str">
-        <f t="shared" si="2"/>
+      <c r="F68" s="46" t="str">
+        <f t="shared" si="3"/>
         <v>05/1992</v>
       </c>
       <c r="G68" s="10"/>
@@ -2692,8 +2704,8 @@
         <v>81</v>
       </c>
       <c r="E69" s="12"/>
-      <c r="F69" s="48" t="str">
-        <f t="shared" si="2"/>
+      <c r="F69" s="46" t="str">
+        <f t="shared" si="3"/>
         <v>02/1998</v>
       </c>
       <c r="G69" s="10"/>
@@ -2795,7 +2807,7 @@
         <v>97</v>
       </c>
       <c r="E77" s="12"/>
-      <c r="F77" s="49" t="s">
+      <c r="F77" s="47" t="s">
         <v>260</v>
       </c>
       <c r="G77" s="10"/>
@@ -2808,8 +2820,8 @@
         <v>98</v>
       </c>
       <c r="E78" s="12"/>
-      <c r="F78" s="48" t="str">
-        <f t="shared" ref="F78:F80" si="3">D78</f>
+      <c r="F78" s="46" t="str">
+        <f t="shared" ref="F78:F80" si="4">D78</f>
         <v>HP Research Labs - Bristol UK</v>
       </c>
       <c r="G78" s="10"/>
@@ -2822,8 +2834,8 @@
         <v>99</v>
       </c>
       <c r="E79" s="12"/>
-      <c r="F79" s="48" t="str">
-        <f t="shared" si="3"/>
+      <c r="F79" s="46" t="str">
+        <f t="shared" si="4"/>
         <v>08/1985</v>
       </c>
       <c r="G79" s="10"/>
@@ -2836,8 +2848,8 @@
         <v>90</v>
       </c>
       <c r="E80" s="12"/>
-      <c r="F80" s="48" t="str">
-        <f t="shared" si="3"/>
+      <c r="F80" s="46" t="str">
+        <f t="shared" si="4"/>
         <v>05/1992</v>
       </c>
       <c r="G80" s="10"/>
@@ -2887,7 +2899,7 @@
         <v>102</v>
       </c>
       <c r="E84" s="12"/>
-      <c r="F84" s="49" t="s">
+      <c r="F84" s="47" t="s">
         <v>263</v>
       </c>
       <c r="G84" s="10"/>
@@ -2900,8 +2912,8 @@
         <v>103</v>
       </c>
       <c r="E85" s="12"/>
-      <c r="F85" s="48" t="str">
-        <f t="shared" ref="F85:F87" si="4">D85</f>
+      <c r="F85" s="46" t="str">
+        <f t="shared" ref="F85:F87" si="5">D85</f>
         <v>BBC Research Labs - UK</v>
       </c>
       <c r="G85" s="10"/>
@@ -2914,8 +2926,8 @@
         <v>104</v>
       </c>
       <c r="E86" s="12"/>
-      <c r="F86" s="48" t="str">
-        <f t="shared" si="4"/>
+      <c r="F86" s="46" t="str">
+        <f t="shared" si="5"/>
         <v>09/1983</v>
       </c>
       <c r="G86" s="10"/>
@@ -2928,8 +2940,8 @@
         <v>105</v>
       </c>
       <c r="E87" s="12"/>
-      <c r="F87" s="48" t="str">
-        <f t="shared" si="4"/>
+      <c r="F87" s="46" t="str">
+        <f t="shared" si="5"/>
         <v>08/1984</v>
       </c>
       <c r="G87" s="10"/>
@@ -2990,7 +3002,7 @@
         <v>108</v>
       </c>
       <c r="E92" s="10"/>
-      <c r="F92" s="48" t="str">
+      <c r="F92" s="46" t="str">
         <f>D92</f>
         <v>Certifications</v>
       </c>
@@ -3004,8 +3016,8 @@
         <v>109</v>
       </c>
       <c r="E93" s="10"/>
-      <c r="F93" s="48" t="str">
-        <f t="shared" ref="F93:F95" si="5">D93</f>
+      <c r="F93" s="46" t="str">
+        <f t="shared" ref="F93:F95" si="6">D93</f>
         <v xml:space="preserve">Sep 2017 CNCF Kubernetes Administration (CKA) </v>
       </c>
       <c r="G93" s="10"/>
@@ -3018,8 +3030,8 @@
         <v>110</v>
       </c>
       <c r="E94" s="10"/>
-      <c r="F94" s="48" t="str">
-        <f t="shared" si="5"/>
+      <c r="F94" s="46" t="str">
+        <f t="shared" si="6"/>
         <v>May 2015 HPE Expert One, SDN Apps (HP0-Y48)</v>
       </c>
       <c r="G94" s="10"/>
@@ -3032,8 +3044,8 @@
         <v>111</v>
       </c>
       <c r="E95" s="10"/>
-      <c r="F95" s="48" t="str">
-        <f t="shared" si="5"/>
+      <c r="F95" s="46" t="str">
+        <f t="shared" si="6"/>
         <v>Nov 2013 RedHat RHCE/RHCSA</v>
       </c>
       <c r="G95" s="10"/>
@@ -3057,7 +3069,7 @@
         <v>112</v>
       </c>
       <c r="E97" s="10"/>
-      <c r="F97" s="48" t="str">
+      <c r="F97" s="46" t="str">
         <f>D97</f>
         <v>Cloud</v>
       </c>
@@ -3071,8 +3083,8 @@
         <v>113</v>
       </c>
       <c r="E98" s="10"/>
-      <c r="F98" s="48" t="str">
-        <f t="shared" ref="F98:F99" si="6">D98</f>
+      <c r="F98" s="46" t="str">
+        <f t="shared" ref="F98:F99" si="7">D98</f>
         <v>PaaS OpenShift, Google App Engine, Heroku</v>
       </c>
       <c r="G98" s="10"/>
@@ -3085,8 +3097,8 @@
         <v>114</v>
       </c>
       <c r="E99" s="10"/>
-      <c r="F99" s="48" t="str">
-        <f t="shared" si="6"/>
+      <c r="F99" s="46" t="str">
+        <f t="shared" si="7"/>
         <v>IaaS Azure, AWS, OpenStack, CloudStack, SDN (OpenDaylight), Docker</v>
       </c>
       <c r="G99" s="10"/>
@@ -3116,8 +3128,8 @@
         <v>115</v>
       </c>
       <c r="E101" s="10"/>
-      <c r="F101" s="48" t="str">
-        <f t="shared" ref="F101:F104" si="7">D101</f>
+      <c r="F101" s="46" t="str">
+        <f t="shared" ref="F101:F103" si="8">D101</f>
         <v>Languages and Paradigms</v>
       </c>
       <c r="G101" s="10"/>
@@ -3143,8 +3155,8 @@
         <v>117</v>
       </c>
       <c r="E103" s="10"/>
-      <c r="F103" s="48" t="str">
-        <f t="shared" si="7"/>
+      <c r="F103" s="46" t="str">
+        <f t="shared" si="8"/>
         <v>SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</v>
       </c>
       <c r="G103" s="10"/>
@@ -3194,8 +3206,8 @@
         <v>120</v>
       </c>
       <c r="E107" s="10"/>
-      <c r="F107" s="48" t="str">
-        <f t="shared" ref="F106:F108" si="8">D107</f>
+      <c r="F107" s="46" t="str">
+        <f t="shared" ref="F107:F108" si="9">D107</f>
         <v>Eclipse, Git, svn, vim, maven, Jenkins, gdb</v>
       </c>
       <c r="G107" s="10"/>
@@ -3208,8 +3220,8 @@
         <v>121</v>
       </c>
       <c r="E108" s="10"/>
-      <c r="F108" s="48" t="str">
-        <f t="shared" si="8"/>
+      <c r="F108" s="46" t="str">
+        <f t="shared" si="9"/>
         <v>Virtualization (vSphere/Pyvmomi, KVM-Qemu, VirtualBox)</v>
       </c>
       <c r="G108" s="10"/>
@@ -3300,8 +3312,8 @@
         <v>125</v>
       </c>
       <c r="E115" s="10"/>
-      <c r="F115" s="48" t="str">
-        <f t="shared" ref="F115:F120" si="9">D115</f>
+      <c r="F115" s="46" t="str">
+        <f t="shared" ref="F115:F118" si="10">D115</f>
         <v>B.Sc/Dip.Eng in  Electronic Control and Robotics</v>
       </c>
       <c r="G115" s="10"/>
@@ -3314,8 +3326,8 @@
         <v>270</v>
       </c>
       <c r="E116" s="10"/>
-      <c r="F116" s="48" t="str">
-        <f t="shared" si="9"/>
+      <c r="F116" s="46" t="str">
+        <f t="shared" si="10"/>
         <v>University Of Hull,  UK</v>
       </c>
       <c r="G116" s="10"/>
@@ -3328,8 +3340,8 @@
         <v>128</v>
       </c>
       <c r="E117" s="10"/>
-      <c r="F117" s="48" t="str">
-        <f t="shared" si="9"/>
+      <c r="F117" s="46" t="str">
+        <f t="shared" si="10"/>
         <v>10/1980</v>
       </c>
       <c r="G117" s="10"/>
@@ -3342,8 +3354,8 @@
         <v>129</v>
       </c>
       <c r="E118" s="10"/>
-      <c r="F118" s="48" t="str">
-        <f t="shared" si="9"/>
+      <c r="F118" s="46" t="str">
+        <f t="shared" si="10"/>
         <v>07/1985</v>
       </c>
       <c r="G118" s="10"/>
@@ -3417,8 +3429,8 @@
         <v>133</v>
       </c>
       <c r="E124" s="10"/>
-      <c r="F124" s="48" t="str">
-        <f t="shared" ref="F124:F129" si="10">D124</f>
+      <c r="F124" s="46" t="str">
+        <f t="shared" ref="F124:F129" si="11">D124</f>
         <v>Conference Talks</v>
       </c>
       <c r="G124" s="10"/>
@@ -3431,8 +3443,8 @@
         <v>134</v>
       </c>
       <c r="E125" s="10"/>
-      <c r="F125" s="48" t="str">
-        <f t="shared" si="10"/>
+      <c r="F125" s="46" t="str">
+        <f t="shared" si="11"/>
         <v>https://mjbright.github.io/Talks</v>
       </c>
       <c r="G125" s="10"/>
@@ -3445,8 +3457,8 @@
         <v>216</v>
       </c>
       <c r="E126" s="10"/>
-      <c r="F126" s="48" t="str">
-        <f t="shared" si="10"/>
+      <c r="F126" s="46" t="str">
+        <f t="shared" si="11"/>
         <v>2018 FOSSCon (Pres+Lab), FOSS Asia (Pres+Lab), Code Europe, PyConfr</v>
       </c>
       <c r="G126" s="10"/>
@@ -3459,8 +3471,8 @@
         <v>136</v>
       </c>
       <c r="E127" s="10"/>
-      <c r="F127" s="48" t="str">
-        <f t="shared" si="10"/>
+      <c r="F127" s="46" t="str">
+        <f t="shared" si="11"/>
         <v>2017 Devconf.cz, Snowcamp.io, HPE TSS, HPE TES, DockerConUS, RMLL, OSS EU (Pres+Lab)</v>
       </c>
       <c r="G127" s="10"/>
@@ -3473,8 +3485,8 @@
         <v>137</v>
       </c>
       <c r="E128" s="10"/>
-      <c r="F128" s="48" t="str">
-        <f t="shared" si="10"/>
+      <c r="F128" s="46" t="str">
+        <f t="shared" si="11"/>
         <v>2016 Europython (Pres+Lab), ContainerCon Europe (Pres+Lab)</v>
       </c>
       <c r="G128" s="10"/>
@@ -3487,8 +3499,8 @@
         <v>138</v>
       </c>
       <c r="E129" s="10"/>
-      <c r="F129" s="48" t="str">
-        <f t="shared" si="10"/>
+      <c r="F129" s="46" t="str">
+        <f t="shared" si="11"/>
         <v>2015 Pyconfr, Ipython vers Jupyter</v>
       </c>
       <c r="G129" s="10"/>
@@ -3513,7 +3525,7 @@
       </c>
       <c r="E131" s="10"/>
       <c r="F131" s="18" t="str">
-        <f t="shared" ref="F131:F133" si="11">D131</f>
+        <f t="shared" ref="F131:F133" si="12">D131</f>
         <v>Startup Weekend</v>
       </c>
       <c r="G131" s="10"/>
@@ -3526,8 +3538,8 @@
         <v>221</v>
       </c>
       <c r="E132" s="10"/>
-      <c r="F132" s="48" t="str">
-        <f t="shared" si="11"/>
+      <c r="F132" s="46" t="str">
+        <f t="shared" si="12"/>
         <v>2018-Nov: Community Security System</v>
       </c>
       <c r="G132" s="10"/>
@@ -3540,8 +3552,8 @@
         <v>141</v>
       </c>
       <c r="E133" s="10"/>
-      <c r="F133" s="48" t="str">
-        <f t="shared" si="11"/>
+      <c r="F133" s="46" t="str">
+        <f t="shared" si="12"/>
         <v>2012-Nov 2nd place: https://www.archionline.com/</v>
       </c>
       <c r="G133" s="10"/>
@@ -3566,7 +3578,7 @@
       </c>
       <c r="E135" s="10"/>
       <c r="F135" s="18" t="str">
-        <f t="shared" ref="F135:F138" si="12">D135</f>
+        <f t="shared" ref="F135" si="13">D135</f>
         <v>Miscellaneous</v>
       </c>
       <c r="G135" s="10"/>
@@ -3579,7 +3591,7 @@
         <v>143</v>
       </c>
       <c r="E136" s="10"/>
-      <c r="F136" s="49" t="s">
+      <c r="F136" s="47" t="s">
         <v>273</v>
       </c>
       <c r="G136" s="10"/>
@@ -3710,14 +3722,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE271112-8313-456B-92F1-71D6C3DCE9AF}">
-  <dimension ref="A1:M144"/>
+  <dimension ref="A1:M145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F148" sqref="F148"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" customWidth="1"/>
     <col min="6" max="6" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3728,20 +3742,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -3828,8 +3842,8 @@
         <v>218</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="F6" s="43" t="str">
-        <f>D6</f>
+      <c r="F6" s="41" t="str">
+        <f t="shared" ref="F6:F11" si="0">D6</f>
         <v>+33 (0)652891534</v>
       </c>
       <c r="G6" s="12"/>
@@ -3845,8 +3859,8 @@
         <v>199</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="F7" s="45" t="str">
-        <f>D7</f>
+      <c r="F7" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>training@mjbright.net</v>
       </c>
       <c r="G7" s="12"/>
@@ -3862,8 +3876,8 @@
         <v>228</v>
       </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="45" t="str">
-        <f>D8</f>
+      <c r="F8" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>https://www.mjbright.net</v>
       </c>
       <c r="G8" s="12"/>
@@ -3879,8 +3893,8 @@
         <v>134</v>
       </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="45" t="str">
-        <f>D9</f>
+      <c r="F9" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>https://mjbright.github.io/Talks</v>
       </c>
       <c r="G9" s="12"/>
@@ -3894,8 +3908,8 @@
         <v>210</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="45" t="str">
-        <f>D10</f>
+      <c r="F10" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>https://github.com/mjbright</v>
       </c>
       <c r="G10" s="12"/>
@@ -3909,8 +3923,8 @@
         <v>28</v>
       </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="45" t="str">
-        <f>D11</f>
+      <c r="F11" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>https://www.linkedin.com/in/mjbright</v>
       </c>
       <c r="G11" s="12"/>
@@ -3938,7 +3952,7 @@
         <v>31</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="45" t="str">
+      <c r="F13" s="43" t="str">
         <f>D13</f>
         <v>Michael Bright</v>
       </c>
@@ -3971,7 +3985,7 @@
         <v>39</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="45" t="str">
+      <c r="F15" s="43" t="str">
         <f>D15</f>
         <v>Grenoble, France</v>
       </c>
@@ -3988,7 +4002,7 @@
         <v>246</v>
       </c>
       <c r="E16" s="12"/>
-      <c r="F16" s="45" t="str">
+      <c r="F16" s="43" t="str">
         <f>D16</f>
         <v xml:space="preserve"> @mjbright Consulting</v>
       </c>
@@ -4038,11 +4052,11 @@
         <v>34</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>212</v>
+        <v>280</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="8" t="s">
-        <v>229</v>
+        <v>281</v>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -4054,7 +4068,7 @@
         <v>247</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="46" t="str">
+      <c r="F20" s="44" t="str">
         <f>D20</f>
         <v xml:space="preserve"> $@$mjbright Consulting</v>
       </c>
@@ -4081,7 +4095,7 @@
         <v>211</v>
       </c>
       <c r="E22" s="10"/>
-      <c r="F22" s="46" t="str">
+      <c r="F22" s="44" t="str">
         <f>D22</f>
         <v>07/2018</v>
       </c>
@@ -4095,7 +4109,7 @@
         <v>58</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="46" t="str">
+      <c r="F23" s="44" t="str">
         <f>D23</f>
         <v>Present</v>
       </c>
@@ -4106,7 +4120,7 @@
         <v>60</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>223</v>
+        <v>283</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" t="s">
@@ -4119,7 +4133,7 @@
         <v>60</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>227</v>
+        <v>282</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" t="s">
@@ -4132,12 +4146,9 @@
         <v>60</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>214</v>
+        <v>284</v>
       </c>
       <c r="E26" s="10"/>
-      <c r="F26" t="s">
-        <v>232</v>
-      </c>
       <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
@@ -4145,111 +4156,111 @@
         <v>60</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>215</v>
+        <v>285</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" t="s">
+        <v>232</v>
+      </c>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C28" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" t="s">
         <v>233</v>
       </c>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-    </row>
-    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D30" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="47" t="str">
-        <f>D29</f>
+      <c r="E30" s="10"/>
+      <c r="F30" s="45" t="str">
+        <f>D30</f>
         <v>Cloud Native Solution Architect</v>
       </c>
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C30" s="8" t="s">
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C31" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D31" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="47" t="str">
-        <f>D30</f>
+      <c r="E31" s="10"/>
+      <c r="F31" s="45" t="str">
+        <f>D31</f>
         <v>HPE Customer Innovation Center - Grenoble France</v>
       </c>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D32" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="47" t="str">
-        <f>D31</f>
+      <c r="E32" s="10"/>
+      <c r="F32" s="45" t="str">
+        <f>D32</f>
         <v>Cloud Native Solution Architect, HPE EG presales</v>
-      </c>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C32" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="47" t="str">
-        <f>D32</f>
-        <v>09/2013</v>
       </c>
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C33" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="39" t="s">
-        <v>219</v>
+        <v>54</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="E33" s="10"/>
-      <c r="F33" s="47" t="str">
+      <c r="F33" s="45" t="str">
         <f>D33</f>
-        <v>06/2018</v>
+        <v>09/2013</v>
       </c>
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C34" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>249</v>
+        <v>219</v>
       </c>
       <c r="E34" s="10"/>
-      <c r="F34" t="s">
-        <v>250</v>
+      <c r="F34" s="45" t="str">
+        <f>D34</f>
+        <v>06/2018</v>
       </c>
       <c r="G34" s="10"/>
     </row>
@@ -4257,12 +4268,12 @@
       <c r="C35" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>61</v>
+      <c r="D35" s="39" t="s">
+        <v>249</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G35" s="10"/>
     </row>
@@ -4271,11 +4282,11 @@
         <v>60</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="G36" s="10"/>
     </row>
@@ -4284,11 +4295,11 @@
         <v>60</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G37" s="10"/>
     </row>
@@ -4297,174 +4308,174 @@
         <v>60</v>
       </c>
       <c r="D38" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" t="s">
+        <v>235</v>
+      </c>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C39" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="10"/>
-      <c r="F38" t="str">
-        <f>D38</f>
+      <c r="E39" s="10"/>
+      <c r="F39" t="str">
+        <f>D39</f>
         <v>Cloud Automation (DigitalO, GCE, Azure, AWS, Terraform, Heat, Ansible, Vagrant)</v>
       </c>
-      <c r="G38" s="10"/>
-    </row>
-    <row r="39" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
-    </row>
-    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C40" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>67</v>
-      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="23"/>
       <c r="E40" s="12"/>
-      <c r="F40" s="48" t="str">
-        <f t="shared" ref="F40:F43" si="0">D40</f>
-        <v>Cloud Engineer</v>
-      </c>
-      <c r="G40" s="25"/>
-      <c r="I40" s="26"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C41" s="11" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E41" s="12"/>
-      <c r="F41" s="48" t="str">
-        <f t="shared" si="0"/>
-        <v>HP CMS - Grenoble France</v>
+      <c r="F41" s="46" t="str">
+        <f t="shared" ref="F41:F44" si="1">D41</f>
+        <v>Cloud Engineer</v>
       </c>
       <c r="G41" s="25"/>
       <c r="I41" s="26"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C42" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>69</v>
+      <c r="C42" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="E42" s="12"/>
-      <c r="F42" s="48" t="str">
-        <f t="shared" si="0"/>
-        <v>09/2005</v>
+      <c r="F42" s="46" t="str">
+        <f t="shared" si="1"/>
+        <v>HP CMS - Grenoble France</v>
       </c>
       <c r="G42" s="25"/>
       <c r="I42" s="26"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C43" s="21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E43" s="12"/>
-      <c r="F43" s="48" t="str">
-        <f t="shared" si="0"/>
-        <v>09/2013</v>
+      <c r="F43" s="46" t="str">
+        <f t="shared" si="1"/>
+        <v>09/2005</v>
       </c>
       <c r="G43" s="25"/>
       <c r="I43" s="26"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C44" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="E44" s="12"/>
-      <c r="F44" t="s">
-        <v>236</v>
+      <c r="F44" s="46" t="str">
+        <f t="shared" si="1"/>
+        <v>09/2013</v>
       </c>
       <c r="G44" s="25"/>
       <c r="I44" s="26"/>
     </row>
-    <row r="45" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C45" s="21" t="s">
         <v>60</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" t="s">
-        <v>254</v>
-      </c>
-      <c r="G45" s="10"/>
+        <v>236</v>
+      </c>
+      <c r="G45" s="25"/>
+      <c r="I45" s="26"/>
     </row>
     <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C46" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E46" s="12"/>
-      <c r="F46" s="44" t="s">
-        <v>237</v>
+      <c r="F46" t="s">
+        <v>254</v>
       </c>
       <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C47" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E47" s="12"/>
-      <c r="F47" t="s">
-        <v>253</v>
+      <c r="F47" s="42" t="s">
+        <v>237</v>
       </c>
       <c r="G47" s="10"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
-      <c r="M47" s="16"/>
     </row>
     <row r="48" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C48" s="21" t="s">
         <v>60</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E48" s="12"/>
       <c r="F48" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G48" s="10"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
     </row>
     <row r="49" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C49" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E49" s="12"/>
-      <c r="F49" s="38" t="s">
-        <v>238</v>
+      <c r="F49" t="s">
+        <v>251</v>
       </c>
       <c r="G49" s="10"/>
     </row>
@@ -4473,163 +4484,163 @@
         <v>220</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E50" s="12"/>
       <c r="F50" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G50" s="10"/>
     </row>
     <row r="51" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C51" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D51" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E51" s="12"/>
+      <c r="F51" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C52" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="E51" s="12"/>
-      <c r="F51" t="s">
-        <v>255</v>
-      </c>
-      <c r="G51" s="10"/>
-    </row>
-    <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C52" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" t="s">
+        <v>255</v>
+      </c>
+      <c r="G52" s="10"/>
+    </row>
+    <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C53" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" s="12"/>
+      <c r="F53" t="s">
         <v>240</v>
       </c>
-      <c r="G52" s="25"/>
-      <c r="I52" s="26"/>
-    </row>
-    <row r="53" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
+      <c r="G53" s="25"/>
+      <c r="I53" s="26"/>
+    </row>
+    <row r="54" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="10"/>
-    </row>
-    <row r="54" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C54" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>79</v>
-      </c>
+      <c r="B54" s="23"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="23"/>
       <c r="E54" s="12"/>
-      <c r="F54" s="48" t="str">
-        <f>D54</f>
-        <v>Solution Architect/Consultant</v>
-      </c>
+      <c r="F54" s="23"/>
       <c r="G54" s="10"/>
     </row>
     <row r="55" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="C55" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E55" s="12"/>
+      <c r="F55" s="46" t="str">
+        <f>D55</f>
+        <v>Solution Architect/Consultant</v>
+      </c>
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C56" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D55" s="18" t="s">
+      <c r="D56" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="12"/>
-      <c r="F55" s="48" t="str">
-        <f t="shared" ref="F55:F57" si="1">D55</f>
+      <c r="E56" s="12"/>
+      <c r="F56" s="46" t="str">
+        <f t="shared" ref="F56:F58" si="2">D56</f>
         <v>HP OCBU - Grenoble France</v>
       </c>
-      <c r="G55" s="10"/>
-      <c r="H55" s="16"/>
-      <c r="I55" s="16"/>
-      <c r="J55" s="16"/>
-      <c r="K55" s="16"/>
-      <c r="L55" s="16"/>
-      <c r="M55" s="16"/>
-    </row>
-    <row r="56" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C56" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D56" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="E56" s="12"/>
-      <c r="F56" s="48" t="str">
-        <f t="shared" si="1"/>
-        <v>02/1998</v>
-      </c>
       <c r="G56" s="10"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
     </row>
     <row r="57" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C57" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>69</v>
+        <v>54</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>81</v>
       </c>
       <c r="E57" s="12"/>
-      <c r="F57" s="48" t="str">
-        <f t="shared" si="1"/>
-        <v>09/2005</v>
+      <c r="F57" s="46" t="str">
+        <f t="shared" si="2"/>
+        <v>02/1998</v>
       </c>
       <c r="G57" s="10"/>
     </row>
     <row r="58" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C58" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E58" s="12"/>
-      <c r="F58" s="11" t="s">
-        <v>256</v>
+      <c r="F58" s="46" t="str">
+        <f t="shared" si="2"/>
+        <v>09/2005</v>
       </c>
       <c r="G58" s="10"/>
     </row>
     <row r="59" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C59" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E59" s="12"/>
       <c r="F59" s="11" t="s">
-        <v>83</v>
+        <v>256</v>
       </c>
       <c r="G59" s="10"/>
     </row>
     <row r="60" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C60" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E60" s="12"/>
       <c r="F60" s="11" t="s">
-        <v>257</v>
+        <v>83</v>
       </c>
       <c r="G60" s="10"/>
     </row>
     <row r="61" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C61" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="D61" s="19" t="s">
-        <v>85</v>
+        <v>60</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="E61" s="12"/>
-      <c r="F61" s="19" t="s">
-        <v>85</v>
+      <c r="F61" s="11" t="s">
+        <v>257</v>
       </c>
       <c r="G61" s="10"/>
     </row>
@@ -4638,11 +4649,11 @@
         <v>220</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E62" s="12"/>
       <c r="F62" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G62" s="10"/>
     </row>
@@ -4651,123 +4662,123 @@
         <v>220</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E63" s="12"/>
       <c r="F63" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="G63" s="14"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
-      <c r="K63" s="9"/>
-      <c r="L63" s="9"/>
-      <c r="M63" s="9"/>
+        <v>86</v>
+      </c>
+      <c r="G63" s="10"/>
     </row>
     <row r="64" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C64" s="21" t="s">
         <v>220</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E64" s="12"/>
       <c r="F64" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G64" s="14"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+    </row>
+    <row r="65" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C65" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D65" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="G64" s="10"/>
-    </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="22" t="s">
+      <c r="E65" s="12"/>
+      <c r="F65" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G65" s="10"/>
+    </row>
+    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B65" s="23"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="10"/>
-    </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C66" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>89</v>
-      </c>
+      <c r="B66" s="23"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="23"/>
       <c r="E66" s="12"/>
-      <c r="F66" s="48" t="str">
-        <f>D66</f>
-        <v>Technical Lead/Software Engineer</v>
-      </c>
+      <c r="F66" s="23"/>
       <c r="G66" s="10"/>
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="C67" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E67" s="12"/>
+      <c r="F67" s="46" t="str">
+        <f>D67</f>
+        <v>Technical Lead/Software Engineer</v>
+      </c>
+      <c r="G67" s="10"/>
+    </row>
+    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C68" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="D68" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E67" s="12"/>
-      <c r="F67" s="48" t="str">
-        <f t="shared" ref="F67:F69" si="2">D67</f>
+      <c r="E68" s="12"/>
+      <c r="F68" s="46" t="str">
+        <f t="shared" ref="F68:F70" si="3">D68</f>
         <v>HP OCBU - Grenoble France</v>
-      </c>
-      <c r="G67" s="10"/>
-    </row>
-    <row r="68" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C68" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D68" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E68" s="12"/>
-      <c r="F68" s="48" t="str">
-        <f t="shared" si="2"/>
-        <v>05/1992</v>
       </c>
       <c r="G68" s="10"/>
     </row>
     <row r="69" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C69" s="21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D69" s="27" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E69" s="12"/>
-      <c r="F69" s="48" t="str">
-        <f t="shared" si="2"/>
-        <v>02/1998</v>
+      <c r="F69" s="46" t="str">
+        <f t="shared" si="3"/>
+        <v>05/1992</v>
       </c>
       <c r="G69" s="10"/>
     </row>
     <row r="70" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C70" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>91</v>
+        <v>57</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>81</v>
       </c>
       <c r="E70" s="12"/>
-      <c r="F70" s="11" t="s">
-        <v>258</v>
+      <c r="F70" s="46" t="str">
+        <f t="shared" si="3"/>
+        <v>02/1998</v>
       </c>
       <c r="G70" s="10"/>
     </row>
     <row r="71" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C71" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E71" s="12"/>
       <c r="F71" s="11" t="s">
-        <v>92</v>
+        <v>258</v>
       </c>
       <c r="G71" s="10"/>
     </row>
@@ -4776,37 +4787,37 @@
         <v>220</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E72" s="12"/>
       <c r="F72" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G72" s="10"/>
     </row>
     <row r="73" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C73" s="21" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E73" s="12"/>
       <c r="F73" s="11" t="s">
-        <v>259</v>
+        <v>93</v>
       </c>
       <c r="G73" s="10"/>
     </row>
     <row r="74" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C74" s="21" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E74" s="12"/>
       <c r="F74" s="11" t="s">
-        <v>95</v>
+        <v>259</v>
       </c>
       <c r="G74" s="10"/>
     </row>
@@ -4815,90 +4826,90 @@
         <v>220</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E75" s="12"/>
       <c r="F75" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G75" s="10"/>
+    </row>
+    <row r="76" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C76" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D76" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="G75" s="10"/>
-    </row>
-    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="22" t="s">
+      <c r="E76" s="12"/>
+      <c r="F76" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G76" s="10"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="23"/>
-      <c r="C76" s="24"/>
-      <c r="D76" s="23"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="23"/>
-      <c r="G76" s="10"/>
-    </row>
-    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C77" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D77" s="18" t="s">
-        <v>97</v>
-      </c>
+      <c r="B77" s="23"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="23"/>
       <c r="E77" s="12"/>
-      <c r="F77" s="49" t="s">
-        <v>260</v>
-      </c>
+      <c r="F77" s="23"/>
       <c r="G77" s="10"/>
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="C78" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E78" s="12"/>
+      <c r="F78" s="47" t="s">
+        <v>260</v>
+      </c>
+      <c r="G78" s="10"/>
+    </row>
+    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C79" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D79" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E78" s="12"/>
-      <c r="F78" s="48" t="str">
-        <f t="shared" ref="F78:F80" si="3">D78</f>
+      <c r="E79" s="12"/>
+      <c r="F79" s="46" t="str">
+        <f t="shared" ref="F79:F81" si="4">D79</f>
         <v>HP Research Labs - Bristol UK</v>
-      </c>
-      <c r="G78" s="10"/>
-    </row>
-    <row r="79" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C79" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D79" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="E79" s="12"/>
-      <c r="F79" s="48" t="str">
-        <f t="shared" si="3"/>
-        <v>08/1985</v>
       </c>
       <c r="G79" s="10"/>
     </row>
     <row r="80" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C80" s="21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D80" s="27" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E80" s="12"/>
-      <c r="F80" s="48" t="str">
-        <f t="shared" si="3"/>
-        <v>05/1992</v>
+      <c r="F80" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>08/1985</v>
       </c>
       <c r="G80" s="10"/>
     </row>
     <row r="81" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C81" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D81" s="19" t="s">
-        <v>100</v>
+        <v>57</v>
+      </c>
+      <c r="D81" s="27" t="s">
+        <v>90</v>
       </c>
       <c r="E81" s="12"/>
-      <c r="F81" s="19" t="s">
-        <v>261</v>
+      <c r="F81" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>05/1992</v>
       </c>
       <c r="G81" s="10"/>
     </row>
@@ -4907,153 +4918,152 @@
         <v>60</v>
       </c>
       <c r="D82" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E82" s="12"/>
       <c r="F82" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="G82" s="10"/>
+    </row>
+    <row r="83" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C83" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D83" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E83" s="12"/>
+      <c r="F83" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="G82" s="10"/>
-    </row>
-    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="22" t="s">
+      <c r="G83" s="10"/>
+    </row>
+    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B83" s="23"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="23"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="23"/>
-      <c r="G83" s="10"/>
-    </row>
-    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C84" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D84" s="18" t="s">
-        <v>102</v>
-      </c>
+      <c r="B84" s="23"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="23"/>
       <c r="E84" s="12"/>
-      <c r="F84" s="49" t="s">
-        <v>263</v>
-      </c>
+      <c r="F84" s="23"/>
       <c r="G84" s="10"/>
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="C85" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E85" s="12"/>
+      <c r="F85" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="G85" s="10"/>
+    </row>
+    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C86" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D85" s="18" t="s">
+      <c r="D86" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E85" s="12"/>
-      <c r="F85" s="48" t="str">
-        <f t="shared" ref="F85:F87" si="4">D85</f>
+      <c r="E86" s="12"/>
+      <c r="F86" s="46" t="str">
+        <f t="shared" ref="F86:F88" si="5">D86</f>
         <v>BBC Research Labs - UK</v>
-      </c>
-      <c r="G85" s="10"/>
-    </row>
-    <row r="86" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C86" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D86" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="E86" s="12"/>
-      <c r="F86" s="48" t="str">
-        <f t="shared" si="4"/>
-        <v>09/1983</v>
       </c>
       <c r="G86" s="10"/>
     </row>
     <row r="87" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C87" s="21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D87" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E87" s="12"/>
-      <c r="F87" s="48" t="str">
-        <f t="shared" si="4"/>
-        <v>08/1984</v>
+      <c r="F87" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v>09/1983</v>
       </c>
       <c r="G87" s="10"/>
     </row>
     <row r="88" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C88" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D88" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D88" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E88" s="12"/>
+      <c r="F88" s="46" t="str">
+        <f t="shared" si="5"/>
+        <v>08/1984</v>
+      </c>
+      <c r="G88" s="10"/>
+    </row>
+    <row r="89" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C89" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D89" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="E88" s="12"/>
-      <c r="F88" s="19" t="s">
+      <c r="E89" s="12"/>
+      <c r="F89" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="G88" s="10"/>
-    </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="22" t="s">
+      <c r="G89" s="10"/>
+    </row>
+    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B89" s="23"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="23"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="23"/>
-      <c r="G89" s="10"/>
-    </row>
-    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="28" t="s">
+      <c r="B90" s="23"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="10"/>
+    </row>
+    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B90" s="28" t="s">
+      <c r="B91" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C90" s="29"/>
-      <c r="D90" s="28"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="10"/>
-    </row>
-    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="22" t="s">
+      <c r="C91" s="29"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="10"/>
+    </row>
+    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B91" s="23"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="23"/>
-      <c r="E91" s="10"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="10"/>
-    </row>
-    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C92" s="21" t="s">
+      <c r="B92" s="23"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="10"/>
+    </row>
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C93" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D92" s="18" t="s">
+      <c r="D93" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="E92" s="10"/>
-      <c r="F92" s="48" t="str">
-        <f>D92</f>
+      <c r="E93" s="10"/>
+      <c r="F93" s="46" t="str">
+        <f>D93</f>
         <v>Certifications</v>
-      </c>
-      <c r="G92" s="10"/>
-    </row>
-    <row r="93" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C93" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D93" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E93" s="10"/>
-      <c r="F93" s="48" t="str">
-        <f t="shared" ref="F93:F95" si="5">D93</f>
-        <v xml:space="preserve">Sep 2017 CNCF Kubernetes Administration (CKA) </v>
       </c>
       <c r="G93" s="10"/>
     </row>
@@ -5062,12 +5072,12 @@
         <v>60</v>
       </c>
       <c r="D94" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E94" s="10"/>
-      <c r="F94" s="48" t="str">
-        <f t="shared" si="5"/>
-        <v>May 2015 HPE Expert One, SDN Apps (HP0-Y48)</v>
+      <c r="F94" s="46" t="str">
+        <f t="shared" ref="F94:F96" si="6">D94</f>
+        <v xml:space="preserve">Sep 2017 CNCF Kubernetes Administration (CKA) </v>
       </c>
       <c r="G94" s="10"/>
     </row>
@@ -5076,51 +5086,51 @@
         <v>60</v>
       </c>
       <c r="D95" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E95" s="10"/>
+      <c r="F95" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v>May 2015 HPE Expert One, SDN Apps (HP0-Y48)</v>
+      </c>
+      <c r="G95" s="10"/>
+    </row>
+    <row r="96" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C96" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D96" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E95" s="10"/>
-      <c r="F95" s="48" t="str">
-        <f t="shared" si="5"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="46" t="str">
+        <f t="shared" si="6"/>
         <v>Nov 2013 RedHat RHCE/RHCSA</v>
       </c>
-      <c r="G95" s="10"/>
-    </row>
-    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="22" t="s">
+      <c r="G96" s="10"/>
+    </row>
+    <row r="97" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B96" s="23"/>
-      <c r="C96" s="24"/>
-      <c r="D96" s="23"/>
-      <c r="E96" s="10"/>
-      <c r="F96" s="23"/>
-      <c r="G96" s="10"/>
-    </row>
-    <row r="97" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C97" s="21" t="s">
+      <c r="B97" s="23"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="10"/>
+    </row>
+    <row r="98" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C98" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D97" s="18" t="s">
+      <c r="D98" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E97" s="10"/>
-      <c r="F97" s="48" t="str">
-        <f>D97</f>
+      <c r="E98" s="10"/>
+      <c r="F98" s="46" t="str">
+        <f>D98</f>
         <v>Cloud</v>
-      </c>
-      <c r="G97" s="10"/>
-    </row>
-    <row r="98" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C98" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D98" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E98" s="10"/>
-      <c r="F98" s="48" t="str">
-        <f t="shared" ref="F98:F99" si="6">D98</f>
-        <v>PaaS OpenShift, Google App Engine, Heroku</v>
       </c>
       <c r="G98" s="10"/>
     </row>
@@ -5129,56 +5139,57 @@
         <v>60</v>
       </c>
       <c r="D99" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E99" s="10"/>
+      <c r="F99" s="46" t="str">
+        <f t="shared" ref="F99:F100" si="7">D99</f>
+        <v>PaaS OpenShift, Google App Engine, Heroku</v>
+      </c>
+      <c r="G99" s="10"/>
+    </row>
+    <row r="100" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C100" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D100" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E99" s="10"/>
-      <c r="F99" s="48" t="str">
-        <f t="shared" si="6"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="46" t="str">
+        <f t="shared" si="7"/>
         <v>IaaS Azure, AWS, OpenStack, CloudStack, SDN (OpenDaylight), Docker</v>
       </c>
-      <c r="G99" s="10"/>
-    </row>
-    <row r="100" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="22" t="s">
+      <c r="G100" s="10"/>
+    </row>
+    <row r="101" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B100" s="23"/>
-      <c r="C100" s="24"/>
-      <c r="D100" s="23"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="23"/>
-      <c r="G100" s="14"/>
-      <c r="H100" s="9"/>
-      <c r="I100" s="9"/>
-      <c r="J100" s="9"/>
-      <c r="K100" s="9"/>
-      <c r="L100" s="9"/>
-      <c r="M100" s="9"/>
-    </row>
-    <row r="101" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C101" s="21" t="s">
+      <c r="B101" s="23"/>
+      <c r="C101" s="24"/>
+      <c r="D101" s="23"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="23"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="9"/>
+      <c r="I101" s="9"/>
+      <c r="J101" s="9"/>
+      <c r="K101" s="9"/>
+      <c r="L101" s="9"/>
+      <c r="M101" s="9"/>
+    </row>
+    <row r="102" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C102" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D101" s="18" t="s">
+      <c r="D102" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="E101" s="10"/>
-      <c r="F101" s="48" t="str">
-        <f t="shared" ref="F101:F104" si="7">D101</f>
+      <c r="E102" s="10"/>
+      <c r="F102" s="46" t="str">
+        <f t="shared" ref="F102:F104" si="8">D102</f>
         <v>Languages and Paradigms</v>
-      </c>
-      <c r="G101" s="10"/>
-    </row>
-    <row r="102" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C102" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D102" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E102" s="10"/>
-      <c r="F102" s="19" t="s">
-        <v>265</v>
       </c>
       <c r="G102" s="10"/>
     </row>
@@ -5187,12 +5198,11 @@
         <v>60</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E103" s="10"/>
-      <c r="F103" s="48" t="str">
-        <f t="shared" si="7"/>
-        <v>SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</v>
+      <c r="F103" s="19" t="s">
+        <v>265</v>
       </c>
       <c r="G103" s="10"/>
     </row>
@@ -5201,49 +5211,49 @@
         <v>60</v>
       </c>
       <c r="D104" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E104" s="10"/>
+      <c r="F104" s="46" t="str">
+        <f t="shared" si="8"/>
+        <v>SQL, NoSQL (MongoDB, Couchbase), Map Reduce. Ruby on Rails, Django</v>
+      </c>
+      <c r="G104" s="10"/>
+    </row>
+    <row r="105" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C105" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D105" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="E104" s="10"/>
-      <c r="F104" s="19" t="s">
+      <c r="E105" s="10"/>
+      <c r="F105" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="G104" s="10"/>
-    </row>
-    <row r="105" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="22" t="s">
+      <c r="G105" s="10"/>
+    </row>
+    <row r="106" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B105" s="23"/>
-      <c r="C105" s="24"/>
-      <c r="D105" s="23"/>
-      <c r="E105" s="10"/>
-      <c r="F105" s="23"/>
-      <c r="G105" s="10"/>
-    </row>
-    <row r="106" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C106" s="21" t="s">
+      <c r="B106" s="23"/>
+      <c r="C106" s="24"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="23"/>
+      <c r="G106" s="10"/>
+    </row>
+    <row r="107" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C107" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D106" s="18" t="s">
+      <c r="D107" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="E106" s="10"/>
-      <c r="F106" s="18" t="s">
+      <c r="E107" s="10"/>
+      <c r="F107" s="18" t="s">
         <v>267</v>
-      </c>
-      <c r="G106" s="10"/>
-    </row>
-    <row r="107" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C107" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D107" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="E107" s="10"/>
-      <c r="F107" s="48" t="str">
-        <f t="shared" ref="F107:F109" si="8">D107</f>
-        <v>Eclipse, Git, svn, vim, maven, Jenkins, gdb</v>
       </c>
       <c r="G107" s="10"/>
     </row>
@@ -5252,159 +5262,160 @@
         <v>60</v>
       </c>
       <c r="D108" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E108" s="10"/>
+      <c r="F108" s="46" t="str">
+        <f t="shared" ref="F108:F109" si="9">D108</f>
+        <v>Eclipse, Git, svn, vim, maven, Jenkins, gdb</v>
+      </c>
+      <c r="G108" s="10"/>
+    </row>
+    <row r="109" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C109" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D109" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="E108" s="10"/>
-      <c r="F108" s="48" t="str">
-        <f t="shared" si="8"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="46" t="str">
+        <f t="shared" si="9"/>
         <v>Virtualization (vSphere/Pyvmomi, KVM-Qemu, VirtualBox)</v>
       </c>
-      <c r="G108" s="10"/>
-    </row>
-    <row r="109" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="22" t="s">
+      <c r="G109" s="10"/>
+    </row>
+    <row r="110" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B109" s="23"/>
-      <c r="C109" s="24"/>
-      <c r="D109" s="23"/>
-      <c r="E109" s="10"/>
-      <c r="F109" s="23"/>
-      <c r="G109" s="14"/>
-      <c r="H109" s="9"/>
-      <c r="I109" s="9"/>
-      <c r="J109" s="9"/>
-      <c r="K109" s="9"/>
-      <c r="L109" s="9"/>
-      <c r="M109" s="9"/>
-    </row>
-    <row r="110" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="C110" s="11" t="s">
+      <c r="B110" s="23"/>
+      <c r="C110" s="24"/>
+      <c r="D110" s="23"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="23"/>
+      <c r="G110" s="14"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="9"/>
+      <c r="J110" s="9"/>
+      <c r="K110" s="9"/>
+      <c r="L110" s="9"/>
+      <c r="M110" s="9"/>
+    </row>
+    <row r="111" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="C111" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D110" s="18" t="s">
+      <c r="D111" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="E110" s="10"/>
-      <c r="F110" s="18" t="s">
+      <c r="E111" s="10"/>
+      <c r="F111" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="G110" s="10"/>
-    </row>
-    <row r="111" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C111" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D111" s="19" t="s">
+      <c r="G111" s="10"/>
+    </row>
+    <row r="112" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C112" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D112" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="E111" s="10"/>
-      <c r="F111" s="19" t="s">
+      <c r="E112" s="10"/>
+      <c r="F112" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="G111" s="10"/>
-    </row>
-    <row r="112" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="22" t="s">
+      <c r="G112" s="10"/>
+    </row>
+    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B112" s="23"/>
-      <c r="C112" s="24"/>
-      <c r="D112" s="23"/>
-      <c r="E112" s="10"/>
-      <c r="F112" s="23"/>
-      <c r="G112" s="10"/>
-    </row>
-    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="28" t="s">
+      <c r="B113" s="23"/>
+      <c r="C113" s="24"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="10"/>
+      <c r="F113" s="23"/>
+      <c r="G113" s="10"/>
+    </row>
+    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B113" s="28" t="s">
+      <c r="B114" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="C113" s="29"/>
-      <c r="D113" s="28"/>
-      <c r="E113" s="10"/>
-      <c r="F113" s="28"/>
-      <c r="G113" s="10"/>
-    </row>
-    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="22" t="s">
+      <c r="C114" s="29"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="10"/>
+      <c r="F114" s="28"/>
+      <c r="G114" s="10"/>
+    </row>
+    <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B114" s="23"/>
-      <c r="C114" s="24"/>
-      <c r="D114" s="23"/>
-      <c r="E114" s="10"/>
-      <c r="F114" s="23"/>
-      <c r="G114" s="10"/>
-    </row>
-    <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C115" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D115" s="18" t="s">
-        <v>125</v>
-      </c>
+      <c r="B115" s="23"/>
+      <c r="C115" s="24"/>
+      <c r="D115" s="23"/>
       <c r="E115" s="10"/>
-      <c r="F115" s="48" t="str">
-        <f t="shared" ref="F115:F120" si="9">D115</f>
-        <v>B.Sc/Dip.Eng in  Electronic Control and Robotics</v>
-      </c>
+      <c r="F115" s="23"/>
       <c r="G115" s="10"/>
     </row>
     <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="C116" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D116" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E116" s="10"/>
+      <c r="F116" s="46" t="str">
+        <f t="shared" ref="F116:F119" si="10">D116</f>
+        <v>B.Sc/Dip.Eng in  Electronic Control and Robotics</v>
+      </c>
+      <c r="G116" s="10"/>
+    </row>
+    <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C117" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D116" s="18" t="s">
+      <c r="D117" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="E116" s="10"/>
-      <c r="F116" s="48" t="str">
-        <f t="shared" si="9"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="46" t="str">
+        <f t="shared" si="10"/>
         <v>University Of Hull,  UK</v>
-      </c>
-      <c r="G116" s="10"/>
-    </row>
-    <row r="117" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C117" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D117" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="E117" s="10"/>
-      <c r="F117" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v>10/1980</v>
       </c>
       <c r="G117" s="10"/>
     </row>
     <row r="118" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C118" s="21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E118" s="10"/>
-      <c r="F118" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v>07/1985</v>
+      <c r="F118" s="46" t="str">
+        <f t="shared" si="10"/>
+        <v>10/1980</v>
       </c>
       <c r="G118" s="10"/>
     </row>
     <row r="119" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C119" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D119" s="19" t="s">
-        <v>130</v>
+        <v>57</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="E119" s="10"/>
-      <c r="F119" s="19" t="s">
-        <v>271</v>
+      <c r="F119" s="46" t="str">
+        <f t="shared" si="10"/>
+        <v>07/1985</v>
       </c>
       <c r="G119" s="10"/>
     </row>
@@ -5413,74 +5424,73 @@
         <v>60</v>
       </c>
       <c r="D120" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E120" s="10"/>
       <c r="F120" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="G120" s="10"/>
+    </row>
+    <row r="121" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C121" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D121" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E121" s="10"/>
+      <c r="F121" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="G120" s="10"/>
-    </row>
-    <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A121" s="22" t="s">
+      <c r="G121" s="10"/>
+    </row>
+    <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B121" s="23"/>
-      <c r="C121" s="24"/>
-      <c r="D121" s="23"/>
-      <c r="E121" s="10"/>
-      <c r="F121" s="23"/>
-      <c r="G121" s="10"/>
-    </row>
-    <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A122" s="28" t="s">
+      <c r="B122" s="23"/>
+      <c r="C122" s="24"/>
+      <c r="D122" s="23"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="23"/>
+      <c r="G122" s="10"/>
+    </row>
+    <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B122" s="28" t="s">
+      <c r="B123" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C122" s="30"/>
-      <c r="D122" s="28"/>
-      <c r="E122" s="10"/>
-      <c r="F122" s="28"/>
-      <c r="G122" s="10"/>
-    </row>
-    <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A123" s="22" t="s">
+      <c r="C123" s="30"/>
+      <c r="D123" s="28"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="28"/>
+      <c r="G123" s="10"/>
+    </row>
+    <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B123" s="23"/>
-      <c r="C123" s="24"/>
-      <c r="D123" s="23"/>
-      <c r="E123" s="10"/>
-      <c r="F123" s="23"/>
-      <c r="G123" s="10"/>
-    </row>
-    <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="C124" s="21" t="s">
+      <c r="B124" s="23"/>
+      <c r="C124" s="24"/>
+      <c r="D124" s="23"/>
+      <c r="E124" s="10"/>
+      <c r="F124" s="23"/>
+      <c r="G124" s="10"/>
+    </row>
+    <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="C125" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D124" s="31" t="s">
+      <c r="D125" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="E124" s="10"/>
-      <c r="F124" s="48" t="str">
-        <f t="shared" ref="F124:F129" si="10">D124</f>
+      <c r="E125" s="10"/>
+      <c r="F125" s="46" t="str">
+        <f t="shared" ref="F125:F130" si="11">D125</f>
         <v>Conference Talks</v>
-      </c>
-      <c r="G124" s="10"/>
-    </row>
-    <row r="125" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C125" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D125" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="E125" s="10"/>
-      <c r="F125" s="48" t="str">
-        <f t="shared" si="10"/>
-        <v>https://mjbright.github.io/Talks</v>
       </c>
       <c r="G125" s="10"/>
     </row>
@@ -5488,13 +5498,13 @@
       <c r="C126" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D126" s="33" t="s">
-        <v>216</v>
+      <c r="D126" s="37" t="s">
+        <v>134</v>
       </c>
       <c r="E126" s="10"/>
-      <c r="F126" s="48" t="str">
-        <f t="shared" si="10"/>
-        <v>2018 FOSSCon (Pres+Lab), FOSS Asia (Pres+Lab), Code Europe, PyConfr</v>
+      <c r="F126" s="46" t="str">
+        <f t="shared" si="11"/>
+        <v>https://mjbright.github.io/Talks</v>
       </c>
       <c r="G126" s="10"/>
     </row>
@@ -5502,27 +5512,27 @@
       <c r="C127" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D127" s="11" t="s">
+      <c r="D127" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="E127" s="10"/>
+      <c r="F127" s="46" t="str">
+        <f t="shared" si="11"/>
+        <v>2018 FOSSCon (Pres+Lab), FOSS Asia (Pres+Lab), Code Europe, PyConfr</v>
+      </c>
+      <c r="G127" s="10"/>
+    </row>
+    <row r="128" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C128" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D128" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="E127" s="10"/>
-      <c r="F127" s="48" t="str">
-        <f t="shared" si="10"/>
+      <c r="E128" s="10"/>
+      <c r="F128" s="46" t="str">
+        <f t="shared" si="11"/>
         <v>2017 Devconf.cz, Snowcamp.io, HPE TSS, HPE TES, DockerConUS, RMLL, OSS EU (Pres+Lab)</v>
-      </c>
-      <c r="G127" s="10"/>
-    </row>
-    <row r="128" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C128" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D128" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="E128" s="10"/>
-      <c r="F128" s="48" t="str">
-        <f t="shared" si="10"/>
-        <v>2016 Europython (Pres+Lab), ContainerCon Europe (Pres+Lab)</v>
       </c>
       <c r="G128" s="10"/>
     </row>
@@ -5531,51 +5541,51 @@
         <v>60</v>
       </c>
       <c r="D129" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="E129" s="10"/>
+      <c r="F129" s="46" t="str">
+        <f t="shared" si="11"/>
+        <v>2016 Europython (Pres+Lab), ContainerCon Europe (Pres+Lab)</v>
+      </c>
+      <c r="G129" s="10"/>
+    </row>
+    <row r="130" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C130" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D130" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="E129" s="10"/>
-      <c r="F129" s="48" t="str">
-        <f t="shared" si="10"/>
+      <c r="E130" s="10"/>
+      <c r="F130" s="46" t="str">
+        <f t="shared" si="11"/>
         <v>2015 Pyconfr, Ipython vers Jupyter</v>
       </c>
-      <c r="G129" s="10"/>
-    </row>
-    <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A130" s="22" t="s">
+      <c r="G130" s="10"/>
+    </row>
+    <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B130" s="23"/>
-      <c r="C130" s="24"/>
-      <c r="D130" s="23"/>
-      <c r="E130" s="10"/>
-      <c r="F130" s="23"/>
-      <c r="G130" s="10"/>
-    </row>
-    <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C131" s="11" t="s">
+      <c r="B131" s="23"/>
+      <c r="C131" s="24"/>
+      <c r="D131" s="23"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="23"/>
+      <c r="G131" s="10"/>
+    </row>
+    <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C132" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D131" s="18" t="s">
+      <c r="D132" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="E131" s="10"/>
-      <c r="F131" s="18" t="str">
-        <f t="shared" ref="F131:F133" si="11">D131</f>
+      <c r="E132" s="10"/>
+      <c r="F132" s="18" t="str">
+        <f t="shared" ref="F132:F134" si="12">D132</f>
         <v>Startup Weekend</v>
-      </c>
-      <c r="G131" s="10"/>
-    </row>
-    <row r="132" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C132" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D132" s="35" t="s">
-        <v>221</v>
-      </c>
-      <c r="E132" s="10"/>
-      <c r="F132" s="48" t="str">
-        <f t="shared" si="11"/>
-        <v>2018-Nov: Community Security System</v>
       </c>
       <c r="G132" s="10"/>
     </row>
@@ -5584,50 +5594,51 @@
         <v>60</v>
       </c>
       <c r="D133" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="E133" s="10"/>
+      <c r="F133" s="46" t="str">
+        <f t="shared" si="12"/>
+        <v>2018-Nov: Community Security System</v>
+      </c>
+      <c r="G133" s="10"/>
+    </row>
+    <row r="134" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C134" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D134" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="E133" s="10"/>
-      <c r="F133" s="48" t="str">
-        <f t="shared" si="11"/>
+      <c r="E134" s="10"/>
+      <c r="F134" s="46" t="str">
+        <f t="shared" si="12"/>
         <v>2012-Nov 2nd place: https://www.archionline.com/</v>
       </c>
-      <c r="G133" s="10"/>
-    </row>
-    <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A134" s="22" t="s">
+      <c r="G134" s="10"/>
+    </row>
+    <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B134" s="23"/>
-      <c r="C134" s="24"/>
-      <c r="D134" s="23"/>
-      <c r="E134" s="10"/>
-      <c r="F134" s="23"/>
-      <c r="G134" s="10"/>
-    </row>
-    <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C135" s="11" t="s">
+      <c r="B135" s="23"/>
+      <c r="C135" s="24"/>
+      <c r="D135" s="23"/>
+      <c r="E135" s="10"/>
+      <c r="F135" s="23"/>
+      <c r="G135" s="10"/>
+    </row>
+    <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C136" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D135" s="18" t="s">
+      <c r="D136" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="E135" s="10"/>
-      <c r="F135" s="18" t="str">
-        <f t="shared" ref="F135:F138" si="12">D135</f>
+      <c r="E136" s="10"/>
+      <c r="F136" s="18" t="str">
+        <f t="shared" ref="F136" si="13">D136</f>
         <v>Miscellaneous</v>
-      </c>
-      <c r="G135" s="10"/>
-    </row>
-    <row r="136" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C136" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D136" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E136" s="10"/>
-      <c r="F136" s="49" t="s">
-        <v>273</v>
       </c>
       <c r="G136" s="10"/>
     </row>
@@ -5636,11 +5647,11 @@
         <v>60</v>
       </c>
       <c r="D137" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E137" s="10"/>
-      <c r="F137" s="19" t="s">
-        <v>274</v>
+      <c r="F137" s="47" t="s">
+        <v>273</v>
       </c>
       <c r="G137" s="10"/>
     </row>
@@ -5649,48 +5660,48 @@
         <v>60</v>
       </c>
       <c r="D138" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E138" s="10"/>
       <c r="F138" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="G138" s="10"/>
+    </row>
+    <row r="139" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C139" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D139" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E139" s="10"/>
+      <c r="F139" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="G138" s="10"/>
-    </row>
-    <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A139" s="22" t="s">
+      <c r="G139" s="10"/>
+    </row>
+    <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A140" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="24"/>
-      <c r="D139" s="23"/>
-      <c r="E139" s="10"/>
-      <c r="F139" s="23"/>
-      <c r="G139" s="10"/>
-    </row>
-    <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="C140" s="11" t="s">
+      <c r="B140" s="23"/>
+      <c r="C140" s="24"/>
+      <c r="D140" s="23"/>
+      <c r="E140" s="10"/>
+      <c r="F140" s="23"/>
+      <c r="G140" s="10"/>
+    </row>
+    <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C141" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D140" s="18" t="s">
+      <c r="D141" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="E140" s="10"/>
-      <c r="F140" s="18" t="s">
+      <c r="E141" s="10"/>
+      <c r="F141" s="18" t="s">
         <v>276</v>
-      </c>
-      <c r="G140" s="10"/>
-    </row>
-    <row r="141" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C141" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D141" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="E141" s="10"/>
-      <c r="F141" s="19" t="s">
-        <v>277</v>
       </c>
       <c r="G141" s="10"/>
     </row>
@@ -5699,11 +5710,11 @@
         <v>60</v>
       </c>
       <c r="D142" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E142" s="10"/>
       <c r="F142" s="19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G142" s="10"/>
     </row>
@@ -5712,24 +5723,37 @@
         <v>60</v>
       </c>
       <c r="D143" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E143" s="10"/>
       <c r="F143" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="G143" s="10"/>
+    </row>
+    <row r="144" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C144" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D144" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E144" s="10"/>
+      <c r="F144" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="G143" s="10"/>
-    </row>
-    <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A144" s="22" t="s">
+      <c r="G144" s="10"/>
+    </row>
+    <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A145" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B144" s="23"/>
-      <c r="C144" s="24"/>
-      <c r="D144" s="23"/>
-      <c r="E144" s="10"/>
-      <c r="F144" s="23"/>
-      <c r="G144" s="10"/>
+      <c r="B145" s="23"/>
+      <c r="C145" s="24"/>
+      <c r="D145" s="23"/>
+      <c r="E145" s="10"/>
+      <c r="F145" s="23"/>
+      <c r="G145" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5741,7 +5765,7 @@
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{D51FD02F-2DA6-4ABC-BF13-5426C418C97F}"/>
     <hyperlink ref="D10" r:id="rId2" xr:uid="{934CAD68-C6A7-41E6-9E62-A741A79CF6B2}"/>
-    <hyperlink ref="D125" r:id="rId3" xr:uid="{5168BA34-B279-4AD8-92C8-4D51073270E8}"/>
+    <hyperlink ref="D126" r:id="rId3" xr:uid="{5168BA34-B279-4AD8-92C8-4D51073270E8}"/>
     <hyperlink ref="D8" r:id="rId4" xr:uid="{3FA3FE92-00D2-4CE9-B37D-29A41681B0E9}"/>
     <hyperlink ref="D9" r:id="rId5" xr:uid="{8445D70B-C4C5-4BE2-BCD9-C99A7F5B4CC3}"/>
   </hyperlinks>
@@ -5772,20 +5796,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -7440,20 +7464,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -9078,20 +9102,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -10608,20 +10632,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -12591,20 +12615,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -14536,20 +14560,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>

</xml_diff>